<commit_message>
Remaining file structure updated
</commit_message>
<xml_diff>
--- a/Project Planning/Project Drawings.xlsx
+++ b/Project Planning/Project Drawings.xlsx
@@ -8,16 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colinmorrison/codeclan_work/Resistance_Temple/Project Planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2BE1B11-064F-8545-B8F9-D535B4BCE74E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78CBBA17-E282-ED4F-A1B1-2D2173B14DF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="440" yWindow="1520" windowWidth="31800" windowHeight="19480" activeTab="1" xr2:uid="{056C3CC7-3EA0-BF47-B5DA-A9694FF9AEB8}"/>
+    <workbookView xWindow="-140" yWindow="500" windowWidth="33140" windowHeight="20500" activeTab="1" xr2:uid="{056C3CC7-3EA0-BF47-B5DA-A9694FF9AEB8}"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" r:id="rId1"/>
     <sheet name="Classes" sheetId="2" r:id="rId2"/>
     <sheet name="File Structure" sheetId="5" r:id="rId3"/>
+    <sheet name="Case Diagrams" sheetId="10" r:id="rId4"/>
+    <sheet name="Activity Diagrams" sheetId="7" r:id="rId5"/>
+    <sheet name="Object diagrams" sheetId="8" r:id="rId6"/>
+    <sheet name="Implementation Constraints" sheetId="6" r:id="rId7"/>
+    <sheet name="User Sitemap" sheetId="9" r:id="rId8"/>
+    <sheet name="README" sheetId="12" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,17 +39,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="165">
   <si>
     <t>1) We have a Gym - Resistance Temple</t>
   </si>
   <si>
-    <t>2) We have customers, who can access many classes</t>
-  </si>
-  <si>
-    <t>3) We have classes, that can be accessed by many customers</t>
-  </si>
-  <si>
     <t>Customers</t>
   </si>
   <si>
@@ -146,9 +146,6 @@
     <t>4) Personal Best lifts of the week or month or all time (Lengthy, unlikely to do)</t>
   </si>
   <si>
-    <t>INT FK</t>
-  </si>
-  <si>
     <t>(room?)</t>
   </si>
   <si>
@@ -270,9 +267,6 @@
   </si>
   <si>
     <t>customer_repository.py</t>
-  </si>
-  <si>
-    <t>sessions_repository.py</t>
   </si>
   <si>
     <t>booking_repository.py</t>
@@ -350,9 +344,6 @@
     <t>This could show recent bookings?</t>
   </si>
   <si>
-    <t>CRUD:</t>
-  </si>
-  <si>
     <t>Create</t>
   </si>
   <si>
@@ -368,21 +359,9 @@
     <t>save()</t>
   </si>
   <si>
-    <t>select_all()</t>
-  </si>
-  <si>
-    <t>find_by_id()</t>
-  </si>
-  <si>
     <t>update()</t>
   </si>
   <si>
-    <t>delete_one()</t>
-  </si>
-  <si>
-    <t>delete_all()</t>
-  </si>
-  <si>
     <t>CRUD</t>
   </si>
   <si>
@@ -390,13 +369,208 @@
   </si>
   <si>
     <t>delete_one()    delete_all()</t>
+  </si>
+  <si>
+    <t>3) We have sessions, that can be accessed by many customers</t>
+  </si>
+  <si>
+    <t>2) We have customers, who can access many gym classes (hereby known as sessions)</t>
+  </si>
+  <si>
+    <t>INT FOREIGN KEY</t>
+  </si>
+  <si>
+    <t>Attributes</t>
+  </si>
+  <si>
+    <t>Methods</t>
+  </si>
+  <si>
+    <t>add_customer()</t>
+  </si>
+  <si>
+    <t>add_session()</t>
+  </si>
+  <si>
+    <t>remove_customer()</t>
+  </si>
+  <si>
+    <t>update_membership_status()</t>
+  </si>
+  <si>
+    <t>update_membership_type()</t>
+  </si>
+  <si>
+    <t>update_sessions_had()</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>session</t>
+  </si>
+  <si>
+    <t>room?</t>
+  </si>
+  <si>
+    <t>**These won't be in the classes, these will be in the repositories?</t>
+  </si>
+  <si>
+    <t>Staff Member</t>
+  </si>
+  <si>
+    <t>Gym</t>
+  </si>
+  <si>
+    <t>View all and individual customers</t>
+  </si>
+  <si>
+    <t>Change customer details including membership level and status</t>
+  </si>
+  <si>
+    <t>Add a new customer</t>
+  </si>
+  <si>
+    <t>Add a new training session</t>
+  </si>
+  <si>
+    <t>Change a training session</t>
+  </si>
+  <si>
+    <t>View all and individual training sessions</t>
+  </si>
+  <si>
+    <t>Book a customer into a training session</t>
+  </si>
+  <si>
+    <t>Cancel a training session</t>
+  </si>
+  <si>
+    <t>Customer being booked to a gym session</t>
+  </si>
+  <si>
+    <t>Asks to be booked in</t>
+  </si>
+  <si>
+    <t>Checks their membership status</t>
+  </si>
+  <si>
+    <t>-&gt; Membership Expired</t>
+  </si>
+  <si>
+    <t>(gate)</t>
+  </si>
+  <si>
+    <t>Membership Status Good</t>
+  </si>
+  <si>
+    <t>|</t>
+  </si>
+  <si>
+    <t>Checks Sessions &lt; Sessions.max for month</t>
+  </si>
+  <si>
+    <t>James: Customer</t>
+  </si>
+  <si>
+    <t>James Mackay</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>(monthly_sessions_had)</t>
+  </si>
+  <si>
+    <t>Xtreme Zumba</t>
+  </si>
+  <si>
+    <t>Xtreme Zumba: Session</t>
+  </si>
+  <si>
+    <t>Endurance</t>
+  </si>
+  <si>
+    <t>✓</t>
+  </si>
+  <si>
+    <t>session_repository.py</t>
+  </si>
+  <si>
+    <t>✓ - Done, extensions commented</t>
+  </si>
+  <si>
+    <t>1) Create a database</t>
+  </si>
+  <si>
+    <t>a) Open Terminal</t>
+  </si>
+  <si>
+    <t>b) Type: createdb resistance_temple</t>
+  </si>
+  <si>
+    <t>a) Open Terminal, cd to the resistance_temple main folder</t>
+  </si>
+  <si>
+    <t>b) Type: psql -d resistance_temple -f db/resistance_temple.sql</t>
+  </si>
+  <si>
+    <t>2) Link the database to the project</t>
+  </si>
+  <si>
+    <t>c) Keep this open</t>
+  </si>
+  <si>
+    <t>3) Enter our initial data to try</t>
+  </si>
+  <si>
+    <t>a) Open a 2nd terminal, cd to the resistance_temple main folder</t>
+  </si>
+  <si>
+    <t>b) Type: python3 console.py</t>
+  </si>
+  <si>
+    <t>c) This will load the database with some starter data for us to try out</t>
+  </si>
+  <si>
+    <t>4) Run Flask</t>
+  </si>
+  <si>
+    <t>a) Open a 3rd terminal, cd to the resistance_temple main folder</t>
+  </si>
+  <si>
+    <t>b) Type: Flask run</t>
+  </si>
+  <si>
+    <t>c) This will load up a local server to test our package in a browser</t>
+  </si>
+  <si>
+    <t>5) Open up out app</t>
+  </si>
+  <si>
+    <t>a) Open Google Chrome</t>
+  </si>
+  <si>
+    <t>b) In the URL bar, enter: http://localhost:5000/</t>
+  </si>
+  <si>
+    <t>c) This will direct us to our home page</t>
+  </si>
+  <si>
+    <t>Customer()</t>
+  </si>
+  <si>
+    <t>Session()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -460,6 +634,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -469,7 +650,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -686,17 +867,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -713,15 +883,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -817,11 +978,104 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -871,17 +1125,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -890,12 +1135,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -907,8 +1146,14 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -919,12 +1164,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1257,16 +1557,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>194734</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1582616</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>205153</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>820616</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>205154</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1281,8 +1581,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="4000500" y="2823634"/>
-          <a:ext cx="1651000" cy="8466"/>
+          <a:off x="4005385" y="2061307"/>
+          <a:ext cx="830385" cy="1"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1309,15 +1609,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:colOff>9769</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>207107</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>795867</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:colOff>805636</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>207107</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1332,8 +1632,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8826500" y="2806700"/>
-          <a:ext cx="1621367" cy="0"/>
+          <a:off x="8040077" y="2063261"/>
+          <a:ext cx="795867" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1355,6 +1655,50 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>459153</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>552938</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>25193</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4398C8E-FAF5-314A-9B31-61A54A974165}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12504615" y="615462"/>
+          <a:ext cx="10058400" cy="5574116"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2484,6 +2828,455 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>4142317</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>106346</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02B3C66A-729C-9B48-923B-CC40763C7DE8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10058400" cy="4373546"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>156989</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C08F8F61-529D-794D-8CC2-B0B0FC4F3C9A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10058400" cy="5888923"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1231900</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>108234</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88825CE1-1D5C-044D-861A-0AC6CB34B29F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="12700"/>
+          <a:ext cx="10058400" cy="5581934"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1582616</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>205153</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>820616</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>205154</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2319D957-CD95-A94D-95DB-757A00A2C760}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3995616" y="2046653"/>
+          <a:ext cx="825500" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9769</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>207107</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>805636</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>207107</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91727320-F293-BF49-9920-5554C3DFE4B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8010769" y="2048607"/>
+          <a:ext cx="795867" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1582616</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>205153</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>820616</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>205154</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF78A2D5-149E-B74D-AF7F-3DD33BD6A0D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3995616" y="6248236"/>
+          <a:ext cx="825500" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9769</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>207107</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>805636</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>207107</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Connector 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8C5D3A8-84A9-3646-9A2E-23944DB2A963}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8010769" y="6250190"/>
+          <a:ext cx="795867" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>153809</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29F8F1F1-FFEF-E147-BEF3-CC57F95EAB59}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10058400" cy="6453009"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>202255</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{577A77F2-171B-DE4B-8C5E-63188A76879F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="127000" y="38100"/>
+          <a:ext cx="10058400" cy="5650555"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2784,7 +3577,7 @@
   <dimension ref="B2:J42"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2796,7 +3589,7 @@
   <sheetData>
     <row r="2" spans="2:9">
       <c r="B2" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="2:9">
@@ -2806,117 +3599,117 @@
     </row>
     <row r="4" spans="2:9">
       <c r="B4" t="s">
-        <v>1</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="2:9">
       <c r="B5" t="s">
-        <v>2</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="17" thickBot="1"/>
     <row r="10" spans="2:9" s="5" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="B10" s="21" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C10" s="22"/>
       <c r="E10" s="21" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F10" s="22"/>
       <c r="H10" s="21" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I10" s="22"/>
     </row>
     <row r="11" spans="2:9">
       <c r="B11" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>37</v>
+        <v>102</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="2:9">
       <c r="B12" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>37</v>
+        <v>102</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="2:9">
       <c r="B13" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F13" s="3"/>
       <c r="H13" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="2:9">
       <c r="B14" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="H14" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="2:9">
       <c r="B15" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="H15" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="2:9">
@@ -2925,10 +3718,10 @@
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="H16" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="2:10">
@@ -2937,13 +3730,13 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="H17" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="2:10">
@@ -2952,10 +3745,10 @@
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="H18" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="2:10">
@@ -2976,83 +3769,83 @@
     </row>
     <row r="24" spans="2:10">
       <c r="B24" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C24" s="1"/>
     </row>
     <row r="25" spans="2:10">
       <c r="B25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="2:10">
       <c r="D26" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="2:10">
       <c r="D27" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="2:10">
       <c r="D28" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="2:10">
       <c r="B30" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="2:10">
       <c r="D31" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="2:10">
       <c r="D32" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="2:4">
       <c r="D33" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="2:4">
       <c r="B35" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="2:4">
       <c r="D36" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="2:4">
       <c r="D37" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39" spans="2:4">
       <c r="B39" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="2:4">
       <c r="D40" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="2:4">
       <c r="D41" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="42" spans="2:4">
       <c r="D42" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -3068,10 +3861,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C703BECF-5A51-894E-B8EF-AE4D25329CF7}">
-  <dimension ref="B2:J20"/>
+  <dimension ref="B2:J32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3083,172 +3876,176 @@
   <sheetData>
     <row r="2" spans="2:9">
       <c r="B2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>106</v>
+        <v>40</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="2:9">
       <c r="B3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="37" t="s">
-        <v>96</v>
-      </c>
-      <c r="F3" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="G3" s="32"/>
+        <v>41</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="G3" s="28"/>
     </row>
     <row r="4" spans="2:9">
       <c r="B4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="41" t="s">
-        <v>97</v>
-      </c>
-      <c r="F4" s="40" t="s">
-        <v>107</v>
-      </c>
-      <c r="G4" s="42"/>
+        <v>42</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="G4" s="37"/>
     </row>
     <row r="5" spans="2:9">
       <c r="B5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" s="43" t="s">
-        <v>98</v>
-      </c>
-      <c r="F5" s="39" t="s">
-        <v>103</v>
-      </c>
-      <c r="G5" s="44"/>
+        <v>54</v>
+      </c>
+      <c r="E5" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="G5" s="39"/>
     </row>
     <row r="6" spans="2:9">
-      <c r="E6" s="38" t="s">
+      <c r="E6" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="F6" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="F6" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="G6" s="35"/>
+      <c r="G6" s="30"/>
     </row>
     <row r="9" spans="2:9" ht="17" thickBot="1"/>
     <row r="10" spans="2:9" s="5" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="B10" s="21" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C10" s="22"/>
       <c r="E10" s="21" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F10" s="22"/>
       <c r="H10" s="21" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I10" s="22"/>
     </row>
-    <row r="11" spans="2:9">
-      <c r="B11" s="2" t="s">
+    <row r="11" spans="2:9" ht="17" thickBot="1">
+      <c r="B11" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" s="41"/>
+      <c r="E11" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="F11" s="41"/>
+      <c r="H11" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="I11" s="41"/>
+    </row>
+    <row r="12" spans="2:9">
+      <c r="B12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9">
+      <c r="B13" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9">
+      <c r="B14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="2" t="s">
+      <c r="C14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="H14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9">
-      <c r="B12" s="6" t="s">
+      <c r="I14" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9">
+      <c r="B15" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C15" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="H15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9">
-      <c r="B13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="3"/>
-      <c r="H13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9">
-      <c r="B14" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="H14" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9">
-      <c r="B15" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="H15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I15" s="9" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="16" spans="2:9">
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
+      <c r="B16" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
-      <c r="H16" s="7" t="s">
-        <v>14</v>
+      <c r="H16" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="2:10">
@@ -3256,11 +4053,11 @@
       <c r="C17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
-      <c r="H17" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>53</v>
+      <c r="H17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>52</v>
       </c>
       <c r="J17" s="10"/>
     </row>
@@ -3270,10 +4067,10 @@
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="H18" s="6" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="2:10">
@@ -3281,8 +4078,12 @@
       <c r="C19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
+      <c r="H19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="20" spans="2:10" ht="17" thickBot="1">
       <c r="B20" s="4"/>
@@ -3292,11 +4093,162 @@
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
     </row>
+    <row r="21" spans="2:10" ht="17" thickBot="1">
+      <c r="B21" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" s="41"/>
+      <c r="E21" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="F21" s="41"/>
+      <c r="H21" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="I21" s="41"/>
+    </row>
+    <row r="22" spans="2:10">
+      <c r="B22" s="51" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="52"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="52"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="51" t="s">
+        <v>106</v>
+      </c>
+      <c r="I22" s="52"/>
+    </row>
+    <row r="23" spans="2:10">
+      <c r="B23" s="53" t="s">
+        <v>107</v>
+      </c>
+      <c r="C23" s="54"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="54"/>
+    </row>
+    <row r="24" spans="2:10">
+      <c r="B24" s="53" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" s="54"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="54"/>
+    </row>
+    <row r="25" spans="2:10">
+      <c r="B25" s="53" t="s">
+        <v>108</v>
+      </c>
+      <c r="C25" s="54"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="54"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="53"/>
+      <c r="I25" s="54"/>
+    </row>
+    <row r="26" spans="2:10">
+      <c r="B26" s="53" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" s="54"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="54"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="54"/>
+    </row>
+    <row r="27" spans="2:10">
+      <c r="B27" s="53"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="54"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="53"/>
+      <c r="I27" s="54"/>
+    </row>
+    <row r="28" spans="2:10">
+      <c r="B28" s="47"/>
+      <c r="C28" s="48"/>
+      <c r="E28" s="47"/>
+      <c r="F28" s="48"/>
+      <c r="H28" s="47"/>
+      <c r="I28" s="48"/>
+    </row>
+    <row r="29" spans="2:10">
+      <c r="B29" s="47"/>
+      <c r="C29" s="48"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="48"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="48"/>
+    </row>
+    <row r="30" spans="2:10" ht="17" thickBot="1">
+      <c r="B30" s="49"/>
+      <c r="C30" s="50"/>
+      <c r="E30" s="49"/>
+      <c r="F30" s="50"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="50"/>
+    </row>
+    <row r="31" spans="2:10">
+      <c r="B31" s="15" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10">
+      <c r="B32" s="15"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="36">
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B26:C26"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3305,10 +4257,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104CFFA4-B0A1-1A4A-AFD7-C18B47CC4B2A}">
-  <dimension ref="B3:I48"/>
+  <dimension ref="B3:J48"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I7" sqref="G3:I7"/>
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3319,272 +4271,308 @@
     <col min="5" max="5" width="20.83203125" customWidth="1"/>
     <col min="7" max="7" width="20.83203125" customWidth="1"/>
     <col min="8" max="8" width="12.1640625" customWidth="1"/>
-    <col min="9" max="9" width="116.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9">
+    <row r="3" spans="2:6">
       <c r="B3" s="25" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="G3" s="30" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9">
+        <v>62</v>
+      </c>
+      <c r="E3" s="62" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
       <c r="B4" s="26"/>
       <c r="D4" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="G4" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="H4" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="I4" s="32"/>
-    </row>
-    <row r="5" spans="2:9">
+        <v>63</v>
+      </c>
+      <c r="E4" s="62" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
       <c r="B5" s="12"/>
       <c r="D5" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="G5" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="H5" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="I5" s="33" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9">
-      <c r="G6" s="28" t="s">
-        <v>98</v>
-      </c>
-      <c r="H6" s="27" t="s">
-        <v>103</v>
-      </c>
-      <c r="I6" s="33"/>
-    </row>
-    <row r="7" spans="2:9">
-      <c r="G7" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="H7" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="I7" s="35" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9">
+        <v>64</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
       <c r="C8" s="23" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9">
+        <v>65</v>
+      </c>
+      <c r="F8" s="62" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
       <c r="C9" s="24"/>
       <c r="E9" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="61" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="E10" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" s="61" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="E11" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="61" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="C14" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="16" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="10" spans="2:9">
-      <c r="E10" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9">
-      <c r="E11" s="17" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9">
-      <c r="C14" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9">
+      <c r="F14" s="62" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
       <c r="C15" s="24"/>
       <c r="E15" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7">
+        <v>70</v>
+      </c>
+      <c r="F15" s="62" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8">
       <c r="C18" s="23" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="3:7">
+        <v>65</v>
+      </c>
+      <c r="F18" s="62" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8">
       <c r="C19" s="24"/>
       <c r="E19" s="18" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="3:7">
+        <v>71</v>
+      </c>
+      <c r="F19" s="62" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="20" spans="3:8">
       <c r="E20" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" s="62" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21" spans="3:8">
+      <c r="E21" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="24" spans="3:8">
+      <c r="C24" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="16" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="21" spans="3:7">
-      <c r="E21" s="17" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="24" spans="3:7">
-      <c r="C24" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="25" spans="3:7">
+      <c r="F24" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="25" spans="3:8">
       <c r="C25" s="24"/>
       <c r="E25" s="18" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="26" spans="3:7">
+        <v>142</v>
+      </c>
+      <c r="F25" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="26" spans="3:8">
       <c r="E26" s="17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="30" spans="3:7">
+        <v>76</v>
+      </c>
+      <c r="F26" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="30" spans="3:8">
       <c r="C30" s="23" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E30" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="G30" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="H30" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="31" spans="3:8">
+      <c r="C31" s="24"/>
+    </row>
+    <row r="33" spans="3:10">
+      <c r="E33" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="G30" s="19" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="31" spans="3:7">
-      <c r="C31" s="24"/>
-    </row>
-    <row r="33" spans="3:9">
-      <c r="E33" s="13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="37" spans="3:9">
+    </row>
+    <row r="37" spans="3:10">
       <c r="C37" s="23" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D37" s="20"/>
       <c r="E37" s="16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="38" spans="3:9">
+        <v>79</v>
+      </c>
+      <c r="F37" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="38" spans="3:10">
       <c r="C38" s="24"/>
       <c r="D38" s="20"/>
       <c r="E38" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="F38" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="40" spans="3:10">
+      <c r="E40" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G40" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="H40" t="s">
+        <v>141</v>
+      </c>
+      <c r="I40" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="J40" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="3:9">
-      <c r="E40" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="G40" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="H40" s="14" t="s">
+    <row r="41" spans="3:10">
+      <c r="G41" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="H41" t="s">
+        <v>141</v>
+      </c>
+      <c r="I41" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="J41" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="3:10">
+      <c r="I42" s="11"/>
+    </row>
+    <row r="43" spans="3:10">
+      <c r="E43" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="G43" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="H43" t="s">
+        <v>141</v>
+      </c>
+      <c r="I43" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="J43" t="s">
         <v>87</v>
       </c>
-      <c r="I40" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="41" spans="3:9">
-      <c r="G41" s="17" t="s">
+    </row>
+    <row r="44" spans="3:10">
+      <c r="G44" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="H44" t="s">
+        <v>141</v>
+      </c>
+      <c r="I44" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="J44" t="s">
         <v>85</v>
       </c>
-      <c r="H41" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="I41" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="42" spans="3:9">
-      <c r="H42" s="11"/>
-    </row>
-    <row r="43" spans="3:9">
-      <c r="E43" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G43" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="H43" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="I43" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="44" spans="3:9">
-      <c r="G44" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="H44" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="I44" t="s">
+    </row>
+    <row r="45" spans="3:10">
+      <c r="I45" s="11"/>
+    </row>
+    <row r="46" spans="3:10">
+      <c r="E46" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="G46" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="H46" t="s">
+        <v>141</v>
+      </c>
+      <c r="I46" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="J46" s="15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="47" spans="3:10">
+      <c r="G47" s="18"/>
+      <c r="I47" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="J47" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="48" spans="3:10">
+      <c r="G48" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="H48" t="s">
+        <v>141</v>
+      </c>
+      <c r="I48" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="J48" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="45" spans="3:9">
-      <c r="H45" s="11"/>
-    </row>
-    <row r="46" spans="3:9">
-      <c r="E46" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="G46" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="H46" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="I46" s="15" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="47" spans="3:9">
-      <c r="G47" s="18"/>
-      <c r="H47" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="I47" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="48" spans="3:9">
-      <c r="G48" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="H48" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="I48" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -3600,4 +4588,648 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8E17ED-892D-D04F-869B-AE05270EAAF6}">
+  <dimension ref="F29:J43"/>
+  <sheetViews>
+    <sheetView topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="54.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="29" spans="8:8">
+      <c r="H29" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="31" spans="8:8">
+      <c r="H31" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="33" spans="6:10">
+      <c r="F33" t="s">
+        <v>115</v>
+      </c>
+      <c r="H33" t="s">
+        <v>123</v>
+      </c>
+      <c r="J33" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="35" spans="6:10">
+      <c r="H35" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="6:10">
+      <c r="H37" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="39" spans="6:10">
+      <c r="H39" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="6:10">
+      <c r="H41" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="43" spans="6:10">
+      <c r="H43" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CBFD39B-43B3-0D45-98DE-0DFDCC0D1885}">
+  <dimension ref="N6:R18"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="14" max="14" width="17.83203125" customWidth="1"/>
+    <col min="17" max="17" width="36.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="14:18">
+      <c r="N6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="14:18">
+      <c r="N8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="14:18" ht="17" thickBot="1"/>
+    <row r="10" spans="14:18" ht="17" thickBot="1">
+      <c r="N10" s="56" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q10" s="56" t="s">
+        <v>127</v>
+      </c>
+      <c r="R10" s="55"/>
+    </row>
+    <row r="12" spans="14:18">
+      <c r="Q12" s="58" t="s">
+        <v>129</v>
+      </c>
+      <c r="R12" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="14:18">
+      <c r="Q13" s="11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="14:18">
+      <c r="Q14" s="11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="14:18">
+      <c r="Q15" s="57" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="14:18">
+      <c r="Q16" s="11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="17:17" ht="17" thickBot="1">
+      <c r="Q17" s="11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="17:17" ht="17" thickBot="1">
+      <c r="Q18" s="56" t="s">
+        <v>132</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2BC9DF8-6225-2246-A893-3AB58E40FBE3}">
+  <dimension ref="B30:I56"/>
+  <sheetViews>
+    <sheetView topLeftCell="A8" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="3" width="20.83203125" customWidth="1"/>
+    <col min="5" max="6" width="20.83203125" customWidth="1"/>
+    <col min="8" max="9" width="20.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="30" spans="2:9" ht="17" thickBot="1"/>
+    <row r="31" spans="2:9" ht="20" thickBot="1">
+      <c r="B31" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="22"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" s="22"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="I31" s="22"/>
+    </row>
+    <row r="32" spans="2:9" ht="17" thickBot="1">
+      <c r="B32" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="C32" s="41"/>
+      <c r="E32" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="F32" s="41"/>
+      <c r="H32" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="I32" s="41"/>
+    </row>
+    <row r="33" spans="2:9">
+      <c r="B33" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F33" s="3"/>
+      <c r="H33" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9">
+      <c r="B34" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F34" s="6"/>
+      <c r="H34" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9">
+      <c r="B35" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F35" s="6"/>
+      <c r="H35" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9">
+      <c r="B36" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F36" s="8"/>
+      <c r="H36" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9">
+      <c r="B37" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="H37" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I37" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9">
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="H38" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I38" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9">
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="H39" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9">
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="H40" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I40" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" ht="17" thickBot="1">
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+    </row>
+    <row r="44" spans="2:9" ht="17" thickBot="1"/>
+    <row r="45" spans="2:9" ht="20" thickBot="1">
+      <c r="B45" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="C45" s="22"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F45" s="22"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="I45" s="22"/>
+    </row>
+    <row r="46" spans="2:9" ht="17" thickBot="1">
+      <c r="B46" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="C46" s="41"/>
+      <c r="E46" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="F46" s="41"/>
+      <c r="H46" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="I46" s="41"/>
+    </row>
+    <row r="47" spans="2:9">
+      <c r="B47" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" s="43"/>
+      <c r="E47" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F47" s="43"/>
+      <c r="H47" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I47" s="3"/>
+    </row>
+    <row r="48" spans="2:9">
+      <c r="B48" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" s="44" t="s">
+        <v>134</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F48" s="44"/>
+      <c r="H48" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I48" s="44" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9">
+      <c r="B49" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" s="43" t="s">
+        <v>135</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F49" s="44"/>
+      <c r="H49" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I49" s="44" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9">
+      <c r="B50" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="44" t="s">
+        <v>136</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F50" s="42"/>
+      <c r="H50" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I50" s="59">
+        <v>44302</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9">
+      <c r="B51" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C51" s="43">
+        <v>3</v>
+      </c>
+      <c r="E51" s="7"/>
+      <c r="F51" s="45"/>
+      <c r="H51" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I51" s="60">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9">
+      <c r="B52" s="6"/>
+      <c r="C52" s="44"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="44"/>
+      <c r="H52" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I52" s="60">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9">
+      <c r="B53" s="8"/>
+      <c r="C53" s="42"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="42"/>
+      <c r="H53" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I53" s="44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9">
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="44"/>
+      <c r="H54" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I54" s="44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" ht="17" thickBot="1">
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="46"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="46"/>
+    </row>
+    <row r="56" spans="2:9">
+      <c r="F56" s="11"/>
+      <c r="I56" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="H32:I32"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{708EB1BC-2998-4147-87D5-799A3B5DE066}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA7FD533-B3EE-FC43-90B2-49FAE6C07009}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDC33A-DF32-4641-B172-56C8FF1D1446}">
+  <dimension ref="B3:C25"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="3" spans="2:3">
+      <c r="B3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="C4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="C5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="C8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="C9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="C10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="C13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3">
+      <c r="C14" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3">
+      <c r="C15" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="C18" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="C19" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="C20" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="C23" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="C24" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="C25" t="s">
+        <v>162</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Home and Customer .html templates linked and tested
</commit_message>
<xml_diff>
--- a/Project Planning/Project Drawings.xlsx
+++ b/Project Planning/Project Drawings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colinmorrison/codeclan_work/Resistance_Temple/Project Planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78CBBA17-E282-ED4F-A1B1-2D2173B14DF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F386FA-DA17-7840-A05C-67D5559738B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-140" yWindow="500" windowWidth="33140" windowHeight="20500" activeTab="1" xr2:uid="{056C3CC7-3EA0-BF47-B5DA-A9694FF9AEB8}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="168">
   <si>
     <t>1) We have a Gym - Resistance Temple</t>
   </si>
@@ -365,12 +365,6 @@
     <t>CRUD</t>
   </si>
   <si>
-    <t>select_all()    find_by_id()</t>
-  </si>
-  <si>
-    <t>delete_one()    delete_all()</t>
-  </si>
-  <si>
     <t>3) We have sessions, that can be accessed by many customers</t>
   </si>
   <si>
@@ -564,6 +558,21 @@
   </si>
   <si>
     <t>Session()</t>
+  </si>
+  <si>
+    <t>Done but no useful methods in yet</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> delete_all()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">delete_one() </t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_all()  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> find_one()</t>
   </si>
 </sst>
 </file>
@@ -642,15 +651,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="34">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -877,29 +892,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -942,33 +935,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="dashed">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dashed">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="dashed">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -1075,7 +1044,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1125,44 +1094,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1185,32 +1130,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1223,8 +1168,31 @@
     <xf numFmtId="20" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3577,7 +3545,7 @@
   <dimension ref="B2:J42"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="B10" sqref="B10:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3599,12 +3567,12 @@
     </row>
     <row r="4" spans="2:9">
       <c r="B4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="2:9">
       <c r="B5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="17" thickBot="1"/>
@@ -3633,7 +3601,7 @@
         <v>7</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>2</v>
@@ -3653,7 +3621,7 @@
         <v>8</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>3</v>
@@ -3864,7 +3832,7 @@
   <dimension ref="B2:J32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3878,7 +3846,7 @@
       <c r="B2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="28" t="s">
         <v>97</v>
       </c>
     </row>
@@ -3886,46 +3854,50 @@
       <c r="B3" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="60" t="s">
         <v>91</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="59" t="s">
         <v>95</v>
       </c>
-      <c r="G3" s="28"/>
+      <c r="G3" s="61"/>
     </row>
     <row r="4" spans="2:9">
       <c r="B4" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="36" t="s">
+      <c r="E4" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="F4" s="35" t="s">
-        <v>98</v>
-      </c>
-      <c r="G4" s="37"/>
+      <c r="F4" s="55" t="s">
+        <v>166</v>
+      </c>
+      <c r="G4" s="56" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="5" spans="2:9">
       <c r="B5" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="38" t="s">
+      <c r="E5" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="F5" s="34" t="s">
+      <c r="F5" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="G5" s="39"/>
+      <c r="G5" s="57"/>
     </row>
     <row r="6" spans="2:9">
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="F6" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="G6" s="30"/>
+      <c r="F6" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="G6" s="58" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="9" spans="2:9" ht="17" thickBot="1"/>
     <row r="10" spans="2:9" s="5" customFormat="1" ht="30" customHeight="1" thickBot="1">
@@ -3943,18 +3915,18 @@
       <c r="I10" s="22"/>
     </row>
     <row r="11" spans="2:9" ht="17" thickBot="1">
-      <c r="B11" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="C11" s="41"/>
-      <c r="E11" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="F11" s="41"/>
-      <c r="H11" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="I11" s="41"/>
+      <c r="B11" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="33"/>
+      <c r="E11" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="F11" s="33"/>
+      <c r="H11" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="I11" s="33"/>
     </row>
     <row r="12" spans="2:9">
       <c r="B12" s="3" t="s">
@@ -3984,10 +3956,10 @@
         <v>49</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H13" s="6" t="s">
         <v>3</v>
@@ -4004,10 +3976,10 @@
         <v>49</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>9</v>
@@ -4034,7 +4006,7 @@
     </row>
     <row r="16" spans="2:9">
       <c r="B16" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>51</v>
@@ -4094,118 +4066,118 @@
       <c r="I20" s="4"/>
     </row>
     <row r="21" spans="2:10" ht="17" thickBot="1">
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21" s="33"/>
+      <c r="E21" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="F21" s="33"/>
+      <c r="H21" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="I21" s="33"/>
+    </row>
+    <row r="22" spans="2:10">
+      <c r="B22" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="C22" s="44"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="C21" s="41"/>
-      <c r="E21" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="F21" s="41"/>
-      <c r="H21" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="I21" s="41"/>
-    </row>
-    <row r="22" spans="2:10">
-      <c r="B22" s="51" t="s">
+      <c r="I22" s="44"/>
+    </row>
+    <row r="23" spans="2:10">
+      <c r="B23" s="45" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="52"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="51"/>
-      <c r="F22" s="52"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="51" t="s">
+      <c r="C23" s="46"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="46"/>
+    </row>
+    <row r="24" spans="2:10">
+      <c r="B24" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" s="46"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="46"/>
+    </row>
+    <row r="25" spans="2:10">
+      <c r="B25" s="45" t="s">
         <v>106</v>
       </c>
-      <c r="I22" s="52"/>
-    </row>
-    <row r="23" spans="2:10">
-      <c r="B23" s="53" t="s">
-        <v>107</v>
-      </c>
-      <c r="C23" s="54"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="53"/>
-      <c r="I23" s="54"/>
-    </row>
-    <row r="24" spans="2:10">
-      <c r="B24" s="53" t="s">
-        <v>109</v>
-      </c>
-      <c r="C24" s="54"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="54"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="53"/>
-      <c r="I24" s="54"/>
-    </row>
-    <row r="25" spans="2:10">
-      <c r="B25" s="53" t="s">
+      <c r="C25" s="46"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="45"/>
+      <c r="I25" s="46"/>
+    </row>
+    <row r="26" spans="2:10">
+      <c r="B26" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="C25" s="54"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="53"/>
-      <c r="F25" s="54"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="53"/>
-      <c r="I25" s="54"/>
-    </row>
-    <row r="26" spans="2:10">
-      <c r="B26" s="53" t="s">
-        <v>110</v>
-      </c>
-      <c r="C26" s="54"/>
+      <c r="C26" s="46"/>
       <c r="D26" s="15"/>
-      <c r="E26" s="53"/>
-      <c r="F26" s="54"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="46"/>
       <c r="G26" s="15"/>
-      <c r="H26" s="53"/>
-      <c r="I26" s="54"/>
+      <c r="H26" s="45"/>
+      <c r="I26" s="46"/>
     </row>
     <row r="27" spans="2:10">
-      <c r="B27" s="53"/>
-      <c r="C27" s="54"/>
+      <c r="B27" s="45"/>
+      <c r="C27" s="46"/>
       <c r="D27" s="15"/>
-      <c r="E27" s="53"/>
-      <c r="F27" s="54"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="46"/>
       <c r="G27" s="15"/>
-      <c r="H27" s="53"/>
-      <c r="I27" s="54"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="46"/>
     </row>
     <row r="28" spans="2:10">
-      <c r="B28" s="47"/>
-      <c r="C28" s="48"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="48"/>
-      <c r="H28" s="47"/>
-      <c r="I28" s="48"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="40"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="40"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="40"/>
     </row>
     <row r="29" spans="2:10">
-      <c r="B29" s="47"/>
-      <c r="C29" s="48"/>
-      <c r="E29" s="47"/>
-      <c r="F29" s="48"/>
-      <c r="H29" s="47"/>
-      <c r="I29" s="48"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="40"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="40"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="40"/>
     </row>
     <row r="30" spans="2:10" ht="17" thickBot="1">
-      <c r="B30" s="49"/>
-      <c r="C30" s="50"/>
-      <c r="E30" s="49"/>
-      <c r="F30" s="50"/>
-      <c r="H30" s="49"/>
-      <c r="I30" s="50"/>
+      <c r="B30" s="41"/>
+      <c r="C30" s="42"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="42"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="42"/>
     </row>
     <row r="31" spans="2:10">
       <c r="B31" s="15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="2:10">
@@ -4260,7 +4232,7 @@
   <dimension ref="B3:J48"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4281,8 +4253,8 @@
       <c r="D3" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="E3" s="62" t="s">
-        <v>141</v>
+      <c r="E3" s="53" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="2:6">
@@ -4290,8 +4262,8 @@
       <c r="D4" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="62" t="s">
-        <v>141</v>
+      <c r="E4" s="53" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="2:6">
@@ -4300,7 +4272,7 @@
         <v>64</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="2:6">
@@ -4310,8 +4282,8 @@
       <c r="E8" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="F8" s="62" t="s">
-        <v>141</v>
+      <c r="F8" s="53" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="2:6">
@@ -4319,24 +4291,24 @@
       <c r="E9" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="61" t="s">
-        <v>141</v>
+      <c r="F9" s="53" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="2:6">
       <c r="E10" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="F10" s="61" t="s">
-        <v>141</v>
+      <c r="F10" s="53" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="2:6">
       <c r="E11" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="F11" s="61" t="s">
-        <v>141</v>
+      <c r="F11" s="53" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="2:6">
@@ -4346,8 +4318,8 @@
       <c r="E14" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="F14" s="62" t="s">
-        <v>141</v>
+      <c r="F14" s="53" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="2:6">
@@ -4355,8 +4327,8 @@
       <c r="E15" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="62" t="s">
-        <v>143</v>
+      <c r="F15" s="53" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="3:8">
@@ -4366,8 +4338,8 @@
       <c r="E18" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="F18" s="62" t="s">
-        <v>141</v>
+      <c r="F18" s="53" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="3:8">
@@ -4375,24 +4347,24 @@
       <c r="E19" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="F19" s="62" t="s">
-        <v>141</v>
+      <c r="F19" s="53" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="3:8">
       <c r="E20" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="F20" s="62" t="s">
-        <v>141</v>
+      <c r="F20" s="53" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="3:8">
       <c r="E21" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="F21" t="s">
-        <v>141</v>
+      <c r="F21" s="53" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="24" spans="3:8">
@@ -4402,25 +4374,34 @@
       <c r="E24" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="F24" t="s">
-        <v>141</v>
+      <c r="F24" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="25" spans="3:8">
       <c r="C25" s="24"/>
       <c r="E25" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="F25" t="s">
-        <v>141</v>
+        <v>140</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="26" spans="3:8">
       <c r="E26" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="F26" t="s">
-        <v>141</v>
+      <c r="F26" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="30" spans="3:8">
@@ -4434,7 +4415,7 @@
         <v>78</v>
       </c>
       <c r="H30" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="3:8">
@@ -4454,7 +4435,7 @@
         <v>79</v>
       </c>
       <c r="F37" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" spans="3:10">
@@ -4464,7 +4445,7 @@
         <v>80</v>
       </c>
       <c r="F38" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40" spans="3:10">
@@ -4475,7 +4456,7 @@
         <v>80</v>
       </c>
       <c r="H40" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I40" s="14" t="s">
         <v>83</v>
@@ -4489,7 +4470,7 @@
         <v>81</v>
       </c>
       <c r="H41" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I41" s="14" t="s">
         <v>83</v>
@@ -4509,7 +4490,7 @@
         <v>80</v>
       </c>
       <c r="H43" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I43" s="14" t="s">
         <v>83</v>
@@ -4523,7 +4504,7 @@
         <v>81</v>
       </c>
       <c r="H44" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I44" s="14" t="s">
         <v>83</v>
@@ -4543,7 +4524,7 @@
         <v>80</v>
       </c>
       <c r="H46" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I46" s="14" t="s">
         <v>83</v>
@@ -4566,7 +4547,7 @@
         <v>82</v>
       </c>
       <c r="H48" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I48" s="14" t="s">
         <v>83</v>
@@ -4606,48 +4587,48 @@
   <sheetData>
     <row r="29" spans="8:8">
       <c r="H29" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="8:8">
       <c r="H31" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="6:10">
       <c r="F33" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H33" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J33" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="6:10">
       <c r="H35" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="6:10">
       <c r="H37" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="6:10">
       <c r="H39" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" spans="6:10">
       <c r="H41" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="6:10">
       <c r="H43" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -4672,7 +4653,7 @@
   <sheetData>
     <row r="6" spans="14:18">
       <c r="N6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="14:18">
@@ -4680,55 +4661,55 @@
         <v>43</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="14:18" ht="17" thickBot="1"/>
     <row r="10" spans="14:18" ht="17" thickBot="1">
-      <c r="N10" s="56" t="s">
+      <c r="N10" s="48" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q10" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="R10" s="47"/>
+    </row>
+    <row r="12" spans="14:18">
+      <c r="Q12" s="50" t="s">
+        <v>127</v>
+      </c>
+      <c r="R12" s="10" t="s">
         <v>126</v>
-      </c>
-      <c r="Q10" s="56" t="s">
-        <v>127</v>
-      </c>
-      <c r="R10" s="55"/>
-    </row>
-    <row r="12" spans="14:18">
-      <c r="Q12" s="58" t="s">
-        <v>129</v>
-      </c>
-      <c r="R12" s="10" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="13" spans="14:18">
       <c r="Q13" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="14:18">
       <c r="Q14" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="14:18">
-      <c r="Q15" s="57" t="s">
-        <v>130</v>
+      <c r="Q15" s="49" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="14:18">
       <c r="Q16" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="17:17" ht="17" thickBot="1">
       <c r="Q17" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="17:17" ht="17" thickBot="1">
-      <c r="Q18" s="56" t="s">
-        <v>132</v>
+      <c r="Q18" s="48" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -4741,8 +4722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2BC9DF8-6225-2246-A893-3AB58E40FBE3}">
   <dimension ref="B30:I56"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4770,18 +4751,18 @@
       <c r="I31" s="22"/>
     </row>
     <row r="32" spans="2:9" ht="17" thickBot="1">
-      <c r="B32" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="C32" s="41"/>
-      <c r="E32" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="F32" s="41"/>
-      <c r="H32" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="I32" s="41"/>
+      <c r="B32" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="C32" s="33"/>
+      <c r="E32" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="F32" s="33"/>
+      <c r="H32" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="I32" s="33"/>
     </row>
     <row r="33" spans="2:9">
       <c r="B33" s="3" t="s">
@@ -4791,7 +4772,7 @@
         <v>53</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F33" s="3"/>
       <c r="H33" s="3" t="s">
@@ -4809,7 +4790,7 @@
         <v>49</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F34" s="6"/>
       <c r="H34" s="6" t="s">
@@ -4827,7 +4808,7 @@
         <v>49</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F35" s="6"/>
       <c r="H35" s="3" t="s">
@@ -4918,7 +4899,7 @@
     <row r="44" spans="2:9" ht="17" thickBot="1"/>
     <row r="45" spans="2:9" ht="20" thickBot="1">
       <c r="B45" s="21" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C45" s="22"/>
       <c r="D45" s="5"/>
@@ -4928,33 +4909,33 @@
       <c r="F45" s="22"/>
       <c r="G45" s="5"/>
       <c r="H45" s="21" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I45" s="22"/>
     </row>
     <row r="46" spans="2:9" ht="17" thickBot="1">
-      <c r="B46" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="C46" s="41"/>
-      <c r="E46" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="F46" s="41"/>
-      <c r="H46" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="I46" s="41"/>
+      <c r="B46" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="C46" s="33"/>
+      <c r="E46" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="F46" s="33"/>
+      <c r="H46" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="I46" s="33"/>
     </row>
     <row r="47" spans="2:9">
       <c r="B47" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C47" s="43"/>
+      <c r="C47" s="35"/>
       <c r="E47" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="F47" s="43"/>
+        <v>109</v>
+      </c>
+      <c r="F47" s="35"/>
       <c r="H47" s="3" t="s">
         <v>2</v>
       </c>
@@ -4964,93 +4945,93 @@
       <c r="B48" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C48" s="44" t="s">
-        <v>134</v>
+      <c r="C48" s="36" t="s">
+        <v>132</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="F48" s="44"/>
+        <v>110</v>
+      </c>
+      <c r="F48" s="36"/>
       <c r="H48" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I48" s="44" t="s">
-        <v>138</v>
+      <c r="I48" s="36" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="49" spans="2:9">
       <c r="B49" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C49" s="43" t="s">
-        <v>135</v>
+      <c r="C49" s="35" t="s">
+        <v>133</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="F49" s="44"/>
+        <v>111</v>
+      </c>
+      <c r="F49" s="36"/>
       <c r="H49" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I49" s="44" t="s">
-        <v>140</v>
+      <c r="I49" s="36" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="50" spans="2:9">
       <c r="B50" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C50" s="44" t="s">
-        <v>136</v>
+      <c r="C50" s="36" t="s">
+        <v>134</v>
       </c>
       <c r="E50" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F50" s="42"/>
+      <c r="F50" s="34"/>
       <c r="H50" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I50" s="59">
+      <c r="I50" s="51">
         <v>44302</v>
       </c>
     </row>
     <row r="51" spans="2:9">
       <c r="B51" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C51" s="43">
+        <v>135</v>
+      </c>
+      <c r="C51" s="35">
         <v>3</v>
       </c>
       <c r="E51" s="7"/>
-      <c r="F51" s="45"/>
+      <c r="F51" s="37"/>
       <c r="H51" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I51" s="60">
+      <c r="I51" s="52">
         <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="52" spans="2:9">
       <c r="B52" s="6"/>
-      <c r="C52" s="44"/>
+      <c r="C52" s="36"/>
       <c r="E52" s="6"/>
-      <c r="F52" s="44"/>
+      <c r="F52" s="36"/>
       <c r="H52" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I52" s="60">
+      <c r="I52" s="52">
         <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="53" spans="2:9">
       <c r="B53" s="8"/>
-      <c r="C53" s="42"/>
+      <c r="C53" s="34"/>
       <c r="E53" s="8"/>
-      <c r="F53" s="42"/>
+      <c r="F53" s="34"/>
       <c r="H53" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I53" s="44" t="b">
+      <c r="I53" s="36" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5058,11 +5039,11 @@
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
       <c r="E54" s="6"/>
-      <c r="F54" s="44"/>
+      <c r="F54" s="36"/>
       <c r="H54" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I54" s="44">
+      <c r="I54" s="36">
         <v>2</v>
       </c>
     </row>
@@ -5070,9 +5051,9 @@
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="E55" s="4"/>
-      <c r="F55" s="46"/>
+      <c r="F55" s="38"/>
       <c r="H55" s="4"/>
-      <c r="I55" s="46"/>
+      <c r="I55" s="38"/>
     </row>
     <row r="56" spans="2:9">
       <c r="F56" s="11"/>
@@ -5136,97 +5117,97 @@
   <sheetData>
     <row r="3" spans="2:3">
       <c r="B3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="2:3">
       <c r="C4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="2:3">
       <c r="C5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="2:3">
       <c r="B7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="2:3">
       <c r="C8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="2:3">
       <c r="C9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="2:3">
       <c r="C10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="2:3">
       <c r="B12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="2:3">
       <c r="C13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="2:3">
       <c r="C14" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="2:3">
       <c r="C15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="2:3">
       <c r="B17" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="2:3">
       <c r="C18" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="2:3">
       <c r="C19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20" spans="2:3">
       <c r="C20" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="2:3">
       <c r="B22" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="2:3">
       <c r="C23" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="2:3">
       <c r="C24" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="2:3">
       <c r="C25" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
html templates all viewable in browser
</commit_message>
<xml_diff>
--- a/Project Planning/Project Drawings.xlsx
+++ b/Project Planning/Project Drawings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colinmorrison/codeclan_work/Resistance_Temple/Project Planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F386FA-DA17-7840-A05C-67D5559738B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF4E751-2892-8243-BC9A-74C1F1F10770}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-140" yWindow="500" windowWidth="33140" windowHeight="20500" activeTab="1" xr2:uid="{056C3CC7-3EA0-BF47-B5DA-A9694FF9AEB8}"/>
   </bookViews>
@@ -3832,7 +3832,7 @@
   <dimension ref="B2:J32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Ability to update Session DB now up and running
</commit_message>
<xml_diff>
--- a/Project Planning/Project Drawings.xlsx
+++ b/Project Planning/Project Drawings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colinmorrison/codeclan_work/Resistance_Temple/Project Planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF4E751-2892-8243-BC9A-74C1F1F10770}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E78488-F1C3-EA4C-9A7E-8A567606D034}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-140" yWindow="500" windowWidth="33140" windowHeight="20500" activeTab="1" xr2:uid="{056C3CC7-3EA0-BF47-B5DA-A9694FF9AEB8}"/>
   </bookViews>
@@ -3832,7 +3832,7 @@
   <dimension ref="B2:J32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Customer update fixed, CSS link added
</commit_message>
<xml_diff>
--- a/Project Planning/Project Drawings.xlsx
+++ b/Project Planning/Project Drawings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colinmorrison/codeclan_work/Resistance_Temple/Project Planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E78488-F1C3-EA4C-9A7E-8A567606D034}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE2A276-BF0E-934C-BCBF-C0FD490C5AC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-140" yWindow="500" windowWidth="33140" windowHeight="20500" activeTab="1" xr2:uid="{056C3CC7-3EA0-BF47-B5DA-A9694FF9AEB8}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33000" windowHeight="20500" activeTab="8" xr2:uid="{056C3CC7-3EA0-BF47-B5DA-A9694FF9AEB8}"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,8 @@
     <sheet name="Object diagrams" sheetId="8" r:id="rId6"/>
     <sheet name="Implementation Constraints" sheetId="6" r:id="rId7"/>
     <sheet name="User Sitemap" sheetId="9" r:id="rId8"/>
-    <sheet name="README" sheetId="12" r:id="rId9"/>
+    <sheet name="Wire Diagrams" sheetId="13" r:id="rId9"/>
+    <sheet name="README" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="185">
   <si>
     <t>1) We have a Gym - Resistance Temple</t>
   </si>
@@ -573,6 +574,57 @@
   </si>
   <si>
     <t xml:space="preserve"> find_one()</t>
+  </si>
+  <si>
+    <t>Gym Name</t>
+  </si>
+  <si>
+    <t>Gym Logo</t>
+  </si>
+  <si>
+    <t>Bookings</t>
+  </si>
+  <si>
+    <t>Pricing Info</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Welcome statement/purpose of this app</t>
+  </si>
+  <si>
+    <t>Quick Access</t>
+  </si>
+  <si>
+    <t>*Make a new booking</t>
+  </si>
+  <si>
+    <t>*Add a new customer</t>
+  </si>
+  <si>
+    <t>*Add a new session</t>
+  </si>
+  <si>
+    <t>Gym Pictures</t>
+  </si>
+  <si>
+    <t>Contact Details</t>
+  </si>
+  <si>
+    <t>*On-Call manager</t>
+  </si>
+  <si>
+    <t>*On-shift PT</t>
+  </si>
+  <si>
+    <t>Site map</t>
+  </si>
+  <si>
+    <t>Website produced</t>
+  </si>
+  <si>
+    <t>Support</t>
   </si>
 </sst>
 </file>
@@ -665,7 +717,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -1040,11 +1092,110 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1076,24 +1227,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1109,12 +1242,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1129,30 +1256,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
@@ -1193,6 +1296,76 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3577,18 +3750,18 @@
     </row>
     <row r="9" spans="2:9" ht="17" thickBot="1"/>
     <row r="10" spans="2:9" s="5" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="22"/>
-      <c r="E10" s="21" t="s">
+      <c r="C10" s="47"/>
+      <c r="E10" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="22"/>
-      <c r="H10" s="21" t="s">
+      <c r="F10" s="47"/>
+      <c r="H10" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="I10" s="22"/>
+      <c r="I10" s="47"/>
     </row>
     <row r="11" spans="2:9">
       <c r="B11" s="2" t="s">
@@ -3827,11 +4000,121 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDC33A-DF32-4641-B172-56C8FF1D1446}">
+  <dimension ref="B3:C25"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="3" spans="2:3">
+      <c r="B3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="C4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="C5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="C8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="C9" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="C10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="C13" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3">
+      <c r="C14" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3">
+      <c r="C15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="C18" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="C19" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="C20" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="C23" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="C24" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="C25" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C703BECF-5A51-894E-B8EF-AE4D25329CF7}">
   <dimension ref="B2:J32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -3846,7 +4129,7 @@
       <c r="B2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="22" t="s">
         <v>97</v>
       </c>
     </row>
@@ -3854,25 +4137,25 @@
       <c r="B3" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="60" t="s">
+      <c r="E3" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="F3" s="59" t="s">
+      <c r="F3" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="G3" s="61"/>
+      <c r="G3" s="45"/>
     </row>
     <row r="4" spans="2:9">
       <c r="B4" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="54" t="s">
+      <c r="E4" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="F4" s="55" t="s">
+      <c r="F4" s="39" t="s">
         <v>166</v>
       </c>
-      <c r="G4" s="56" t="s">
+      <c r="G4" s="40" t="s">
         <v>167</v>
       </c>
     </row>
@@ -3880,53 +4163,53 @@
       <c r="B5" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="F5" s="30" t="s">
+      <c r="F5" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="G5" s="57"/>
+      <c r="G5" s="41"/>
     </row>
     <row r="6" spans="2:9">
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="G6" s="58" t="s">
+      <c r="G6" s="42" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="17" thickBot="1"/>
     <row r="10" spans="2:9" s="5" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="22"/>
-      <c r="E10" s="21" t="s">
+      <c r="C10" s="47"/>
+      <c r="E10" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="22"/>
-      <c r="H10" s="21" t="s">
+      <c r="F10" s="47"/>
+      <c r="H10" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="I10" s="22"/>
+      <c r="I10" s="47"/>
     </row>
     <row r="11" spans="2:9" ht="17" thickBot="1">
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="E11" s="32" t="s">
+      <c r="C11" s="57"/>
+      <c r="E11" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="F11" s="33"/>
-      <c r="H11" s="32" t="s">
+      <c r="F11" s="57"/>
+      <c r="H11" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="I11" s="33"/>
+      <c r="I11" s="57"/>
     </row>
     <row r="12" spans="2:9">
       <c r="B12" s="3" t="s">
@@ -4066,114 +4349,114 @@
       <c r="I20" s="4"/>
     </row>
     <row r="21" spans="2:10" ht="17" thickBot="1">
-      <c r="B21" s="32" t="s">
+      <c r="B21" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="C21" s="33"/>
-      <c r="E21" s="32" t="s">
+      <c r="C21" s="57"/>
+      <c r="E21" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="F21" s="33"/>
-      <c r="H21" s="32" t="s">
+      <c r="F21" s="57"/>
+      <c r="H21" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="I21" s="33"/>
+      <c r="I21" s="57"/>
     </row>
     <row r="22" spans="2:10">
-      <c r="B22" s="43" t="s">
+      <c r="B22" s="54" t="s">
         <v>103</v>
       </c>
-      <c r="C22" s="44"/>
+      <c r="C22" s="55"/>
       <c r="D22" s="15"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="44"/>
+      <c r="E22" s="54"/>
+      <c r="F22" s="55"/>
       <c r="G22" s="15"/>
-      <c r="H22" s="43" t="s">
+      <c r="H22" s="54" t="s">
         <v>104</v>
       </c>
-      <c r="I22" s="44"/>
+      <c r="I22" s="55"/>
     </row>
     <row r="23" spans="2:10">
-      <c r="B23" s="45" t="s">
+      <c r="B23" s="48" t="s">
         <v>105</v>
       </c>
-      <c r="C23" s="46"/>
+      <c r="C23" s="49"/>
       <c r="D23" s="15"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="46"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="49"/>
       <c r="G23" s="15"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="46"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="49"/>
     </row>
     <row r="24" spans="2:10">
-      <c r="B24" s="45" t="s">
+      <c r="B24" s="48" t="s">
         <v>107</v>
       </c>
-      <c r="C24" s="46"/>
+      <c r="C24" s="49"/>
       <c r="D24" s="15"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="46"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="49"/>
       <c r="G24" s="15"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="46"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="49"/>
     </row>
     <row r="25" spans="2:10">
-      <c r="B25" s="45" t="s">
+      <c r="B25" s="48" t="s">
         <v>106</v>
       </c>
-      <c r="C25" s="46"/>
+      <c r="C25" s="49"/>
       <c r="D25" s="15"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="46"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="49"/>
       <c r="G25" s="15"/>
-      <c r="H25" s="45"/>
-      <c r="I25" s="46"/>
+      <c r="H25" s="48"/>
+      <c r="I25" s="49"/>
     </row>
     <row r="26" spans="2:10">
-      <c r="B26" s="45" t="s">
+      <c r="B26" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="C26" s="46"/>
+      <c r="C26" s="49"/>
       <c r="D26" s="15"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="46"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="49"/>
       <c r="G26" s="15"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="46"/>
+      <c r="H26" s="48"/>
+      <c r="I26" s="49"/>
     </row>
     <row r="27" spans="2:10">
-      <c r="B27" s="45"/>
-      <c r="C27" s="46"/>
+      <c r="B27" s="48"/>
+      <c r="C27" s="49"/>
       <c r="D27" s="15"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="46"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="49"/>
       <c r="G27" s="15"/>
-      <c r="H27" s="45"/>
-      <c r="I27" s="46"/>
+      <c r="H27" s="48"/>
+      <c r="I27" s="49"/>
     </row>
     <row r="28" spans="2:10">
-      <c r="B28" s="39"/>
-      <c r="C28" s="40"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="40"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="40"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="51"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="51"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="51"/>
     </row>
     <row r="29" spans="2:10">
-      <c r="B29" s="39"/>
-      <c r="C29" s="40"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="40"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="40"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="51"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="51"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="51"/>
     </row>
     <row r="30" spans="2:10" ht="17" thickBot="1">
-      <c r="B30" s="41"/>
-      <c r="C30" s="42"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="42"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="42"/>
+      <c r="B30" s="52"/>
+      <c r="C30" s="53"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="53"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="53"/>
     </row>
     <row r="31" spans="2:10">
       <c r="B31" s="15" t="s">
@@ -4185,6 +4468,33 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
     <mergeCell ref="H27:I27"/>
     <mergeCell ref="H28:I28"/>
     <mergeCell ref="H29:I29"/>
@@ -4194,33 +4504,6 @@
     <mergeCell ref="H24:I24"/>
     <mergeCell ref="H25:I25"/>
     <mergeCell ref="H26:I26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4247,22 +4530,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:6">
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="58" t="s">
         <v>55</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="37" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="26"/>
+      <c r="B4" s="59"/>
       <c r="D4" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="53" t="s">
+      <c r="E4" s="37" t="s">
         <v>139</v>
       </c>
     </row>
@@ -4276,22 +4559,22 @@
       </c>
     </row>
     <row r="8" spans="2:6">
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="60" t="s">
         <v>56</v>
       </c>
       <c r="E8" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="F8" s="53" t="s">
+      <c r="F8" s="37" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="9" spans="2:6">
-      <c r="C9" s="24"/>
+      <c r="C9" s="61"/>
       <c r="E9" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="53" t="s">
+      <c r="F9" s="37" t="s">
         <v>139</v>
       </c>
     </row>
@@ -4299,7 +4582,7 @@
       <c r="E10" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="F10" s="53" t="s">
+      <c r="F10" s="37" t="s">
         <v>139</v>
       </c>
     </row>
@@ -4307,47 +4590,47 @@
       <c r="E11" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="F11" s="53" t="s">
+      <c r="F11" s="37" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="14" spans="2:6">
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="60" t="s">
         <v>57</v>
       </c>
       <c r="E14" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="F14" s="53" t="s">
+      <c r="F14" s="37" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="15" spans="2:6">
-      <c r="C15" s="24"/>
+      <c r="C15" s="61"/>
       <c r="E15" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="53" t="s">
+      <c r="F15" s="37" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="18" spans="3:8">
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="60" t="s">
         <v>58</v>
       </c>
       <c r="E18" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="F18" s="53" t="s">
+      <c r="F18" s="37" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="19" spans="3:8">
-      <c r="C19" s="24"/>
+      <c r="C19" s="61"/>
       <c r="E19" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="F19" s="53" t="s">
+      <c r="F19" s="37" t="s">
         <v>139</v>
       </c>
     </row>
@@ -4355,7 +4638,7 @@
       <c r="E20" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="F20" s="53" t="s">
+      <c r="F20" s="37" t="s">
         <v>139</v>
       </c>
     </row>
@@ -4363,12 +4646,12 @@
       <c r="E21" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="F21" s="53" t="s">
+      <c r="F21" s="37" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="24" spans="3:8">
-      <c r="C24" s="23" t="s">
+      <c r="C24" s="60" t="s">
         <v>60</v>
       </c>
       <c r="E24" s="16" t="s">
@@ -4382,7 +4665,7 @@
       </c>
     </row>
     <row r="25" spans="3:8">
-      <c r="C25" s="24"/>
+      <c r="C25" s="61"/>
       <c r="E25" s="18" t="s">
         <v>140</v>
       </c>
@@ -4405,7 +4688,7 @@
       </c>
     </row>
     <row r="30" spans="3:8">
-      <c r="C30" s="23" t="s">
+      <c r="C30" s="60" t="s">
         <v>61</v>
       </c>
       <c r="E30" s="13" t="s">
@@ -4419,7 +4702,7 @@
       </c>
     </row>
     <row r="31" spans="3:8">
-      <c r="C31" s="24"/>
+      <c r="C31" s="61"/>
     </row>
     <row r="33" spans="3:10">
       <c r="E33" s="13" t="s">
@@ -4427,7 +4710,7 @@
       </c>
     </row>
     <row r="37" spans="3:10">
-      <c r="C37" s="23" t="s">
+      <c r="C37" s="60" t="s">
         <v>59</v>
       </c>
       <c r="D37" s="20"/>
@@ -4439,7 +4722,7 @@
       </c>
     </row>
     <row r="38" spans="3:10">
-      <c r="C38" s="24"/>
+      <c r="C38" s="61"/>
       <c r="D38" s="20"/>
       <c r="E38" s="17" t="s">
         <v>80</v>
@@ -4666,16 +4949,16 @@
     </row>
     <row r="9" spans="14:18" ht="17" thickBot="1"/>
     <row r="10" spans="14:18" ht="17" thickBot="1">
-      <c r="N10" s="48" t="s">
+      <c r="N10" s="32" t="s">
         <v>124</v>
       </c>
-      <c r="Q10" s="48" t="s">
+      <c r="Q10" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="R10" s="47"/>
+      <c r="R10" s="31"/>
     </row>
     <row r="12" spans="14:18">
-      <c r="Q12" s="50" t="s">
+      <c r="Q12" s="34" t="s">
         <v>127</v>
       </c>
       <c r="R12" s="10" t="s">
@@ -4693,7 +4976,7 @@
       </c>
     </row>
     <row r="15" spans="14:18">
-      <c r="Q15" s="49" t="s">
+      <c r="Q15" s="33" t="s">
         <v>128</v>
       </c>
     </row>
@@ -4708,7 +4991,7 @@
       </c>
     </row>
     <row r="18" spans="17:17" ht="17" thickBot="1">
-      <c r="Q18" s="48" t="s">
+      <c r="Q18" s="32" t="s">
         <v>130</v>
       </c>
     </row>
@@ -4735,34 +5018,34 @@
   <sheetData>
     <row r="30" spans="2:9" ht="17" thickBot="1"/>
     <row r="31" spans="2:9" ht="20" thickBot="1">
-      <c r="B31" s="21" t="s">
+      <c r="B31" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="C31" s="22"/>
+      <c r="C31" s="47"/>
       <c r="D31" s="5"/>
-      <c r="E31" s="21" t="s">
+      <c r="E31" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="F31" s="22"/>
+      <c r="F31" s="47"/>
       <c r="G31" s="5"/>
-      <c r="H31" s="21" t="s">
+      <c r="H31" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="I31" s="22"/>
+      <c r="I31" s="47"/>
     </row>
     <row r="32" spans="2:9" ht="17" thickBot="1">
-      <c r="B32" s="32" t="s">
+      <c r="B32" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="C32" s="33"/>
-      <c r="E32" s="32" t="s">
+      <c r="C32" s="57"/>
+      <c r="E32" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="F32" s="33"/>
-      <c r="H32" s="32" t="s">
+      <c r="F32" s="57"/>
+      <c r="H32" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="I32" s="33"/>
+      <c r="I32" s="57"/>
     </row>
     <row r="33" spans="2:9">
       <c r="B33" s="3" t="s">
@@ -4898,44 +5181,44 @@
     </row>
     <row r="44" spans="2:9" ht="17" thickBot="1"/>
     <row r="45" spans="2:9" ht="20" thickBot="1">
-      <c r="B45" s="21" t="s">
+      <c r="B45" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="C45" s="22"/>
+      <c r="C45" s="47"/>
       <c r="D45" s="5"/>
-      <c r="E45" s="21" t="s">
+      <c r="E45" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="F45" s="22"/>
+      <c r="F45" s="47"/>
       <c r="G45" s="5"/>
-      <c r="H45" s="21" t="s">
+      <c r="H45" s="46" t="s">
         <v>137</v>
       </c>
-      <c r="I45" s="22"/>
+      <c r="I45" s="47"/>
     </row>
     <row r="46" spans="2:9" ht="17" thickBot="1">
-      <c r="B46" s="32" t="s">
+      <c r="B46" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="C46" s="33"/>
-      <c r="E46" s="32" t="s">
+      <c r="C46" s="57"/>
+      <c r="E46" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="F46" s="33"/>
-      <c r="H46" s="32" t="s">
+      <c r="F46" s="57"/>
+      <c r="H46" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="I46" s="33"/>
+      <c r="I46" s="57"/>
     </row>
     <row r="47" spans="2:9">
       <c r="B47" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C47" s="35"/>
+      <c r="C47" s="27"/>
       <c r="E47" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="F47" s="35"/>
+      <c r="F47" s="27"/>
       <c r="H47" s="3" t="s">
         <v>2</v>
       </c>
@@ -4945,17 +5228,17 @@
       <c r="B48" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C48" s="36" t="s">
+      <c r="C48" s="28" t="s">
         <v>132</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="F48" s="36"/>
+      <c r="F48" s="28"/>
       <c r="H48" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I48" s="36" t="s">
+      <c r="I48" s="28" t="s">
         <v>136</v>
       </c>
     </row>
@@ -4963,17 +5246,17 @@
       <c r="B49" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C49" s="35" t="s">
+      <c r="C49" s="27" t="s">
         <v>133</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="F49" s="36"/>
+      <c r="F49" s="28"/>
       <c r="H49" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I49" s="36" t="s">
+      <c r="I49" s="28" t="s">
         <v>138</v>
       </c>
     </row>
@@ -4981,17 +5264,17 @@
       <c r="B50" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C50" s="36" t="s">
+      <c r="C50" s="28" t="s">
         <v>134</v>
       </c>
       <c r="E50" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F50" s="34"/>
+      <c r="F50" s="26"/>
       <c r="H50" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I50" s="51">
+      <c r="I50" s="35">
         <v>44302</v>
       </c>
     </row>
@@ -4999,39 +5282,39 @@
       <c r="B51" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C51" s="35">
+      <c r="C51" s="27">
         <v>3</v>
       </c>
       <c r="E51" s="7"/>
-      <c r="F51" s="37"/>
+      <c r="F51" s="29"/>
       <c r="H51" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I51" s="52">
+      <c r="I51" s="36">
         <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="52" spans="2:9">
       <c r="B52" s="6"/>
-      <c r="C52" s="36"/>
+      <c r="C52" s="28"/>
       <c r="E52" s="6"/>
-      <c r="F52" s="36"/>
+      <c r="F52" s="28"/>
       <c r="H52" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I52" s="52">
+      <c r="I52" s="36">
         <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="53" spans="2:9">
       <c r="B53" s="8"/>
-      <c r="C53" s="34"/>
+      <c r="C53" s="26"/>
       <c r="E53" s="8"/>
-      <c r="F53" s="34"/>
+      <c r="F53" s="26"/>
       <c r="H53" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I53" s="36" t="b">
+      <c r="I53" s="28" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5039,11 +5322,11 @@
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
       <c r="E54" s="6"/>
-      <c r="F54" s="36"/>
+      <c r="F54" s="28"/>
       <c r="H54" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I54" s="36">
+      <c r="I54" s="28">
         <v>2</v>
       </c>
     </row>
@@ -5051,9 +5334,9 @@
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="E55" s="4"/>
-      <c r="F55" s="38"/>
+      <c r="F55" s="30"/>
       <c r="H55" s="4"/>
-      <c r="I55" s="38"/>
+      <c r="I55" s="30"/>
     </row>
     <row r="56" spans="2:9">
       <c r="F56" s="11"/>
@@ -5061,18 +5344,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="H32:I32"/>
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="E45:F45"/>
     <mergeCell ref="H45:I45"/>
     <mergeCell ref="B46:C46"/>
     <mergeCell ref="E46:F46"/>
     <mergeCell ref="H46:I46"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="H32:I32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5106,109 +5389,433 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDC33A-DF32-4641-B172-56C8FF1D1446}">
-  <dimension ref="B3:C25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05B7CD6E-8190-E842-88F1-7A7CF2B387AC}">
+  <dimension ref="B3:L31"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14:L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="9.83203125" customWidth="1"/>
+    <col min="2" max="2" width="3.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="2:3">
-      <c r="B3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3">
-      <c r="C4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3">
-      <c r="C5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3">
-      <c r="B7" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3">
-      <c r="C8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3">
-      <c r="C9" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3">
-      <c r="C10" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3">
-      <c r="B12" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3">
-      <c r="C13" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3">
-      <c r="C14" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3">
-      <c r="C15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3">
-      <c r="B17" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3">
-      <c r="C18" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3">
-      <c r="C19" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3">
-      <c r="C20" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3">
-      <c r="B22" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3">
-      <c r="C23" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3">
-      <c r="C24" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3">
-      <c r="C25" t="s">
-        <v>160</v>
-      </c>
+    <row r="3" spans="2:12">
+      <c r="B3" s="62"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="64"/>
+    </row>
+    <row r="4" spans="2:12">
+      <c r="B4" s="65"/>
+      <c r="C4" s="78" t="s">
+        <v>172</v>
+      </c>
+      <c r="D4" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="78" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="78" t="s">
+        <v>170</v>
+      </c>
+      <c r="G4" s="78" t="s">
+        <v>171</v>
+      </c>
+      <c r="H4" s="66"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="77" t="s">
+        <v>168</v>
+      </c>
+      <c r="K4" s="76" t="s">
+        <v>169</v>
+      </c>
+      <c r="L4" s="67"/>
+    </row>
+    <row r="5" spans="2:12">
+      <c r="B5" s="68"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="69"/>
+      <c r="L5" s="70"/>
+    </row>
+    <row r="6" spans="2:12">
+      <c r="B6" s="65"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="66"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="66"/>
+      <c r="L6" s="67"/>
+    </row>
+    <row r="7" spans="2:12">
+      <c r="B7" s="65"/>
+      <c r="C7" s="72" t="s">
+        <v>173</v>
+      </c>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="63"/>
+      <c r="K7" s="64"/>
+      <c r="L7" s="67"/>
+    </row>
+    <row r="8" spans="2:12">
+      <c r="B8" s="65"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="66"/>
+      <c r="H8" s="65"/>
+      <c r="I8" s="66"/>
+      <c r="J8" s="66"/>
+      <c r="K8" s="67"/>
+      <c r="L8" s="67"/>
+    </row>
+    <row r="9" spans="2:12">
+      <c r="B9" s="65"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="65"/>
+      <c r="I9" s="66"/>
+      <c r="J9" s="66"/>
+      <c r="K9" s="67"/>
+      <c r="L9" s="67"/>
+    </row>
+    <row r="10" spans="2:12">
+      <c r="B10" s="65"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="71" t="s">
+        <v>178</v>
+      </c>
+      <c r="J10" s="66"/>
+      <c r="K10" s="67"/>
+      <c r="L10" s="67"/>
+    </row>
+    <row r="11" spans="2:12">
+      <c r="B11" s="65"/>
+      <c r="C11" s="72" t="s">
+        <v>174</v>
+      </c>
+      <c r="D11" s="63"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="66"/>
+      <c r="H11" s="65"/>
+      <c r="I11" s="66"/>
+      <c r="J11" s="66"/>
+      <c r="K11" s="67"/>
+      <c r="L11" s="67"/>
+    </row>
+    <row r="12" spans="2:12">
+      <c r="B12" s="65"/>
+      <c r="C12" s="65" t="s">
+        <v>176</v>
+      </c>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="66"/>
+      <c r="H12" s="65"/>
+      <c r="I12" s="66"/>
+      <c r="J12" s="66"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="67"/>
+    </row>
+    <row r="13" spans="2:12">
+      <c r="B13" s="65"/>
+      <c r="C13" s="65" t="s">
+        <v>177</v>
+      </c>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="66"/>
+      <c r="H13" s="65"/>
+      <c r="I13" s="66"/>
+      <c r="J13" s="66"/>
+      <c r="K13" s="67"/>
+      <c r="L13" s="67"/>
+    </row>
+    <row r="14" spans="2:12">
+      <c r="B14" s="65"/>
+      <c r="C14" s="73" t="s">
+        <v>175</v>
+      </c>
+      <c r="D14" s="69"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="70"/>
+      <c r="G14" s="66"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="66"/>
+      <c r="J14" s="66"/>
+      <c r="K14" s="67"/>
+      <c r="L14" s="67"/>
+    </row>
+    <row r="15" spans="2:12">
+      <c r="B15" s="65"/>
+      <c r="C15" s="66"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="66"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="66"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="66"/>
+      <c r="J15" s="66"/>
+      <c r="K15" s="67"/>
+      <c r="L15" s="67"/>
+    </row>
+    <row r="16" spans="2:12">
+      <c r="B16" s="65"/>
+      <c r="C16" s="74" t="s">
+        <v>179</v>
+      </c>
+      <c r="D16" s="63"/>
+      <c r="E16" s="63"/>
+      <c r="F16" s="64"/>
+      <c r="G16" s="66"/>
+      <c r="H16" s="65"/>
+      <c r="I16" s="66"/>
+      <c r="J16" s="66"/>
+      <c r="K16" s="67"/>
+      <c r="L16" s="67"/>
+    </row>
+    <row r="17" spans="2:12">
+      <c r="B17" s="65"/>
+      <c r="C17" s="75" t="s">
+        <v>180</v>
+      </c>
+      <c r="D17" s="66"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="66"/>
+      <c r="H17" s="65"/>
+      <c r="I17" s="66"/>
+      <c r="J17" s="66"/>
+      <c r="K17" s="67"/>
+      <c r="L17" s="67"/>
+    </row>
+    <row r="18" spans="2:12">
+      <c r="B18" s="65"/>
+      <c r="C18" s="75" t="s">
+        <v>181</v>
+      </c>
+      <c r="D18" s="66"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="66"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="66"/>
+      <c r="J18" s="66"/>
+      <c r="K18" s="67"/>
+      <c r="L18" s="67"/>
+    </row>
+    <row r="19" spans="2:12">
+      <c r="B19" s="65"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="66"/>
+      <c r="H19" s="65"/>
+      <c r="I19" s="66"/>
+      <c r="J19" s="66"/>
+      <c r="K19" s="67"/>
+      <c r="L19" s="67"/>
+    </row>
+    <row r="20" spans="2:12">
+      <c r="B20" s="65"/>
+      <c r="C20" s="68"/>
+      <c r="D20" s="69"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="66"/>
+      <c r="H20" s="68"/>
+      <c r="I20" s="69"/>
+      <c r="J20" s="69"/>
+      <c r="K20" s="70"/>
+      <c r="L20" s="67"/>
+    </row>
+    <row r="21" spans="2:12">
+      <c r="B21" s="65"/>
+      <c r="C21" s="66"/>
+      <c r="D21" s="66"/>
+      <c r="E21" s="66"/>
+      <c r="F21" s="66"/>
+      <c r="G21" s="66"/>
+      <c r="H21" s="66"/>
+      <c r="I21" s="66"/>
+      <c r="J21" s="66"/>
+      <c r="K21" s="66"/>
+      <c r="L21" s="67"/>
+    </row>
+    <row r="22" spans="2:12">
+      <c r="B22" s="65"/>
+      <c r="C22" s="66"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="66"/>
+      <c r="F22" s="66"/>
+      <c r="G22" s="66"/>
+      <c r="H22" s="66"/>
+      <c r="I22" s="66"/>
+      <c r="J22" s="66"/>
+      <c r="K22" s="66"/>
+      <c r="L22" s="67"/>
+    </row>
+    <row r="23" spans="2:12">
+      <c r="B23" s="65"/>
+      <c r="C23" s="66"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="66"/>
+      <c r="F23" s="66"/>
+      <c r="G23" s="66"/>
+      <c r="H23" s="66"/>
+      <c r="I23" s="66"/>
+      <c r="J23" s="66"/>
+      <c r="K23" s="66"/>
+      <c r="L23" s="67"/>
+    </row>
+    <row r="24" spans="2:12">
+      <c r="B24" s="65"/>
+      <c r="C24" s="66"/>
+      <c r="D24" s="66"/>
+      <c r="E24" s="66"/>
+      <c r="F24" s="66"/>
+      <c r="G24" s="66"/>
+      <c r="H24" s="66"/>
+      <c r="I24" s="66"/>
+      <c r="J24" s="66"/>
+      <c r="K24" s="66"/>
+      <c r="L24" s="67"/>
+    </row>
+    <row r="25" spans="2:12">
+      <c r="B25" s="65"/>
+      <c r="C25" s="66"/>
+      <c r="D25" s="66"/>
+      <c r="E25" s="66"/>
+      <c r="F25" s="66"/>
+      <c r="G25" s="66"/>
+      <c r="H25" s="66"/>
+      <c r="I25" s="66"/>
+      <c r="J25" s="66"/>
+      <c r="K25" s="66"/>
+      <c r="L25" s="67"/>
+    </row>
+    <row r="26" spans="2:12">
+      <c r="B26" s="65"/>
+      <c r="C26" s="66"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="66"/>
+      <c r="F26" s="66"/>
+      <c r="G26" s="66"/>
+      <c r="H26" s="66"/>
+      <c r="I26" s="66"/>
+      <c r="J26" s="66"/>
+      <c r="K26" s="66"/>
+      <c r="L26" s="67"/>
+    </row>
+    <row r="27" spans="2:12">
+      <c r="B27" s="65"/>
+      <c r="C27" s="66"/>
+      <c r="D27" s="66"/>
+      <c r="E27" s="66"/>
+      <c r="F27" s="66"/>
+      <c r="G27" s="66"/>
+      <c r="H27" s="66"/>
+      <c r="I27" s="66"/>
+      <c r="J27" s="66"/>
+      <c r="K27" s="66"/>
+      <c r="L27" s="67"/>
+    </row>
+    <row r="28" spans="2:12">
+      <c r="B28" s="65"/>
+      <c r="C28" s="66"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="66"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="66"/>
+      <c r="H28" s="66"/>
+      <c r="I28" s="66"/>
+      <c r="J28" s="66"/>
+      <c r="K28" s="66"/>
+      <c r="L28" s="67"/>
+    </row>
+    <row r="29" spans="2:12">
+      <c r="B29" s="65"/>
+      <c r="C29" s="66"/>
+      <c r="D29" s="66"/>
+      <c r="E29" s="66"/>
+      <c r="F29" s="66"/>
+      <c r="G29" s="66"/>
+      <c r="H29" s="66"/>
+      <c r="I29" s="66"/>
+      <c r="J29" s="66"/>
+      <c r="K29" s="66"/>
+      <c r="L29" s="67"/>
+    </row>
+    <row r="30" spans="2:12">
+      <c r="B30" s="62"/>
+      <c r="C30" s="76" t="s">
+        <v>182</v>
+      </c>
+      <c r="D30" s="76" t="s">
+        <v>184</v>
+      </c>
+      <c r="E30" s="63"/>
+      <c r="F30" s="63"/>
+      <c r="G30" s="63"/>
+      <c r="H30" s="63"/>
+      <c r="I30" s="63"/>
+      <c r="J30" s="81" t="s">
+        <v>183</v>
+      </c>
+      <c r="K30" s="79"/>
+      <c r="L30" s="80"/>
+    </row>
+    <row r="31" spans="2:12">
+      <c r="B31" s="68"/>
+      <c r="C31" s="69"/>
+      <c r="D31" s="69"/>
+      <c r="E31" s="69"/>
+      <c r="F31" s="69"/>
+      <c r="G31" s="69"/>
+      <c r="H31" s="69"/>
+      <c r="I31" s="69"/>
+      <c r="J31" s="69"/>
+      <c r="K31" s="69"/>
+      <c r="L31" s="70"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add new customer, session, booking all working. Pre-double book prevention trial
</commit_message>
<xml_diff>
--- a/Project Planning/Project Drawings.xlsx
+++ b/Project Planning/Project Drawings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colinmorrison/codeclan_work/Resistance_Temple/Project Planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE2A276-BF0E-934C-BCBF-C0FD490C5AC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6BE57F-D890-3E4C-A99A-7D99107CD850}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33000" windowHeight="20500" activeTab="8" xr2:uid="{056C3CC7-3EA0-BF47-B5DA-A9694FF9AEB8}"/>
   </bookViews>
@@ -5393,7 +5393,7 @@
   <dimension ref="B3:L31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14:L15"/>
+      <selection activeCell="Q10" activeCellId="1" sqref="K24 Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
CSS Styling began, work in progress
</commit_message>
<xml_diff>
--- a/Project Planning/Project Drawings.xlsx
+++ b/Project Planning/Project Drawings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colinmorrison/codeclan_work/Resistance_Temple/Project Planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6BE57F-D890-3E4C-A99A-7D99107CD850}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF740D67-195C-C44F-8592-585C76120462}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33000" windowHeight="20500" activeTab="8" xr2:uid="{056C3CC7-3EA0-BF47-B5DA-A9694FF9AEB8}"/>
   </bookViews>
@@ -1296,54 +1296,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
@@ -1366,6 +1318,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3750,18 +3750,18 @@
     </row>
     <row r="9" spans="2:9" ht="17" thickBot="1"/>
     <row r="10" spans="2:9" s="5" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="E10" s="46" t="s">
+      <c r="C10" s="67"/>
+      <c r="E10" s="66" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="47"/>
-      <c r="H10" s="46" t="s">
+      <c r="F10" s="67"/>
+      <c r="H10" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="I10" s="47"/>
+      <c r="I10" s="67"/>
     </row>
     <row r="11" spans="2:9">
       <c r="B11" s="2" t="s">
@@ -4184,32 +4184,32 @@
     </row>
     <row r="9" spans="2:9" ht="17" thickBot="1"/>
     <row r="10" spans="2:9" s="5" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="E10" s="46" t="s">
+      <c r="C10" s="67"/>
+      <c r="E10" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="47"/>
-      <c r="H10" s="46" t="s">
+      <c r="F10" s="67"/>
+      <c r="H10" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="I10" s="47"/>
+      <c r="I10" s="67"/>
     </row>
     <row r="11" spans="2:9" ht="17" thickBot="1">
-      <c r="B11" s="56" t="s">
+      <c r="B11" s="68" t="s">
         <v>101</v>
       </c>
-      <c r="C11" s="57"/>
-      <c r="E11" s="56" t="s">
+      <c r="C11" s="69"/>
+      <c r="E11" s="68" t="s">
         <v>101</v>
       </c>
-      <c r="F11" s="57"/>
-      <c r="H11" s="56" t="s">
+      <c r="F11" s="69"/>
+      <c r="H11" s="68" t="s">
         <v>101</v>
       </c>
-      <c r="I11" s="57"/>
+      <c r="I11" s="69"/>
     </row>
     <row r="12" spans="2:9">
       <c r="B12" s="3" t="s">
@@ -4349,114 +4349,114 @@
       <c r="I20" s="4"/>
     </row>
     <row r="21" spans="2:10" ht="17" thickBot="1">
-      <c r="B21" s="56" t="s">
+      <c r="B21" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="C21" s="57"/>
-      <c r="E21" s="56" t="s">
+      <c r="C21" s="69"/>
+      <c r="E21" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="F21" s="57"/>
-      <c r="H21" s="56" t="s">
+      <c r="F21" s="69"/>
+      <c r="H21" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="I21" s="57"/>
+      <c r="I21" s="69"/>
     </row>
     <row r="22" spans="2:10">
-      <c r="B22" s="54" t="s">
+      <c r="B22" s="76" t="s">
         <v>103</v>
       </c>
-      <c r="C22" s="55"/>
+      <c r="C22" s="77"/>
       <c r="D22" s="15"/>
-      <c r="E22" s="54"/>
-      <c r="F22" s="55"/>
+      <c r="E22" s="76"/>
+      <c r="F22" s="77"/>
       <c r="G22" s="15"/>
-      <c r="H22" s="54" t="s">
+      <c r="H22" s="76" t="s">
         <v>104</v>
       </c>
-      <c r="I22" s="55"/>
+      <c r="I22" s="77"/>
     </row>
     <row r="23" spans="2:10">
-      <c r="B23" s="48" t="s">
+      <c r="B23" s="74" t="s">
         <v>105</v>
       </c>
-      <c r="C23" s="49"/>
+      <c r="C23" s="75"/>
       <c r="D23" s="15"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="49"/>
+      <c r="E23" s="74"/>
+      <c r="F23" s="75"/>
       <c r="G23" s="15"/>
-      <c r="H23" s="48"/>
-      <c r="I23" s="49"/>
+      <c r="H23" s="74"/>
+      <c r="I23" s="75"/>
     </row>
     <row r="24" spans="2:10">
-      <c r="B24" s="48" t="s">
+      <c r="B24" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="C24" s="49"/>
+      <c r="C24" s="75"/>
       <c r="D24" s="15"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="49"/>
+      <c r="E24" s="74"/>
+      <c r="F24" s="75"/>
       <c r="G24" s="15"/>
-      <c r="H24" s="48"/>
-      <c r="I24" s="49"/>
+      <c r="H24" s="74"/>
+      <c r="I24" s="75"/>
     </row>
     <row r="25" spans="2:10">
-      <c r="B25" s="48" t="s">
+      <c r="B25" s="74" t="s">
         <v>106</v>
       </c>
-      <c r="C25" s="49"/>
+      <c r="C25" s="75"/>
       <c r="D25" s="15"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="49"/>
+      <c r="E25" s="74"/>
+      <c r="F25" s="75"/>
       <c r="G25" s="15"/>
-      <c r="H25" s="48"/>
-      <c r="I25" s="49"/>
+      <c r="H25" s="74"/>
+      <c r="I25" s="75"/>
     </row>
     <row r="26" spans="2:10">
-      <c r="B26" s="48" t="s">
+      <c r="B26" s="74" t="s">
         <v>108</v>
       </c>
-      <c r="C26" s="49"/>
+      <c r="C26" s="75"/>
       <c r="D26" s="15"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="49"/>
+      <c r="E26" s="74"/>
+      <c r="F26" s="75"/>
       <c r="G26" s="15"/>
-      <c r="H26" s="48"/>
-      <c r="I26" s="49"/>
+      <c r="H26" s="74"/>
+      <c r="I26" s="75"/>
     </row>
     <row r="27" spans="2:10">
-      <c r="B27" s="48"/>
-      <c r="C27" s="49"/>
+      <c r="B27" s="74"/>
+      <c r="C27" s="75"/>
       <c r="D27" s="15"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="49"/>
+      <c r="E27" s="74"/>
+      <c r="F27" s="75"/>
       <c r="G27" s="15"/>
-      <c r="H27" s="48"/>
-      <c r="I27" s="49"/>
+      <c r="H27" s="74"/>
+      <c r="I27" s="75"/>
     </row>
     <row r="28" spans="2:10">
-      <c r="B28" s="50"/>
-      <c r="C28" s="51"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="51"/>
-      <c r="H28" s="50"/>
-      <c r="I28" s="51"/>
+      <c r="B28" s="72"/>
+      <c r="C28" s="73"/>
+      <c r="E28" s="72"/>
+      <c r="F28" s="73"/>
+      <c r="H28" s="72"/>
+      <c r="I28" s="73"/>
     </row>
     <row r="29" spans="2:10">
-      <c r="B29" s="50"/>
-      <c r="C29" s="51"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="51"/>
-      <c r="H29" s="50"/>
-      <c r="I29" s="51"/>
+      <c r="B29" s="72"/>
+      <c r="C29" s="73"/>
+      <c r="E29" s="72"/>
+      <c r="F29" s="73"/>
+      <c r="H29" s="72"/>
+      <c r="I29" s="73"/>
     </row>
     <row r="30" spans="2:10" ht="17" thickBot="1">
-      <c r="B30" s="52"/>
-      <c r="C30" s="53"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="53"/>
-      <c r="H30" s="52"/>
-      <c r="I30" s="53"/>
+      <c r="B30" s="70"/>
+      <c r="C30" s="71"/>
+      <c r="E30" s="70"/>
+      <c r="F30" s="71"/>
+      <c r="H30" s="70"/>
+      <c r="I30" s="71"/>
     </row>
     <row r="31" spans="2:10">
       <c r="B31" s="15" t="s">
@@ -4468,6 +4468,33 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B26:C26"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="H10:I10"/>
@@ -4477,33 +4504,6 @@
     <mergeCell ref="H11:I11"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H26:I26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4530,7 +4530,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:6">
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="78" t="s">
         <v>55</v>
       </c>
       <c r="D3" s="16" t="s">
@@ -4541,7 +4541,7 @@
       </c>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="59"/>
+      <c r="B4" s="79"/>
       <c r="D4" s="18" t="s">
         <v>63</v>
       </c>
@@ -4559,7 +4559,7 @@
       </c>
     </row>
     <row r="8" spans="2:6">
-      <c r="C8" s="60" t="s">
+      <c r="C8" s="80" t="s">
         <v>56</v>
       </c>
       <c r="E8" s="16" t="s">
@@ -4570,7 +4570,7 @@
       </c>
     </row>
     <row r="9" spans="2:6">
-      <c r="C9" s="61"/>
+      <c r="C9" s="81"/>
       <c r="E9" s="18" t="s">
         <v>66</v>
       </c>
@@ -4595,7 +4595,7 @@
       </c>
     </row>
     <row r="14" spans="2:6">
-      <c r="C14" s="60" t="s">
+      <c r="C14" s="80" t="s">
         <v>57</v>
       </c>
       <c r="E14" s="16" t="s">
@@ -4606,7 +4606,7 @@
       </c>
     </row>
     <row r="15" spans="2:6">
-      <c r="C15" s="61"/>
+      <c r="C15" s="81"/>
       <c r="E15" s="17" t="s">
         <v>70</v>
       </c>
@@ -4615,7 +4615,7 @@
       </c>
     </row>
     <row r="18" spans="3:8">
-      <c r="C18" s="60" t="s">
+      <c r="C18" s="80" t="s">
         <v>58</v>
       </c>
       <c r="E18" s="16" t="s">
@@ -4626,7 +4626,7 @@
       </c>
     </row>
     <row r="19" spans="3:8">
-      <c r="C19" s="61"/>
+      <c r="C19" s="81"/>
       <c r="E19" s="18" t="s">
         <v>71</v>
       </c>
@@ -4651,7 +4651,7 @@
       </c>
     </row>
     <row r="24" spans="3:8">
-      <c r="C24" s="60" t="s">
+      <c r="C24" s="80" t="s">
         <v>60</v>
       </c>
       <c r="E24" s="16" t="s">
@@ -4665,7 +4665,7 @@
       </c>
     </row>
     <row r="25" spans="3:8">
-      <c r="C25" s="61"/>
+      <c r="C25" s="81"/>
       <c r="E25" s="18" t="s">
         <v>140</v>
       </c>
@@ -4688,7 +4688,7 @@
       </c>
     </row>
     <row r="30" spans="3:8">
-      <c r="C30" s="60" t="s">
+      <c r="C30" s="80" t="s">
         <v>61</v>
       </c>
       <c r="E30" s="13" t="s">
@@ -4702,7 +4702,7 @@
       </c>
     </row>
     <row r="31" spans="3:8">
-      <c r="C31" s="61"/>
+      <c r="C31" s="81"/>
     </row>
     <row r="33" spans="3:10">
       <c r="E33" s="13" t="s">
@@ -4710,7 +4710,7 @@
       </c>
     </row>
     <row r="37" spans="3:10">
-      <c r="C37" s="60" t="s">
+      <c r="C37" s="80" t="s">
         <v>59</v>
       </c>
       <c r="D37" s="20"/>
@@ -4722,7 +4722,7 @@
       </c>
     </row>
     <row r="38" spans="3:10">
-      <c r="C38" s="61"/>
+      <c r="C38" s="81"/>
       <c r="D38" s="20"/>
       <c r="E38" s="17" t="s">
         <v>80</v>
@@ -5018,34 +5018,34 @@
   <sheetData>
     <row r="30" spans="2:9" ht="17" thickBot="1"/>
     <row r="31" spans="2:9" ht="20" thickBot="1">
-      <c r="B31" s="46" t="s">
+      <c r="B31" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="C31" s="47"/>
+      <c r="C31" s="67"/>
       <c r="D31" s="5"/>
-      <c r="E31" s="46" t="s">
+      <c r="E31" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="F31" s="47"/>
+      <c r="F31" s="67"/>
       <c r="G31" s="5"/>
-      <c r="H31" s="46" t="s">
+      <c r="H31" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="I31" s="47"/>
+      <c r="I31" s="67"/>
     </row>
     <row r="32" spans="2:9" ht="17" thickBot="1">
-      <c r="B32" s="56" t="s">
+      <c r="B32" s="68" t="s">
         <v>101</v>
       </c>
-      <c r="C32" s="57"/>
-      <c r="E32" s="56" t="s">
+      <c r="C32" s="69"/>
+      <c r="E32" s="68" t="s">
         <v>101</v>
       </c>
-      <c r="F32" s="57"/>
-      <c r="H32" s="56" t="s">
+      <c r="F32" s="69"/>
+      <c r="H32" s="68" t="s">
         <v>101</v>
       </c>
-      <c r="I32" s="57"/>
+      <c r="I32" s="69"/>
     </row>
     <row r="33" spans="2:9">
       <c r="B33" s="3" t="s">
@@ -5181,34 +5181,34 @@
     </row>
     <row r="44" spans="2:9" ht="17" thickBot="1"/>
     <row r="45" spans="2:9" ht="20" thickBot="1">
-      <c r="B45" s="46" t="s">
+      <c r="B45" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="C45" s="47"/>
+      <c r="C45" s="67"/>
       <c r="D45" s="5"/>
-      <c r="E45" s="46" t="s">
+      <c r="E45" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="F45" s="47"/>
+      <c r="F45" s="67"/>
       <c r="G45" s="5"/>
-      <c r="H45" s="46" t="s">
+      <c r="H45" s="66" t="s">
         <v>137</v>
       </c>
-      <c r="I45" s="47"/>
+      <c r="I45" s="67"/>
     </row>
     <row r="46" spans="2:9" ht="17" thickBot="1">
-      <c r="B46" s="56" t="s">
+      <c r="B46" s="68" t="s">
         <v>101</v>
       </c>
-      <c r="C46" s="57"/>
-      <c r="E46" s="56" t="s">
+      <c r="C46" s="69"/>
+      <c r="E46" s="68" t="s">
         <v>101</v>
       </c>
-      <c r="F46" s="57"/>
-      <c r="H46" s="56" t="s">
+      <c r="F46" s="69"/>
+      <c r="H46" s="68" t="s">
         <v>101</v>
       </c>
-      <c r="I46" s="57"/>
+      <c r="I46" s="69"/>
     </row>
     <row r="47" spans="2:9">
       <c r="B47" s="3" t="s">
@@ -5344,18 +5344,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="H46:I46"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="E31:F31"/>
     <mergeCell ref="H31:I31"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="H32:I32"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="H46:I46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5393,7 +5393,7 @@
   <dimension ref="B3:L31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q10" activeCellId="1" sqref="K24 Q10"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5403,419 +5403,419 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:12">
-      <c r="B3" s="62"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="63"/>
-      <c r="L3" s="64"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="48"/>
     </row>
     <row r="4" spans="2:12">
-      <c r="B4" s="65"/>
-      <c r="C4" s="78" t="s">
+      <c r="B4" s="49"/>
+      <c r="C4" s="62" t="s">
         <v>172</v>
       </c>
-      <c r="D4" s="78" t="s">
+      <c r="D4" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="78" t="s">
+      <c r="E4" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="78" t="s">
+      <c r="F4" s="62" t="s">
         <v>170</v>
       </c>
-      <c r="G4" s="78" t="s">
+      <c r="G4" s="62" t="s">
         <v>171</v>
       </c>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="77" t="s">
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="61" t="s">
         <v>168</v>
       </c>
-      <c r="K4" s="76" t="s">
+      <c r="K4" s="60" t="s">
         <v>169</v>
       </c>
-      <c r="L4" s="67"/>
+      <c r="L4" s="51"/>
     </row>
     <row r="5" spans="2:12">
-      <c r="B5" s="68"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="69"/>
-      <c r="K5" s="69"/>
-      <c r="L5" s="70"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="54"/>
     </row>
     <row r="6" spans="2:12">
-      <c r="B6" s="65"/>
-      <c r="C6" s="66"/>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="66"/>
-      <c r="J6" s="66"/>
-      <c r="K6" s="66"/>
-      <c r="L6" s="67"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="51"/>
     </row>
     <row r="7" spans="2:12">
-      <c r="B7" s="65"/>
-      <c r="C7" s="72" t="s">
+      <c r="B7" s="49"/>
+      <c r="C7" s="56" t="s">
         <v>173</v>
       </c>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="64"/>
-      <c r="G7" s="66"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="63"/>
-      <c r="J7" s="63"/>
-      <c r="K7" s="64"/>
-      <c r="L7" s="67"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="51"/>
     </row>
     <row r="8" spans="2:12">
-      <c r="B8" s="65"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="66"/>
-      <c r="E8" s="66"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="66"/>
-      <c r="H8" s="65"/>
-      <c r="I8" s="66"/>
-      <c r="J8" s="66"/>
-      <c r="K8" s="67"/>
-      <c r="L8" s="67"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="51"/>
+      <c r="L8" s="51"/>
     </row>
     <row r="9" spans="2:12">
-      <c r="B9" s="65"/>
-      <c r="C9" s="68"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="70"/>
-      <c r="G9" s="66"/>
-      <c r="H9" s="65"/>
-      <c r="I9" s="66"/>
-      <c r="J9" s="66"/>
-      <c r="K9" s="67"/>
-      <c r="L9" s="67"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="51"/>
+      <c r="L9" s="51"/>
     </row>
     <row r="10" spans="2:12">
-      <c r="B10" s="65"/>
-      <c r="C10" s="66"/>
-      <c r="D10" s="66"/>
-      <c r="E10" s="66"/>
-      <c r="F10" s="66"/>
-      <c r="G10" s="66"/>
-      <c r="H10" s="65"/>
-      <c r="I10" s="71" t="s">
+      <c r="B10" s="49"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="55" t="s">
         <v>178</v>
       </c>
-      <c r="J10" s="66"/>
-      <c r="K10" s="67"/>
-      <c r="L10" s="67"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="51"/>
+      <c r="L10" s="51"/>
     </row>
     <row r="11" spans="2:12">
-      <c r="B11" s="65"/>
-      <c r="C11" s="72" t="s">
+      <c r="B11" s="49"/>
+      <c r="C11" s="56" t="s">
         <v>174</v>
       </c>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="66"/>
-      <c r="H11" s="65"/>
-      <c r="I11" s="66"/>
-      <c r="J11" s="66"/>
-      <c r="K11" s="67"/>
-      <c r="L11" s="67"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="51"/>
     </row>
     <row r="12" spans="2:12">
-      <c r="B12" s="65"/>
-      <c r="C12" s="65" t="s">
+      <c r="B12" s="49"/>
+      <c r="C12" s="49" t="s">
         <v>176</v>
       </c>
-      <c r="D12" s="66"/>
-      <c r="E12" s="66"/>
-      <c r="F12" s="67"/>
-      <c r="G12" s="66"/>
-      <c r="H12" s="65"/>
-      <c r="I12" s="66"/>
-      <c r="J12" s="66"/>
-      <c r="K12" s="67"/>
-      <c r="L12" s="67"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="51"/>
     </row>
     <row r="13" spans="2:12">
-      <c r="B13" s="65"/>
-      <c r="C13" s="65" t="s">
+      <c r="B13" s="49"/>
+      <c r="C13" s="49" t="s">
         <v>177</v>
       </c>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="67"/>
-      <c r="G13" s="66"/>
-      <c r="H13" s="65"/>
-      <c r="I13" s="66"/>
-      <c r="J13" s="66"/>
-      <c r="K13" s="67"/>
-      <c r="L13" s="67"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="50"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="51"/>
+      <c r="L13" s="51"/>
     </row>
     <row r="14" spans="2:12">
-      <c r="B14" s="65"/>
-      <c r="C14" s="73" t="s">
+      <c r="B14" s="49"/>
+      <c r="C14" s="57" t="s">
         <v>175</v>
       </c>
-      <c r="D14" s="69"/>
-      <c r="E14" s="69"/>
-      <c r="F14" s="70"/>
-      <c r="G14" s="66"/>
-      <c r="H14" s="65"/>
-      <c r="I14" s="66"/>
-      <c r="J14" s="66"/>
-      <c r="K14" s="67"/>
-      <c r="L14" s="67"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="50"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="51"/>
+      <c r="L14" s="51"/>
     </row>
     <row r="15" spans="2:12">
-      <c r="B15" s="65"/>
-      <c r="C15" s="66"/>
-      <c r="D15" s="66"/>
-      <c r="E15" s="66"/>
-      <c r="F15" s="66"/>
-      <c r="G15" s="66"/>
-      <c r="H15" s="65"/>
-      <c r="I15" s="66"/>
-      <c r="J15" s="66"/>
-      <c r="K15" s="67"/>
-      <c r="L15" s="67"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="50"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="51"/>
+      <c r="L15" s="51"/>
     </row>
     <row r="16" spans="2:12">
-      <c r="B16" s="65"/>
-      <c r="C16" s="74" t="s">
+      <c r="B16" s="49"/>
+      <c r="C16" s="58" t="s">
         <v>179</v>
       </c>
-      <c r="D16" s="63"/>
-      <c r="E16" s="63"/>
-      <c r="F16" s="64"/>
-      <c r="G16" s="66"/>
-      <c r="H16" s="65"/>
-      <c r="I16" s="66"/>
-      <c r="J16" s="66"/>
-      <c r="K16" s="67"/>
-      <c r="L16" s="67"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="50"/>
+      <c r="K16" s="51"/>
+      <c r="L16" s="51"/>
     </row>
     <row r="17" spans="2:12">
-      <c r="B17" s="65"/>
-      <c r="C17" s="75" t="s">
+      <c r="B17" s="49"/>
+      <c r="C17" s="59" t="s">
         <v>180</v>
       </c>
-      <c r="D17" s="66"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="67"/>
-      <c r="G17" s="66"/>
-      <c r="H17" s="65"/>
-      <c r="I17" s="66"/>
-      <c r="J17" s="66"/>
-      <c r="K17" s="67"/>
-      <c r="L17" s="67"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="50"/>
+      <c r="J17" s="50"/>
+      <c r="K17" s="51"/>
+      <c r="L17" s="51"/>
     </row>
     <row r="18" spans="2:12">
-      <c r="B18" s="65"/>
-      <c r="C18" s="75" t="s">
+      <c r="B18" s="49"/>
+      <c r="C18" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="D18" s="66"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="67"/>
-      <c r="G18" s="66"/>
-      <c r="H18" s="65"/>
-      <c r="I18" s="66"/>
-      <c r="J18" s="66"/>
-      <c r="K18" s="67"/>
-      <c r="L18" s="67"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="50"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="50"/>
+      <c r="J18" s="50"/>
+      <c r="K18" s="51"/>
+      <c r="L18" s="51"/>
     </row>
     <row r="19" spans="2:12">
-      <c r="B19" s="65"/>
-      <c r="C19" s="65"/>
-      <c r="D19" s="66"/>
-      <c r="E19" s="66"/>
-      <c r="F19" s="67"/>
-      <c r="G19" s="66"/>
-      <c r="H19" s="65"/>
-      <c r="I19" s="66"/>
-      <c r="J19" s="66"/>
-      <c r="K19" s="67"/>
-      <c r="L19" s="67"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="50"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="51"/>
     </row>
     <row r="20" spans="2:12">
-      <c r="B20" s="65"/>
-      <c r="C20" s="68"/>
-      <c r="D20" s="69"/>
-      <c r="E20" s="69"/>
-      <c r="F20" s="70"/>
-      <c r="G20" s="66"/>
-      <c r="H20" s="68"/>
-      <c r="I20" s="69"/>
-      <c r="J20" s="69"/>
-      <c r="K20" s="70"/>
-      <c r="L20" s="67"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="50"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="53"/>
+      <c r="K20" s="54"/>
+      <c r="L20" s="51"/>
     </row>
     <row r="21" spans="2:12">
-      <c r="B21" s="65"/>
-      <c r="C21" s="66"/>
-      <c r="D21" s="66"/>
-      <c r="E21" s="66"/>
-      <c r="F21" s="66"/>
-      <c r="G21" s="66"/>
-      <c r="H21" s="66"/>
-      <c r="I21" s="66"/>
-      <c r="J21" s="66"/>
-      <c r="K21" s="66"/>
-      <c r="L21" s="67"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="50"/>
+      <c r="H21" s="50"/>
+      <c r="I21" s="50"/>
+      <c r="J21" s="50"/>
+      <c r="K21" s="50"/>
+      <c r="L21" s="51"/>
     </row>
     <row r="22" spans="2:12">
-      <c r="B22" s="65"/>
-      <c r="C22" s="66"/>
-      <c r="D22" s="66"/>
-      <c r="E22" s="66"/>
-      <c r="F22" s="66"/>
-      <c r="G22" s="66"/>
-      <c r="H22" s="66"/>
-      <c r="I22" s="66"/>
-      <c r="J22" s="66"/>
-      <c r="K22" s="66"/>
-      <c r="L22" s="67"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="50"/>
+      <c r="H22" s="50"/>
+      <c r="I22" s="50"/>
+      <c r="J22" s="50"/>
+      <c r="K22" s="50"/>
+      <c r="L22" s="51"/>
     </row>
     <row r="23" spans="2:12">
-      <c r="B23" s="65"/>
-      <c r="C23" s="66"/>
-      <c r="D23" s="66"/>
-      <c r="E23" s="66"/>
-      <c r="F23" s="66"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="66"/>
-      <c r="I23" s="66"/>
-      <c r="J23" s="66"/>
-      <c r="K23" s="66"/>
-      <c r="L23" s="67"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="50"/>
+      <c r="H23" s="50"/>
+      <c r="I23" s="50"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="50"/>
+      <c r="L23" s="51"/>
     </row>
     <row r="24" spans="2:12">
-      <c r="B24" s="65"/>
-      <c r="C24" s="66"/>
-      <c r="D24" s="66"/>
-      <c r="E24" s="66"/>
-      <c r="F24" s="66"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="66"/>
-      <c r="I24" s="66"/>
-      <c r="J24" s="66"/>
-      <c r="K24" s="66"/>
-      <c r="L24" s="67"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="50"/>
+      <c r="H24" s="50"/>
+      <c r="I24" s="50"/>
+      <c r="J24" s="50"/>
+      <c r="K24" s="50"/>
+      <c r="L24" s="51"/>
     </row>
     <row r="25" spans="2:12">
-      <c r="B25" s="65"/>
-      <c r="C25" s="66"/>
-      <c r="D25" s="66"/>
-      <c r="E25" s="66"/>
-      <c r="F25" s="66"/>
-      <c r="G25" s="66"/>
-      <c r="H25" s="66"/>
-      <c r="I25" s="66"/>
-      <c r="J25" s="66"/>
-      <c r="K25" s="66"/>
-      <c r="L25" s="67"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="50"/>
+      <c r="H25" s="50"/>
+      <c r="I25" s="50"/>
+      <c r="J25" s="50"/>
+      <c r="K25" s="50"/>
+      <c r="L25" s="51"/>
     </row>
     <row r="26" spans="2:12">
-      <c r="B26" s="65"/>
-      <c r="C26" s="66"/>
-      <c r="D26" s="66"/>
-      <c r="E26" s="66"/>
-      <c r="F26" s="66"/>
-      <c r="G26" s="66"/>
-      <c r="H26" s="66"/>
-      <c r="I26" s="66"/>
-      <c r="J26" s="66"/>
-      <c r="K26" s="66"/>
-      <c r="L26" s="67"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="50"/>
+      <c r="J26" s="50"/>
+      <c r="K26" s="50"/>
+      <c r="L26" s="51"/>
     </row>
     <row r="27" spans="2:12">
-      <c r="B27" s="65"/>
-      <c r="C27" s="66"/>
-      <c r="D27" s="66"/>
-      <c r="E27" s="66"/>
-      <c r="F27" s="66"/>
-      <c r="G27" s="66"/>
-      <c r="H27" s="66"/>
-      <c r="I27" s="66"/>
-      <c r="J27" s="66"/>
-      <c r="K27" s="66"/>
-      <c r="L27" s="67"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="50"/>
+      <c r="H27" s="50"/>
+      <c r="I27" s="50"/>
+      <c r="J27" s="50"/>
+      <c r="K27" s="50"/>
+      <c r="L27" s="51"/>
     </row>
     <row r="28" spans="2:12">
-      <c r="B28" s="65"/>
-      <c r="C28" s="66"/>
-      <c r="D28" s="66"/>
-      <c r="E28" s="66"/>
-      <c r="F28" s="66"/>
-      <c r="G28" s="66"/>
-      <c r="H28" s="66"/>
-      <c r="I28" s="66"/>
-      <c r="J28" s="66"/>
-      <c r="K28" s="66"/>
-      <c r="L28" s="67"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
+      <c r="K28" s="50"/>
+      <c r="L28" s="51"/>
     </row>
     <row r="29" spans="2:12">
-      <c r="B29" s="65"/>
-      <c r="C29" s="66"/>
-      <c r="D29" s="66"/>
-      <c r="E29" s="66"/>
-      <c r="F29" s="66"/>
-      <c r="G29" s="66"/>
-      <c r="H29" s="66"/>
-      <c r="I29" s="66"/>
-      <c r="J29" s="66"/>
-      <c r="K29" s="66"/>
-      <c r="L29" s="67"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="50"/>
+      <c r="K29" s="50"/>
+      <c r="L29" s="51"/>
     </row>
     <row r="30" spans="2:12">
-      <c r="B30" s="62"/>
-      <c r="C30" s="76" t="s">
+      <c r="B30" s="46"/>
+      <c r="C30" s="60" t="s">
         <v>182</v>
       </c>
-      <c r="D30" s="76" t="s">
+      <c r="D30" s="60" t="s">
         <v>184</v>
       </c>
-      <c r="E30" s="63"/>
-      <c r="F30" s="63"/>
-      <c r="G30" s="63"/>
-      <c r="H30" s="63"/>
-      <c r="I30" s="63"/>
-      <c r="J30" s="81" t="s">
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="65" t="s">
         <v>183</v>
       </c>
-      <c r="K30" s="79"/>
-      <c r="L30" s="80"/>
+      <c r="K30" s="63"/>
+      <c r="L30" s="64"/>
     </row>
     <row r="31" spans="2:12">
-      <c r="B31" s="68"/>
-      <c r="C31" s="69"/>
-      <c r="D31" s="69"/>
-      <c r="E31" s="69"/>
-      <c r="F31" s="69"/>
-      <c r="G31" s="69"/>
-      <c r="H31" s="69"/>
-      <c r="I31" s="69"/>
-      <c r="J31" s="69"/>
-      <c r="K31" s="69"/>
-      <c r="L31" s="70"/>
+      <c r="B31" s="52"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="53"/>
+      <c r="E31" s="53"/>
+      <c r="F31" s="53"/>
+      <c r="G31" s="53"/>
+      <c r="H31" s="53"/>
+      <c r="I31" s="53"/>
+      <c r="J31" s="53"/>
+      <c r="K31" s="53"/>
+      <c r="L31" s="54"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Class tests active and passed
</commit_message>
<xml_diff>
--- a/Project Planning/Project Drawings.xlsx
+++ b/Project Planning/Project Drawings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colinmorrison/codeclan_work/Resistance_Temple/Project Planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF740D67-195C-C44F-8592-585C76120462}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1924F0F7-31B4-7342-AC95-6733830FE3F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33000" windowHeight="20500" activeTab="8" xr2:uid="{056C3CC7-3EA0-BF47-B5DA-A9694FF9AEB8}"/>
   </bookViews>
@@ -5393,7 +5393,7 @@
   <dimension ref="B3:L31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Additional images viewable and zoomable in browser
</commit_message>
<xml_diff>
--- a/Project Planning/Project Drawings.xlsx
+++ b/Project Planning/Project Drawings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colinmorrison/codeclan_work/Resistance_Temple/Project Planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28CD0B5-F86B-E946-9FBD-78BAC0DB58D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E609A76-193A-8F4A-8046-020C68FEAA83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1900" yWindow="-20500" windowWidth="33000" windowHeight="20500" xr2:uid="{056C3CC7-3EA0-BF47-B5DA-A9694FF9AEB8}"/>
+    <workbookView xWindow="-1900" yWindow="-20500" windowWidth="33000" windowHeight="20500" activeTab="3" xr2:uid="{056C3CC7-3EA0-BF47-B5DA-A9694FF9AEB8}"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="179">
   <si>
     <t>1) We have a Gym - Resistance Temple</t>
   </si>
@@ -577,6 +577,9 @@
   </si>
   <si>
     <t>Persistent Storage and Transactions</t>
+  </si>
+  <si>
+    <t>Additional Information</t>
   </si>
 </sst>
 </file>
@@ -1243,54 +1246,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1320,66 +1275,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1390,54 +1285,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1462,6 +1309,162 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2207,15 +2210,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>719666</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>21165</xdr:rowOff>
+      <xdr:colOff>719667</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>21164</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1566333</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>10582</xdr:rowOff>
+      <xdr:colOff>1576917</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>42335</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2230,12 +2233,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="-2439459" y="4259790"/>
-          <a:ext cx="7715251" cy="846667"/>
+          <a:off x="-4561419" y="6381750"/>
+          <a:ext cx="11969755" cy="857250"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 99931"/>
+            <a:gd name="adj1" fmla="val 99955"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln w="12700">
@@ -2263,13 +2266,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>730250</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>21166</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1576916</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>21166</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2316,13 +2319,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>734485</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>14816</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1581151</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>14816</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2369,13 +2372,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>719666</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>10584</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2422,13 +2425,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>730244</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>169333</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1576910</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>169333</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2475,13 +2478,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>730248</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>179916</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1576914</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>179916</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2528,13 +2531,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>10583</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1576916</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2581,13 +2584,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1344083</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>105833</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>990599</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>116417</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2634,13 +2637,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1333500</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>992716</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2687,13 +2690,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1344084</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>963085</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>84667</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2742,13 +2745,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>427568</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>152401</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>984254</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>116418</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2797,13 +2800,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>10583</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>52917</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1534583</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>52917</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2850,13 +2853,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>105833</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>941916</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>105833</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2903,13 +2906,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>31749</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>105833</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>973665</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>105833</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2956,13 +2959,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>10583</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>116417</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>952499</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>116417</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3009,13 +3012,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>105835</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>941916</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>105835</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3062,13 +3065,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>941916</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3115,13 +3118,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>84666</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>793750</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>84666</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3168,13 +3171,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>84668</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>793750</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>84668</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3221,13 +3224,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>84664</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>793750</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>84664</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3274,13 +3277,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>95247</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>793750</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>95247</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3327,13 +3330,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>433916</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>105833</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>992716</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>105833</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3380,13 +3383,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>740834</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>14816</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>14816</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3433,13 +3436,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>16932</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>116417</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>958848</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>116417</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3480,6 +3483,103 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>730248</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>201079</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1576914</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>201079</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="Straight Arrow Connector 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC51850C-1723-0046-9D7A-06879A5C6585}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1005415" y="9334496"/>
+          <a:ext cx="846666" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>55034</xdr:colOff>
+      <xdr:row>129</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DE1C0C9-F1A5-FF41-8D36-A996DA67300A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="52917" y="13059833"/>
+          <a:ext cx="8267700" cy="12788900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -4024,7 +4124,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7C4CE97-99AC-5D44-A588-63C7E74AFBA6}">
   <dimension ref="B2:J20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
@@ -4057,18 +4157,18 @@
     </row>
     <row r="9" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="2:9" s="5" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="50"/>
-      <c r="E10" s="49" t="s">
+      <c r="C10" s="78"/>
+      <c r="E10" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="50"/>
-      <c r="H10" s="49" t="s">
+      <c r="F10" s="78"/>
+      <c r="H10" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="50"/>
+      <c r="I10" s="78"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
@@ -4263,32 +4363,32 @@
     </row>
     <row r="9" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="2:9" s="5" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="50"/>
-      <c r="E10" s="49" t="s">
+      <c r="C10" s="78"/>
+      <c r="E10" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="50"/>
-      <c r="H10" s="49" t="s">
+      <c r="F10" s="78"/>
+      <c r="H10" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="50"/>
+      <c r="I10" s="78"/>
     </row>
     <row r="11" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="51" t="s">
+      <c r="B11" s="79" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="52"/>
-      <c r="E11" s="51" t="s">
+      <c r="C11" s="80"/>
+      <c r="E11" s="79" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="52"/>
-      <c r="H11" s="51" t="s">
+      <c r="F11" s="80"/>
+      <c r="H11" s="79" t="s">
         <v>58</v>
       </c>
-      <c r="I11" s="52"/>
+      <c r="I11" s="80"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
@@ -4420,54 +4520,54 @@
       <c r="I19" s="21"/>
     </row>
     <row r="20" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="51" t="s">
+      <c r="B20" s="79" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="52"/>
-      <c r="E20" s="51" t="s">
+      <c r="C20" s="80"/>
+      <c r="E20" s="79" t="s">
         <v>59</v>
       </c>
-      <c r="F20" s="52"/>
-      <c r="H20" s="51" t="s">
+      <c r="F20" s="80"/>
+      <c r="H20" s="79" t="s">
         <v>59</v>
       </c>
-      <c r="I20" s="52"/>
+      <c r="I20" s="80"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B21" s="59"/>
-      <c r="C21" s="60"/>
+      <c r="B21" s="85"/>
+      <c r="C21" s="86"/>
       <c r="D21" s="14"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="60"/>
+      <c r="E21" s="85"/>
+      <c r="F21" s="86"/>
       <c r="G21" s="14"/>
-      <c r="H21" s="59"/>
-      <c r="I21" s="60"/>
+      <c r="H21" s="85"/>
+      <c r="I21" s="86"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B22" s="57"/>
-      <c r="C22" s="58"/>
+      <c r="B22" s="87"/>
+      <c r="C22" s="88"/>
       <c r="D22" s="14"/>
-      <c r="E22" s="57"/>
-      <c r="F22" s="58"/>
+      <c r="E22" s="87"/>
+      <c r="F22" s="88"/>
       <c r="G22" s="14"/>
-      <c r="H22" s="57"/>
-      <c r="I22" s="58"/>
+      <c r="H22" s="87"/>
+      <c r="I22" s="88"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B23" s="55"/>
-      <c r="C23" s="56"/>
-      <c r="E23" s="55"/>
-      <c r="F23" s="56"/>
-      <c r="H23" s="55"/>
-      <c r="I23" s="56"/>
+      <c r="B23" s="81"/>
+      <c r="C23" s="82"/>
+      <c r="E23" s="81"/>
+      <c r="F23" s="82"/>
+      <c r="H23" s="81"/>
+      <c r="I23" s="82"/>
     </row>
     <row r="24" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="53"/>
-      <c r="C24" s="54"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="54"/>
-      <c r="H24" s="53"/>
-      <c r="I24" s="54"/>
+      <c r="B24" s="83"/>
+      <c r="C24" s="84"/>
+      <c r="E24" s="83"/>
+      <c r="F24" s="84"/>
+      <c r="H24" s="83"/>
+      <c r="I24" s="84"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B25" s="14"/>
@@ -4477,6 +4577,12 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="H23:I23"/>
@@ -4492,12 +4598,6 @@
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="E24:F24"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4522,29 +4622,29 @@
   </cols>
   <sheetData>
     <row r="30" spans="2:13" ht="21" x14ac:dyDescent="0.25">
-      <c r="H30" s="78" t="s">
+      <c r="H30" s="62" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="31" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="2:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="49" t="s">
+      <c r="B32" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="C32" s="50"/>
+      <c r="C32" s="78"/>
       <c r="D32" s="5"/>
-      <c r="E32" s="49" t="s">
+      <c r="E32" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="F32" s="50"/>
-      <c r="H32" s="75" t="s">
+      <c r="F32" s="78"/>
+      <c r="H32" s="59" t="s">
         <v>18</v>
       </c>
       <c r="I32" s="5"/>
-      <c r="J32" s="75" t="s">
+      <c r="J32" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="M32" s="75" t="s">
+      <c r="M32" s="59" t="s">
         <v>18</v>
       </c>
     </row>
@@ -4561,13 +4661,13 @@
       <c r="F33" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="H33" s="69" t="s">
+      <c r="H33" s="53" t="s">
         <v>118</v>
       </c>
-      <c r="J33" s="69" t="s">
+      <c r="J33" s="53" t="s">
         <v>118</v>
       </c>
-      <c r="M33" s="69" t="s">
+      <c r="M33" s="53" t="s">
         <v>156</v>
       </c>
     </row>
@@ -4584,13 +4684,13 @@
       <c r="F34" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="H34" s="70" t="s">
+      <c r="H34" s="54" t="s">
         <v>117</v>
       </c>
-      <c r="J34" s="70" t="s">
+      <c r="J34" s="54" t="s">
         <v>123</v>
       </c>
-      <c r="M34" s="70" t="s">
+      <c r="M34" s="54" t="s">
         <v>157</v>
       </c>
     </row>
@@ -4607,13 +4707,13 @@
       <c r="F35" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="H35" s="71" t="s">
+      <c r="H35" s="55" t="s">
         <v>119</v>
       </c>
-      <c r="J35" s="71" t="s">
+      <c r="J35" s="55" t="s">
         <v>124</v>
       </c>
-      <c r="M35" s="70" t="s">
+      <c r="M35" s="54" t="s">
         <v>158</v>
       </c>
     </row>
@@ -4630,13 +4730,13 @@
       <c r="F36" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="H36" s="70" t="s">
+      <c r="H36" s="54" t="s">
         <v>120</v>
       </c>
-      <c r="J36" s="70" t="s">
+      <c r="J36" s="54" t="s">
         <v>125</v>
       </c>
-      <c r="M36" s="70" t="s">
+      <c r="M36" s="54" t="s">
         <v>159</v>
       </c>
     </row>
@@ -4653,16 +4753,16 @@
       <c r="F37" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="H37" s="71" t="s">
+      <c r="H37" s="55" t="s">
         <v>121</v>
       </c>
-      <c r="J37" s="71" t="s">
+      <c r="J37" s="55" t="s">
         <v>126</v>
       </c>
-      <c r="M37" s="71"/>
+      <c r="M37" s="55"/>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B38" s="68" t="s">
+      <c r="B38" s="52" t="s">
         <v>98</v>
       </c>
       <c r="C38" s="21" t="s">
@@ -4674,30 +4774,30 @@
       <c r="F38" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="H38" s="72" t="s">
+      <c r="H38" s="56" t="s">
         <v>122</v>
       </c>
-      <c r="J38" s="73" t="s">
+      <c r="J38" s="57" t="s">
         <v>127</v>
       </c>
-      <c r="M38" s="69" t="s">
+      <c r="M38" s="53" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="39" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
-      <c r="E39" s="66" t="s">
+      <c r="E39" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="F39" s="67" t="s">
+      <c r="F39" s="51" t="s">
         <v>25</v>
       </c>
       <c r="H39" s="4"/>
-      <c r="J39" s="74" t="s">
+      <c r="J39" s="58" t="s">
         <v>128</v>
       </c>
-      <c r="M39" s="70" t="s">
+      <c r="M39" s="54" t="s">
         <v>161</v>
       </c>
     </row>
@@ -4705,10 +4805,10 @@
       <c r="B40" s="29"/>
       <c r="C40" s="29"/>
       <c r="E40" s="29"/>
-      <c r="F40" s="76"/>
+      <c r="F40" s="60"/>
       <c r="H40" s="29"/>
-      <c r="J40" s="77"/>
-      <c r="M40" s="70" t="s">
+      <c r="J40" s="61"/>
+      <c r="M40" s="54" t="s">
         <v>162</v>
       </c>
     </row>
@@ -4716,26 +4816,26 @@
       <c r="M41" s="4"/>
     </row>
     <row r="42" spans="2:13" ht="21" x14ac:dyDescent="0.25">
-      <c r="H42" s="78" t="s">
+      <c r="H42" s="62" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="43" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="2:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="49" t="s">
+      <c r="B44" s="77" t="s">
         <v>72</v>
       </c>
-      <c r="C44" s="50"/>
+      <c r="C44" s="78"/>
       <c r="D44" s="5"/>
-      <c r="E44" s="49" t="s">
+      <c r="E44" s="77" t="s">
         <v>75</v>
       </c>
-      <c r="F44" s="50"/>
-      <c r="H44" s="75" t="s">
+      <c r="F44" s="78"/>
+      <c r="H44" s="59" t="s">
         <v>72</v>
       </c>
       <c r="I44" s="5"/>
-      <c r="J44" s="75" t="s">
+      <c r="J44" s="59" t="s">
         <v>142</v>
       </c>
     </row>
@@ -4752,10 +4852,10 @@
       <c r="F45" s="20">
         <v>8</v>
       </c>
-      <c r="H45" s="69" t="s">
+      <c r="H45" s="53" t="s">
         <v>134</v>
       </c>
-      <c r="J45" s="69" t="s">
+      <c r="J45" s="53" t="s">
         <v>135</v>
       </c>
     </row>
@@ -4772,10 +4872,10 @@
       <c r="F46" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="H46" s="70" t="s">
+      <c r="H46" s="54" t="s">
         <v>129</v>
       </c>
-      <c r="J46" s="70" t="s">
+      <c r="J46" s="54" t="s">
         <v>136</v>
       </c>
     </row>
@@ -4792,10 +4892,10 @@
       <c r="F47" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="H47" s="71" t="s">
+      <c r="H47" s="55" t="s">
         <v>130</v>
       </c>
-      <c r="J47" s="71" t="s">
+      <c r="J47" s="55" t="s">
         <v>137</v>
       </c>
     </row>
@@ -4809,13 +4909,13 @@
       <c r="E48" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F48" s="65" t="s">
+      <c r="F48" s="49" t="s">
         <v>116</v>
       </c>
-      <c r="H48" s="70" t="s">
+      <c r="H48" s="54" t="s">
         <v>131</v>
       </c>
-      <c r="J48" s="70" t="s">
+      <c r="J48" s="54" t="s">
         <v>138</v>
       </c>
     </row>
@@ -4832,15 +4932,15 @@
       <c r="F49" s="23">
         <v>0.75</v>
       </c>
-      <c r="H49" s="71" t="s">
+      <c r="H49" s="55" t="s">
         <v>132</v>
       </c>
-      <c r="J49" s="71" t="s">
+      <c r="J49" s="55" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B50" s="68" t="s">
+      <c r="B50" s="52" t="s">
         <v>98</v>
       </c>
       <c r="C50" s="21" t="s">
@@ -4852,24 +4952,24 @@
       <c r="F50" s="23">
         <v>0.8125</v>
       </c>
-      <c r="H50" s="72" t="s">
+      <c r="H50" s="56" t="s">
         <v>133</v>
       </c>
-      <c r="J50" s="73" t="s">
+      <c r="J50" s="57" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="51" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
-      <c r="E51" s="66" t="s">
+      <c r="E51" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="F51" s="67">
+      <c r="F51" s="51">
         <v>4</v>
       </c>
       <c r="H51" s="4"/>
-      <c r="J51" s="74" t="s">
+      <c r="J51" s="58" t="s">
         <v>141</v>
       </c>
     </row>
@@ -4895,347 +4995,358 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104CFFA4-B0A1-1A4A-AFD7-C18B47CC4B2A}">
-  <dimension ref="B3:J62"/>
+  <dimension ref="B1:J64"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A103" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="L120" sqref="L120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="1" max="1" width="0.6640625" customWidth="1"/>
     <col min="2" max="3" width="20.83203125" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="20.83203125" customWidth="1"/>
     <col min="7" max="7" width="20.83203125" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" customWidth="1"/>
+    <col min="8" max="8" width="0.5" customWidth="1"/>
     <col min="9" max="9" width="7.83203125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:6" ht="5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="89" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="24"/>
+    </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="61" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>34</v>
+      <c r="B3" s="90"/>
+      <c r="D3" s="17" t="s">
+        <v>106</v>
       </c>
       <c r="E3" s="24"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="62"/>
+    <row r="4" spans="2:6" ht="19" x14ac:dyDescent="0.2">
+      <c r="B4" s="48"/>
       <c r="D4" s="17" t="s">
-        <v>106</v>
+        <v>35</v>
       </c>
       <c r="E4" s="24"/>
     </row>
     <row r="5" spans="2:6" ht="19" x14ac:dyDescent="0.2">
       <c r="B5" s="48"/>
       <c r="D5" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E5" s="24"/>
     </row>
-    <row r="6" spans="2:6" ht="19" x14ac:dyDescent="0.2">
-      <c r="B6" s="48"/>
-      <c r="D6" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="24"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="11"/>
-      <c r="D7" s="16" t="s">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="11"/>
+      <c r="D6" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="E7" s="14"/>
+      <c r="E6" s="14"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C9" s="91" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="24"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C10" s="63" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="15" t="s">
+      <c r="C10" s="92"/>
+      <c r="E10" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="24"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E11" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="24"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E12" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="24"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C15" s="91" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="24"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C16" s="92"/>
+      <c r="E16" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="24"/>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C19" s="91" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="24"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C11" s="64"/>
-      <c r="E11" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" s="24"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E12" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="24"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E13" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="24"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C16" s="63" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="F16" s="24"/>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C17" s="64"/>
-      <c r="E17" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" s="24"/>
+      <c r="F19" s="24"/>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C20" s="63" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20" s="15" t="s">
+      <c r="C20" s="92"/>
+      <c r="E20" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="24"/>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E21" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" s="24"/>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E22" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="24"/>
+    </row>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E23" s="29"/>
+      <c r="F23" s="24"/>
+    </row>
+    <row r="25" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C25" s="91" t="s">
+        <v>107</v>
+      </c>
+      <c r="E25" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F20" s="24"/>
-    </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C21" s="64"/>
-      <c r="E21" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="F21" s="24"/>
-    </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E22" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="F22" s="24"/>
-    </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E23" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="F23" s="24"/>
-    </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E24" s="29"/>
-      <c r="F24" s="24"/>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C26" s="63" t="s">
-        <v>107</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>37</v>
+      <c r="C26" s="92"/>
+      <c r="E26" s="17" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C27" s="64"/>
       <c r="E27" s="17" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E28" s="17" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E29" s="16" t="s">
+      <c r="E28" s="16" t="s">
         <v>110</v>
       </c>
     </row>
+    <row r="30" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E30" s="29"/>
+    </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E31" s="29"/>
+      <c r="C31" s="91" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F31" s="24"/>
+      <c r="G31" s="14"/>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C32" s="63" t="s">
-        <v>32</v>
-      </c>
-      <c r="E32" s="15" t="s">
-        <v>47</v>
+      <c r="C32" s="92"/>
+      <c r="E32" s="17" t="s">
+        <v>76</v>
       </c>
       <c r="F32" s="24"/>
       <c r="G32" s="14"/>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C33" s="64"/>
-      <c r="E33" s="17" t="s">
-        <v>76</v>
+    <row r="33" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="E33" s="16" t="s">
+        <v>48</v>
       </c>
       <c r="F33" s="24"/>
       <c r="G33" s="14"/>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E34" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="F34" s="24"/>
-      <c r="G34" s="14"/>
-    </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C37" s="63" t="s">
+    <row r="36" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C36" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="E37" s="12" t="s">
+      <c r="E36" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="G37" s="15" t="s">
+      <c r="G36" s="15" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C38" s="64"/>
-      <c r="G38" s="17" t="s">
+    <row r="37" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C37" s="92"/>
+      <c r="G37" s="17" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C38" s="11"/>
+      <c r="G38" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C39" s="11"/>
-      <c r="G39" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E39" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="G39" s="29"/>
+    </row>
+    <row r="40" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C40" s="11"/>
-      <c r="E40" s="12" t="s">
-        <v>104</v>
-      </c>
       <c r="G40" s="29"/>
     </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C41" s="11"/>
+    <row r="41" spans="3:9" x14ac:dyDescent="0.2">
       <c r="G41" s="29"/>
     </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="E42" s="12" t="s">
+        <v>49</v>
+      </c>
       <c r="G42" s="29"/>
     </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E43" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="G43" s="29"/>
-    </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C46" s="63" t="s">
+    <row r="45" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C45" s="91" t="s">
         <v>31</v>
       </c>
+      <c r="D45" s="18"/>
+      <c r="E45" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G45" s="29"/>
+    </row>
+    <row r="46" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C46" s="92"/>
       <c r="D46" s="18"/>
-      <c r="E46" s="15" t="s">
-        <v>51</v>
+      <c r="E46" s="16" t="s">
+        <v>52</v>
       </c>
       <c r="G46" s="29"/>
     </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C47" s="64"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="16" t="s">
+    <row r="47" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="G47" s="29"/>
+    </row>
+    <row r="48" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="E48" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G48" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="G47" s="29"/>
-    </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="G48" s="29"/>
-    </row>
-    <row r="49" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E49" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="G49" s="15" t="s">
+      <c r="I48" s="13"/>
+    </row>
+    <row r="49" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="G49" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I49" s="13"/>
+    </row>
+    <row r="50" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="G50" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="I50" s="13"/>
+    </row>
+    <row r="51" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="G51" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="I51" s="13"/>
+    </row>
+    <row r="52" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="G52" s="29"/>
+      <c r="I52" s="10"/>
+    </row>
+    <row r="53" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="E53" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G53" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="I49" s="13"/>
-    </row>
-    <row r="50" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="G50" s="17" t="s">
+      <c r="I53" s="13"/>
+    </row>
+    <row r="54" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="G54" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="I50" s="13"/>
-    </row>
-    <row r="51" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="G51" s="17" t="s">
+      <c r="I54" s="13"/>
+    </row>
+    <row r="55" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="G55" s="47" t="s">
         <v>101</v>
       </c>
-      <c r="I51" s="13"/>
-    </row>
-    <row r="52" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="G52" s="46" t="s">
+      <c r="I55" s="13"/>
+    </row>
+    <row r="56" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="G56" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="I52" s="13"/>
-    </row>
-    <row r="53" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="G53" s="29"/>
-      <c r="I53" s="10"/>
-    </row>
-    <row r="54" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E54" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="G54" s="15" t="s">
+      <c r="I56" s="13"/>
+    </row>
+    <row r="57" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="G57" s="29"/>
+      <c r="I57" s="10"/>
+    </row>
+    <row r="58" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="E58" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G58" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="I54" s="13"/>
-    </row>
-    <row r="55" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="G55" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="I55" s="13"/>
-    </row>
-    <row r="56" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="G56" s="47" t="s">
-        <v>101</v>
-      </c>
-      <c r="I56" s="13"/>
-    </row>
-    <row r="57" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="G57" s="46" t="s">
+      <c r="I58" s="13"/>
+      <c r="J58" s="14"/>
+    </row>
+    <row r="59" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="G59" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="I57" s="13"/>
-    </row>
-    <row r="58" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="G58" s="29"/>
-      <c r="I58" s="10"/>
-    </row>
-    <row r="59" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E59" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G59" s="15" t="s">
-        <v>52</v>
-      </c>
       <c r="I59" s="13"/>
-      <c r="J59" s="14"/>
-    </row>
-    <row r="60" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="G60" s="16" t="s">
-        <v>54</v>
-      </c>
+    </row>
+    <row r="60" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="G60" s="29"/>
       <c r="I60" s="13"/>
     </row>
-    <row r="61" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="3:10" x14ac:dyDescent="0.2">
       <c r="G61" s="29"/>
-      <c r="I61" s="13"/>
-    </row>
-    <row r="62" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="G62" s="29"/>
-    </row>
+    </row>
+    <row r="62" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C62" s="91" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="63" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C63" s="92"/>
+    </row>
+    <row r="64" spans="3:10" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="C26:C27"/>
+  <mergeCells count="9">
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="C25:C26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5246,7 +5357,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA7FD533-B3EE-FC43-90B2-49FAE6C07009}">
   <dimension ref="N3:T19"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
@@ -5306,7 +5417,7 @@
       <c r="S7"/>
       <c r="T7"/>
     </row>
-    <row r="8" spans="14:20" s="79" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="14:20" s="63" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="9" spans="14:20" x14ac:dyDescent="0.2">
       <c r="N9"/>
       <c r="O9"/>
@@ -5502,12 +5613,12 @@
       <c r="E7" s="26"/>
       <c r="F7" s="27"/>
       <c r="G7" s="29"/>
-      <c r="H7" s="91" t="s">
+      <c r="H7" s="108" t="s">
         <v>145</v>
       </c>
-      <c r="I7" s="92"/>
-      <c r="J7" s="92"/>
-      <c r="K7" s="93"/>
+      <c r="I7" s="109"/>
+      <c r="J7" s="109"/>
+      <c r="K7" s="110"/>
       <c r="L7" s="30"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
@@ -5517,10 +5628,10 @@
       <c r="E8" s="29"/>
       <c r="F8" s="30"/>
       <c r="G8" s="29"/>
-      <c r="H8" s="94"/>
-      <c r="I8" s="95"/>
-      <c r="J8" s="95"/>
-      <c r="K8" s="96"/>
+      <c r="H8" s="111"/>
+      <c r="I8" s="112"/>
+      <c r="J8" s="112"/>
+      <c r="K8" s="113"/>
       <c r="L8" s="30"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
@@ -5530,10 +5641,10 @@
       <c r="E9" s="32"/>
       <c r="F9" s="33"/>
       <c r="G9" s="29"/>
-      <c r="H9" s="94"/>
-      <c r="I9" s="95"/>
-      <c r="J9" s="95"/>
-      <c r="K9" s="96"/>
+      <c r="H9" s="111"/>
+      <c r="I9" s="112"/>
+      <c r="J9" s="112"/>
+      <c r="K9" s="113"/>
       <c r="L9" s="30"/>
     </row>
     <row r="10" spans="2:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -5543,10 +5654,10 @@
       <c r="E10" s="29"/>
       <c r="F10" s="29"/>
       <c r="G10" s="29"/>
-      <c r="H10" s="94"/>
-      <c r="I10" s="95"/>
-      <c r="J10" s="95"/>
-      <c r="K10" s="96"/>
+      <c r="H10" s="111"/>
+      <c r="I10" s="112"/>
+      <c r="J10" s="112"/>
+      <c r="K10" s="113"/>
       <c r="L10" s="30"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.2">
@@ -5558,10 +5669,10 @@
       <c r="E11" s="26"/>
       <c r="F11" s="27"/>
       <c r="G11" s="29"/>
-      <c r="H11" s="94"/>
-      <c r="I11" s="95"/>
-      <c r="J11" s="95"/>
-      <c r="K11" s="96"/>
+      <c r="H11" s="111"/>
+      <c r="I11" s="112"/>
+      <c r="J11" s="112"/>
+      <c r="K11" s="113"/>
       <c r="L11" s="30"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
@@ -5573,10 +5684,10 @@
       <c r="E12" s="29"/>
       <c r="F12" s="30"/>
       <c r="G12" s="29"/>
-      <c r="H12" s="94"/>
-      <c r="I12" s="95"/>
-      <c r="J12" s="95"/>
-      <c r="K12" s="96"/>
+      <c r="H12" s="111"/>
+      <c r="I12" s="112"/>
+      <c r="J12" s="112"/>
+      <c r="K12" s="113"/>
       <c r="L12" s="30"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.2">
@@ -5588,10 +5699,10 @@
       <c r="E13" s="29"/>
       <c r="F13" s="30"/>
       <c r="G13" s="29"/>
-      <c r="H13" s="94"/>
-      <c r="I13" s="95"/>
-      <c r="J13" s="95"/>
-      <c r="K13" s="96"/>
+      <c r="H13" s="111"/>
+      <c r="I13" s="112"/>
+      <c r="J13" s="112"/>
+      <c r="K13" s="113"/>
       <c r="L13" s="30"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.2">
@@ -5603,10 +5714,10 @@
       <c r="E14" s="32"/>
       <c r="F14" s="33"/>
       <c r="G14" s="29"/>
-      <c r="H14" s="94"/>
-      <c r="I14" s="95"/>
-      <c r="J14" s="95"/>
-      <c r="K14" s="96"/>
+      <c r="H14" s="111"/>
+      <c r="I14" s="112"/>
+      <c r="J14" s="112"/>
+      <c r="K14" s="113"/>
       <c r="L14" s="30"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
@@ -5616,10 +5727,10 @@
       <c r="E15" s="29"/>
       <c r="F15" s="29"/>
       <c r="G15" s="29"/>
-      <c r="H15" s="94"/>
-      <c r="I15" s="95"/>
-      <c r="J15" s="95"/>
-      <c r="K15" s="96"/>
+      <c r="H15" s="111"/>
+      <c r="I15" s="112"/>
+      <c r="J15" s="112"/>
+      <c r="K15" s="113"/>
       <c r="L15" s="30"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.2">
@@ -5631,10 +5742,10 @@
       <c r="E16" s="26"/>
       <c r="F16" s="27"/>
       <c r="G16" s="29"/>
-      <c r="H16" s="94"/>
-      <c r="I16" s="95"/>
-      <c r="J16" s="95"/>
-      <c r="K16" s="96"/>
+      <c r="H16" s="111"/>
+      <c r="I16" s="112"/>
+      <c r="J16" s="112"/>
+      <c r="K16" s="113"/>
       <c r="L16" s="30"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.2">
@@ -5646,10 +5757,10 @@
       <c r="E17" s="29"/>
       <c r="F17" s="30"/>
       <c r="G17" s="29"/>
-      <c r="H17" s="94"/>
-      <c r="I17" s="95"/>
-      <c r="J17" s="95"/>
-      <c r="K17" s="96"/>
+      <c r="H17" s="111"/>
+      <c r="I17" s="112"/>
+      <c r="J17" s="112"/>
+      <c r="K17" s="113"/>
       <c r="L17" s="30"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.2">
@@ -5661,10 +5772,10 @@
       <c r="E18" s="29"/>
       <c r="F18" s="30"/>
       <c r="G18" s="29"/>
-      <c r="H18" s="94"/>
-      <c r="I18" s="95"/>
-      <c r="J18" s="95"/>
-      <c r="K18" s="96"/>
+      <c r="H18" s="111"/>
+      <c r="I18" s="112"/>
+      <c r="J18" s="112"/>
+      <c r="K18" s="113"/>
       <c r="L18" s="30"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.2">
@@ -5674,10 +5785,10 @@
       <c r="E19" s="29"/>
       <c r="F19" s="30"/>
       <c r="G19" s="29"/>
-      <c r="H19" s="94"/>
-      <c r="I19" s="95"/>
-      <c r="J19" s="95"/>
-      <c r="K19" s="96"/>
+      <c r="H19" s="111"/>
+      <c r="I19" s="112"/>
+      <c r="J19" s="112"/>
+      <c r="K19" s="113"/>
       <c r="L19" s="30"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
@@ -5687,10 +5798,10 @@
       <c r="E20" s="32"/>
       <c r="F20" s="33"/>
       <c r="G20" s="29"/>
-      <c r="H20" s="97"/>
-      <c r="I20" s="98"/>
-      <c r="J20" s="98"/>
-      <c r="K20" s="99"/>
+      <c r="H20" s="114"/>
+      <c r="I20" s="115"/>
+      <c r="J20" s="115"/>
+      <c r="K20" s="116"/>
       <c r="L20" s="30"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.2">
@@ -5857,34 +5968,34 @@
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B36" s="28"/>
-      <c r="C36" s="104" t="s">
+      <c r="C36" s="93" t="s">
         <v>148</v>
       </c>
-      <c r="D36" s="105"/>
-      <c r="E36" s="106"/>
-      <c r="F36" s="63" t="s">
+      <c r="D36" s="94"/>
+      <c r="E36" s="95"/>
+      <c r="F36" s="91" t="s">
         <v>149</v>
       </c>
       <c r="G36" s="29"/>
-      <c r="H36" s="82" t="s">
+      <c r="H36" s="99" t="s">
         <v>155</v>
       </c>
-      <c r="I36" s="83"/>
-      <c r="J36" s="83"/>
-      <c r="K36" s="84"/>
+      <c r="I36" s="100"/>
+      <c r="J36" s="100"/>
+      <c r="K36" s="101"/>
       <c r="L36" s="30"/>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B37" s="28"/>
-      <c r="C37" s="107"/>
-      <c r="D37" s="108"/>
-      <c r="E37" s="109"/>
-      <c r="F37" s="64"/>
+      <c r="C37" s="96"/>
+      <c r="D37" s="97"/>
+      <c r="E37" s="98"/>
+      <c r="F37" s="92"/>
       <c r="G37" s="29"/>
-      <c r="H37" s="85"/>
-      <c r="I37" s="86"/>
-      <c r="J37" s="86"/>
-      <c r="K37" s="87"/>
+      <c r="H37" s="102"/>
+      <c r="I37" s="103"/>
+      <c r="J37" s="103"/>
+      <c r="K37" s="104"/>
       <c r="L37" s="30"/>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.2">
@@ -5896,23 +6007,23 @@
       <c r="E38" s="118"/>
       <c r="F38" s="119"/>
       <c r="G38" s="29"/>
-      <c r="H38" s="88"/>
-      <c r="I38" s="89"/>
-      <c r="J38" s="89"/>
-      <c r="K38" s="90"/>
+      <c r="H38" s="105"/>
+      <c r="I38" s="106"/>
+      <c r="J38" s="106"/>
+      <c r="K38" s="107"/>
       <c r="L38" s="30"/>
     </row>
     <row r="39" spans="2:12" ht="19" x14ac:dyDescent="0.2">
       <c r="B39" s="28"/>
-      <c r="C39" s="100"/>
-      <c r="D39" s="100"/>
-      <c r="E39" s="100"/>
-      <c r="F39" s="100"/>
+      <c r="C39" s="64"/>
+      <c r="D39" s="64"/>
+      <c r="E39" s="64"/>
+      <c r="F39" s="64"/>
       <c r="G39" s="29"/>
-      <c r="H39" s="120"/>
-      <c r="I39" s="120"/>
-      <c r="J39" s="120"/>
-      <c r="K39" s="120"/>
+      <c r="H39" s="68"/>
+      <c r="I39" s="68"/>
+      <c r="J39" s="68"/>
+      <c r="K39" s="68"/>
       <c r="L39" s="30"/>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.2">
@@ -5922,291 +6033,291 @@
       <c r="E40" s="29"/>
       <c r="F40" s="29"/>
       <c r="G40" s="29"/>
-      <c r="H40" s="102"/>
-      <c r="I40" s="102"/>
-      <c r="J40" s="102"/>
-      <c r="K40" s="102"/>
-      <c r="L40" s="103"/>
+      <c r="H40" s="66"/>
+      <c r="I40" s="66"/>
+      <c r="J40" s="66"/>
+      <c r="K40" s="66"/>
+      <c r="L40" s="67"/>
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B41" s="28"/>
-      <c r="C41" s="110" t="s">
+      <c r="C41" s="120" t="s">
         <v>150</v>
       </c>
-      <c r="D41" s="111"/>
-      <c r="E41" s="111"/>
-      <c r="F41" s="111"/>
-      <c r="G41" s="111"/>
-      <c r="H41" s="111"/>
-      <c r="I41" s="111"/>
-      <c r="J41" s="111"/>
-      <c r="K41" s="112"/>
-      <c r="L41" s="103"/>
+      <c r="D41" s="121"/>
+      <c r="E41" s="121"/>
+      <c r="F41" s="121"/>
+      <c r="G41" s="121"/>
+      <c r="H41" s="121"/>
+      <c r="I41" s="121"/>
+      <c r="J41" s="121"/>
+      <c r="K41" s="122"/>
+      <c r="L41" s="67"/>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B42" s="28"/>
-      <c r="C42" s="80"/>
-      <c r="D42" s="81"/>
-      <c r="E42" s="81"/>
-      <c r="F42" s="81"/>
-      <c r="G42" s="81"/>
-      <c r="H42" s="81"/>
-      <c r="I42" s="81"/>
-      <c r="J42" s="81"/>
-      <c r="K42" s="113"/>
-      <c r="L42" s="103"/>
+      <c r="C42" s="123"/>
+      <c r="D42" s="124"/>
+      <c r="E42" s="124"/>
+      <c r="F42" s="124"/>
+      <c r="G42" s="124"/>
+      <c r="H42" s="124"/>
+      <c r="I42" s="124"/>
+      <c r="J42" s="124"/>
+      <c r="K42" s="125"/>
+      <c r="L42" s="67"/>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B43" s="28"/>
-      <c r="C43" s="80"/>
-      <c r="D43" s="81"/>
-      <c r="E43" s="81"/>
-      <c r="F43" s="81"/>
-      <c r="G43" s="81"/>
-      <c r="H43" s="81"/>
-      <c r="I43" s="81"/>
-      <c r="J43" s="81"/>
-      <c r="K43" s="113"/>
-      <c r="L43" s="103"/>
+      <c r="C43" s="123"/>
+      <c r="D43" s="124"/>
+      <c r="E43" s="124"/>
+      <c r="F43" s="124"/>
+      <c r="G43" s="124"/>
+      <c r="H43" s="124"/>
+      <c r="I43" s="124"/>
+      <c r="J43" s="124"/>
+      <c r="K43" s="125"/>
+      <c r="L43" s="67"/>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B44" s="28"/>
-      <c r="C44" s="80"/>
-      <c r="D44" s="81"/>
-      <c r="E44" s="81"/>
-      <c r="F44" s="81"/>
-      <c r="G44" s="81"/>
-      <c r="H44" s="81"/>
-      <c r="I44" s="81"/>
-      <c r="J44" s="81"/>
-      <c r="K44" s="113"/>
-      <c r="L44" s="103"/>
+      <c r="C44" s="123"/>
+      <c r="D44" s="124"/>
+      <c r="E44" s="124"/>
+      <c r="F44" s="124"/>
+      <c r="G44" s="124"/>
+      <c r="H44" s="124"/>
+      <c r="I44" s="124"/>
+      <c r="J44" s="124"/>
+      <c r="K44" s="125"/>
+      <c r="L44" s="67"/>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B45" s="28"/>
-      <c r="C45" s="80"/>
-      <c r="D45" s="81"/>
-      <c r="E45" s="81"/>
-      <c r="F45" s="81"/>
-      <c r="G45" s="81"/>
-      <c r="H45" s="81"/>
-      <c r="I45" s="81"/>
-      <c r="J45" s="81"/>
-      <c r="K45" s="113"/>
-      <c r="L45" s="103"/>
+      <c r="C45" s="123"/>
+      <c r="D45" s="124"/>
+      <c r="E45" s="124"/>
+      <c r="F45" s="124"/>
+      <c r="G45" s="124"/>
+      <c r="H45" s="124"/>
+      <c r="I45" s="124"/>
+      <c r="J45" s="124"/>
+      <c r="K45" s="125"/>
+      <c r="L45" s="67"/>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B46" s="28"/>
-      <c r="C46" s="114"/>
-      <c r="D46" s="115"/>
-      <c r="E46" s="115"/>
-      <c r="F46" s="115"/>
-      <c r="G46" s="115"/>
-      <c r="H46" s="115"/>
-      <c r="I46" s="115"/>
-      <c r="J46" s="115"/>
-      <c r="K46" s="116"/>
-      <c r="L46" s="103"/>
+      <c r="C46" s="126"/>
+      <c r="D46" s="127"/>
+      <c r="E46" s="127"/>
+      <c r="F46" s="127"/>
+      <c r="G46" s="127"/>
+      <c r="H46" s="127"/>
+      <c r="I46" s="127"/>
+      <c r="J46" s="127"/>
+      <c r="K46" s="128"/>
+      <c r="L46" s="67"/>
     </row>
     <row r="47" spans="2:12" ht="21" x14ac:dyDescent="0.2">
       <c r="B47" s="28"/>
-      <c r="C47" s="121"/>
-      <c r="D47" s="121"/>
-      <c r="E47" s="121"/>
-      <c r="F47" s="121"/>
-      <c r="G47" s="121"/>
-      <c r="H47" s="121"/>
-      <c r="I47" s="121"/>
-      <c r="J47" s="121"/>
-      <c r="K47" s="121"/>
-      <c r="L47" s="103"/>
+      <c r="C47" s="69"/>
+      <c r="D47" s="69"/>
+      <c r="E47" s="69"/>
+      <c r="F47" s="69"/>
+      <c r="G47" s="69"/>
+      <c r="H47" s="69"/>
+      <c r="I47" s="69"/>
+      <c r="J47" s="69"/>
+      <c r="K47" s="69"/>
+      <c r="L47" s="67"/>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B48" s="28"/>
-      <c r="C48" s="101"/>
+      <c r="C48" s="65"/>
       <c r="D48" s="29"/>
       <c r="E48" s="29"/>
       <c r="F48" s="29"/>
       <c r="G48" s="29"/>
-      <c r="H48" s="102"/>
-      <c r="I48" s="102"/>
-      <c r="J48" s="102"/>
-      <c r="K48" s="102"/>
-      <c r="L48" s="103"/>
+      <c r="H48" s="66"/>
+      <c r="I48" s="66"/>
+      <c r="J48" s="66"/>
+      <c r="K48" s="66"/>
+      <c r="L48" s="67"/>
     </row>
     <row r="49" spans="2:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="28"/>
-      <c r="C49" s="104" t="s">
+      <c r="C49" s="93" t="s">
         <v>152</v>
       </c>
-      <c r="D49" s="105"/>
-      <c r="E49" s="105"/>
-      <c r="F49" s="106"/>
+      <c r="D49" s="94"/>
+      <c r="E49" s="94"/>
+      <c r="F49" s="95"/>
       <c r="G49" s="29"/>
-      <c r="H49" s="91" t="s">
+      <c r="H49" s="108" t="s">
         <v>154</v>
       </c>
-      <c r="I49" s="92"/>
-      <c r="J49" s="92"/>
-      <c r="K49" s="93"/>
-      <c r="L49" s="103"/>
+      <c r="I49" s="109"/>
+      <c r="J49" s="109"/>
+      <c r="K49" s="110"/>
+      <c r="L49" s="67"/>
     </row>
     <row r="50" spans="2:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="28"/>
-      <c r="C50" s="107"/>
-      <c r="D50" s="108"/>
-      <c r="E50" s="108"/>
-      <c r="F50" s="109"/>
+      <c r="C50" s="96"/>
+      <c r="D50" s="97"/>
+      <c r="E50" s="97"/>
+      <c r="F50" s="98"/>
       <c r="G50" s="29"/>
-      <c r="H50" s="94"/>
-      <c r="I50" s="95"/>
-      <c r="J50" s="95"/>
-      <c r="K50" s="96"/>
-      <c r="L50" s="103"/>
+      <c r="H50" s="111"/>
+      <c r="I50" s="112"/>
+      <c r="J50" s="112"/>
+      <c r="K50" s="113"/>
+      <c r="L50" s="67"/>
     </row>
     <row r="51" spans="2:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="28"/>
-      <c r="C51" s="101"/>
+      <c r="C51" s="65"/>
       <c r="D51" s="29"/>
       <c r="E51" s="29"/>
       <c r="F51" s="29"/>
       <c r="G51" s="29"/>
-      <c r="H51" s="94"/>
-      <c r="I51" s="95"/>
-      <c r="J51" s="95"/>
-      <c r="K51" s="96"/>
-      <c r="L51" s="103"/>
+      <c r="H51" s="111"/>
+      <c r="I51" s="112"/>
+      <c r="J51" s="112"/>
+      <c r="K51" s="113"/>
+      <c r="L51" s="67"/>
     </row>
     <row r="52" spans="2:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" s="28"/>
-      <c r="C52" s="101"/>
+      <c r="C52" s="65"/>
       <c r="D52" s="29"/>
       <c r="E52" s="29"/>
       <c r="F52" s="29"/>
       <c r="G52" s="29"/>
-      <c r="H52" s="94"/>
-      <c r="I52" s="95"/>
-      <c r="J52" s="95"/>
-      <c r="K52" s="96"/>
-      <c r="L52" s="103"/>
+      <c r="H52" s="111"/>
+      <c r="I52" s="112"/>
+      <c r="J52" s="112"/>
+      <c r="K52" s="113"/>
+      <c r="L52" s="67"/>
     </row>
     <row r="53" spans="2:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B53" s="28"/>
-      <c r="C53" s="82" t="s">
+      <c r="C53" s="99" t="s">
         <v>153</v>
       </c>
-      <c r="D53" s="83"/>
-      <c r="E53" s="83"/>
-      <c r="F53" s="84"/>
+      <c r="D53" s="100"/>
+      <c r="E53" s="100"/>
+      <c r="F53" s="101"/>
       <c r="G53" s="29"/>
-      <c r="H53" s="94"/>
-      <c r="I53" s="95"/>
-      <c r="J53" s="95"/>
-      <c r="K53" s="96"/>
-      <c r="L53" s="103"/>
+      <c r="H53" s="111"/>
+      <c r="I53" s="112"/>
+      <c r="J53" s="112"/>
+      <c r="K53" s="113"/>
+      <c r="L53" s="67"/>
     </row>
     <row r="54" spans="2:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B54" s="28"/>
-      <c r="C54" s="85"/>
-      <c r="D54" s="86"/>
-      <c r="E54" s="86"/>
-      <c r="F54" s="87"/>
+      <c r="C54" s="102"/>
+      <c r="D54" s="103"/>
+      <c r="E54" s="103"/>
+      <c r="F54" s="104"/>
       <c r="G54" s="29"/>
-      <c r="H54" s="94"/>
-      <c r="I54" s="95"/>
-      <c r="J54" s="95"/>
-      <c r="K54" s="96"/>
-      <c r="L54" s="103"/>
+      <c r="H54" s="111"/>
+      <c r="I54" s="112"/>
+      <c r="J54" s="112"/>
+      <c r="K54" s="113"/>
+      <c r="L54" s="67"/>
     </row>
     <row r="55" spans="2:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="28"/>
-      <c r="C55" s="85"/>
-      <c r="D55" s="86"/>
-      <c r="E55" s="86"/>
-      <c r="F55" s="87"/>
+      <c r="C55" s="102"/>
+      <c r="D55" s="103"/>
+      <c r="E55" s="103"/>
+      <c r="F55" s="104"/>
       <c r="G55" s="29"/>
-      <c r="H55" s="94"/>
-      <c r="I55" s="95"/>
-      <c r="J55" s="95"/>
-      <c r="K55" s="96"/>
-      <c r="L55" s="103"/>
+      <c r="H55" s="111"/>
+      <c r="I55" s="112"/>
+      <c r="J55" s="112"/>
+      <c r="K55" s="113"/>
+      <c r="L55" s="67"/>
     </row>
     <row r="56" spans="2:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B56" s="28"/>
-      <c r="C56" s="85"/>
-      <c r="D56" s="86"/>
-      <c r="E56" s="86"/>
-      <c r="F56" s="87"/>
+      <c r="C56" s="102"/>
+      <c r="D56" s="103"/>
+      <c r="E56" s="103"/>
+      <c r="F56" s="104"/>
       <c r="G56" s="29"/>
-      <c r="H56" s="94"/>
-      <c r="I56" s="95"/>
-      <c r="J56" s="95"/>
-      <c r="K56" s="96"/>
-      <c r="L56" s="103"/>
+      <c r="H56" s="111"/>
+      <c r="I56" s="112"/>
+      <c r="J56" s="112"/>
+      <c r="K56" s="113"/>
+      <c r="L56" s="67"/>
     </row>
     <row r="57" spans="2:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="28"/>
-      <c r="C57" s="85"/>
-      <c r="D57" s="86"/>
-      <c r="E57" s="86"/>
-      <c r="F57" s="87"/>
+      <c r="C57" s="102"/>
+      <c r="D57" s="103"/>
+      <c r="E57" s="103"/>
+      <c r="F57" s="104"/>
       <c r="G57" s="29"/>
-      <c r="H57" s="94"/>
-      <c r="I57" s="95"/>
-      <c r="J57" s="95"/>
-      <c r="K57" s="96"/>
-      <c r="L57" s="103"/>
+      <c r="H57" s="111"/>
+      <c r="I57" s="112"/>
+      <c r="J57" s="112"/>
+      <c r="K57" s="113"/>
+      <c r="L57" s="67"/>
     </row>
     <row r="58" spans="2:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="28"/>
-      <c r="C58" s="85"/>
-      <c r="D58" s="86"/>
-      <c r="E58" s="86"/>
-      <c r="F58" s="87"/>
+      <c r="C58" s="102"/>
+      <c r="D58" s="103"/>
+      <c r="E58" s="103"/>
+      <c r="F58" s="104"/>
       <c r="G58" s="29"/>
-      <c r="H58" s="94"/>
-      <c r="I58" s="95"/>
-      <c r="J58" s="95"/>
-      <c r="K58" s="96"/>
+      <c r="H58" s="111"/>
+      <c r="I58" s="112"/>
+      <c r="J58" s="112"/>
+      <c r="K58" s="113"/>
       <c r="L58" s="30"/>
     </row>
     <row r="59" spans="2:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="28"/>
-      <c r="C59" s="85"/>
-      <c r="D59" s="86"/>
-      <c r="E59" s="86"/>
-      <c r="F59" s="87"/>
+      <c r="C59" s="102"/>
+      <c r="D59" s="103"/>
+      <c r="E59" s="103"/>
+      <c r="F59" s="104"/>
       <c r="G59" s="29"/>
-      <c r="H59" s="94"/>
-      <c r="I59" s="95"/>
-      <c r="J59" s="95"/>
-      <c r="K59" s="96"/>
+      <c r="H59" s="111"/>
+      <c r="I59" s="112"/>
+      <c r="J59" s="112"/>
+      <c r="K59" s="113"/>
       <c r="L59" s="30"/>
     </row>
     <row r="60" spans="2:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B60" s="28"/>
-      <c r="C60" s="85"/>
-      <c r="D60" s="86"/>
-      <c r="E60" s="86"/>
-      <c r="F60" s="87"/>
+      <c r="C60" s="102"/>
+      <c r="D60" s="103"/>
+      <c r="E60" s="103"/>
+      <c r="F60" s="104"/>
       <c r="G60" s="29"/>
-      <c r="H60" s="94"/>
-      <c r="I60" s="95"/>
-      <c r="J60" s="95"/>
-      <c r="K60" s="96"/>
+      <c r="H60" s="111"/>
+      <c r="I60" s="112"/>
+      <c r="J60" s="112"/>
+      <c r="K60" s="113"/>
       <c r="L60" s="30"/>
     </row>
     <row r="61" spans="2:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B61" s="28"/>
-      <c r="C61" s="88"/>
-      <c r="D61" s="89"/>
-      <c r="E61" s="89"/>
-      <c r="F61" s="90"/>
+      <c r="C61" s="105"/>
+      <c r="D61" s="106"/>
+      <c r="E61" s="106"/>
+      <c r="F61" s="107"/>
       <c r="G61" s="29"/>
-      <c r="H61" s="97"/>
-      <c r="I61" s="98"/>
-      <c r="J61" s="98"/>
-      <c r="K61" s="99"/>
+      <c r="H61" s="114"/>
+      <c r="I61" s="115"/>
+      <c r="J61" s="115"/>
+      <c r="K61" s="116"/>
       <c r="L61" s="30"/>
     </row>
     <row r="62" spans="2:12" x14ac:dyDescent="0.2">
@@ -6250,15 +6361,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="H7:K20"/>
+    <mergeCell ref="C36:E37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="C41:K46"/>
     <mergeCell ref="C49:F50"/>
     <mergeCell ref="C53:F61"/>
     <mergeCell ref="H49:K61"/>
     <mergeCell ref="C38:F38"/>
     <mergeCell ref="H36:K38"/>
-    <mergeCell ref="H7:K20"/>
-    <mergeCell ref="C36:E37"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="C41:K46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6366,68 +6477,68 @@
   </cols>
   <sheetData>
     <row r="34" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="2:4" s="122" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="128" t="s">
+    <row r="35" spans="2:4" s="70" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="76" t="s">
         <v>170</v>
       </c>
-      <c r="C35" s="128" t="s">
+      <c r="C35" s="76" t="s">
         <v>164</v>
       </c>
-      <c r="D35" s="128" t="s">
+      <c r="D35" s="76" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="85" x14ac:dyDescent="0.2">
-      <c r="B36" s="127" t="s">
+      <c r="B36" s="75" t="s">
         <v>166</v>
       </c>
-      <c r="C36" s="127" t="s">
+      <c r="C36" s="75" t="s">
         <v>175</v>
       </c>
-      <c r="D36" s="127" t="s">
+      <c r="D36" s="75" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="B37" s="125" t="s">
+      <c r="B37" s="73" t="s">
         <v>167</v>
       </c>
-      <c r="C37" s="125" t="s">
+      <c r="C37" s="73" t="s">
         <v>173</v>
       </c>
-      <c r="D37" s="125" t="s">
+      <c r="D37" s="73" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="B38" s="124" t="s">
+      <c r="B38" s="72" t="s">
         <v>177</v>
       </c>
-      <c r="C38" s="124"/>
-      <c r="D38" s="124"/>
+      <c r="C38" s="72"/>
+      <c r="D38" s="72"/>
     </row>
     <row r="39" spans="2:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B39" s="125" t="s">
+      <c r="B39" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="C39" s="125"/>
-      <c r="D39" s="125"/>
+      <c r="C39" s="73"/>
+      <c r="D39" s="73"/>
     </row>
     <row r="40" spans="2:4" ht="86" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="126" t="s">
+      <c r="B40" s="74" t="s">
         <v>169</v>
       </c>
-      <c r="C40" s="126" t="s">
+      <c r="C40" s="74" t="s">
         <v>172</v>
       </c>
-      <c r="D40" s="126" t="s">
+      <c r="D40" s="74" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B41" s="123"/>
-      <c r="C41" s="123"/>
-      <c r="D41" s="123"/>
+      <c r="B41" s="71"/>
+      <c r="C41" s="71"/>
+      <c r="D41" s="71"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added more to readme
</commit_message>
<xml_diff>
--- a/Project Planning/Project Drawings.xlsx
+++ b/Project Planning/Project Drawings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colinmorrison/codeclan_work/Resistance_Temple/Project Planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E609A76-193A-8F4A-8046-020C68FEAA83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A510ED52-0792-F047-9054-BA4ED82C7560}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1900" yWindow="-20500" windowWidth="33000" windowHeight="20500" activeTab="3" xr2:uid="{056C3CC7-3EA0-BF47-B5DA-A9694FF9AEB8}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23620" windowHeight="20500" activeTab="1" xr2:uid="{056C3CC7-3EA0-BF47-B5DA-A9694FF9AEB8}"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="197">
   <si>
     <t>1) We have a Gym - Resistance Temple</t>
   </si>
@@ -561,11 +561,6 @@
   </si>
   <si>
     <t>Logic within HTML slowing page load, and lowering performance</t>
-  </si>
-  <si>
-    <t>*Implement daily milestones to track progress
-*Utilize TDD - Do not leave testing till end
-*Start on minimal functionality logic and styling, then additional functionality after</t>
   </si>
   <si>
     <t>1) Software package issues
@@ -580,13 +575,74 @@
   </si>
   <si>
     <t>Additional Information</t>
+  </si>
+  <si>
+    <t>Data not being stored after submission, or after local server host closes</t>
+  </si>
+  <si>
+    <t>Use a PSQL database to store added data</t>
+  </si>
+  <si>
+    <t>*Implement daily milestones to track progress
+*Utilize TDD to test as we progress
+*Finish the needed functionality and styling, before starting on the additional wants</t>
+  </si>
+  <si>
+    <t>Use stock fonts, icons, and background images</t>
+  </si>
+  <si>
+    <t>No budget for photography or additional styling</t>
+  </si>
+  <si>
+    <t>Usability</t>
+  </si>
+  <si>
+    <t>1) Accidental pressing of delete buttons
+2) Popular links requiring multiple steps to get to</t>
+  </si>
+  <si>
+    <t>1) Move delete button to side of page, highlight in red, and highlight when hovered upon as additional warning
+2) Quick access links for favourites</t>
+  </si>
+  <si>
+    <t>forename: string</t>
+  </si>
+  <si>
+    <t>surname: string</t>
+  </si>
+  <si>
+    <t>id: int</t>
+  </si>
+  <si>
+    <t>name: string</t>
+  </si>
+  <si>
+    <t>type: string</t>
+  </si>
+  <si>
+    <t>capacity: int</t>
+  </si>
+  <si>
+    <t>upgrade_membership()</t>
+  </si>
+  <si>
+    <t>book_session(session)</t>
+  </si>
+  <si>
+    <t>membership_status: boolean</t>
+  </si>
+  <si>
+    <t>membership_type: string</t>
+  </si>
+  <si>
+    <t>check_if_full()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -676,8 +732,34 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -696,8 +778,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="38">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -1166,11 +1254,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1301,15 +1404,38 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1346,17 +1472,80 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1375,69 +1564,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1875,6 +2001,57 @@
         <a:xfrm>
           <a:off x="8040077" y="2063261"/>
           <a:ext cx="795867" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9769</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1572846</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>9769</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65E2E24F-6A8C-A549-8A1A-D03666B8FE25}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2432538" y="6359770"/>
+          <a:ext cx="1563077" cy="9768"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3773,6 +3950,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>582083</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>184150</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>139699</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E01FC50-75D9-3645-A210-FCDE3A3C6348}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10488083" y="1195916"/>
+          <a:ext cx="7137400" cy="8394700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4157,18 +4378,18 @@
     </row>
     <row r="9" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="2:9" s="5" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="77" t="s">
+      <c r="B10" s="92" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="78"/>
-      <c r="E10" s="77" t="s">
+      <c r="C10" s="93"/>
+      <c r="E10" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="78"/>
-      <c r="H10" s="77" t="s">
+      <c r="F10" s="93"/>
+      <c r="H10" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="78"/>
+      <c r="I10" s="93"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
@@ -4328,70 +4549,73 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C703BECF-5A51-894E-B8EF-AE4D25329CF7}">
-  <dimension ref="B2:J26"/>
+  <dimension ref="B2:J56"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="35.83203125" style="81" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="35.83203125" style="81" customWidth="1"/>
     <col min="5" max="6" width="20.83203125" customWidth="1"/>
     <col min="8" max="9" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="90" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+      <c r="B3" s="81" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
+      <c r="B4" s="81" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+      <c r="B5" s="81" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="2:9" s="5" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="77" t="s">
+      <c r="B10" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="78"/>
-      <c r="E10" s="77" t="s">
+      <c r="C10" s="93"/>
+      <c r="D10" s="82"/>
+      <c r="E10" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="78"/>
-      <c r="H10" s="77" t="s">
+      <c r="F10" s="93"/>
+      <c r="H10" s="92" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="78"/>
+      <c r="I10" s="93"/>
     </row>
     <row r="11" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="79" t="s">
+      <c r="B11" s="94" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="80"/>
-      <c r="E11" s="79" t="s">
+      <c r="C11" s="95"/>
+      <c r="E11" s="94" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="80"/>
-      <c r="H11" s="79" t="s">
+      <c r="F11" s="95"/>
+      <c r="H11" s="94" t="s">
         <v>58</v>
       </c>
-      <c r="I11" s="80"/>
+      <c r="I11" s="95"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="84" t="s">
         <v>2</v>
       </c>
       <c r="C12" s="20" t="s">
@@ -4411,7 +4635,7 @@
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="85" t="s">
         <v>93</v>
       </c>
       <c r="C13" s="21" t="s">
@@ -4431,7 +4655,7 @@
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="86" t="s">
         <v>94</v>
       </c>
       <c r="C14" s="20" t="s">
@@ -4451,7 +4675,7 @@
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="85" t="s">
         <v>95</v>
       </c>
       <c r="C15" s="21" t="s">
@@ -4467,7 +4691,7 @@
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="86" t="s">
         <v>97</v>
       </c>
       <c r="C16" s="20" t="s">
@@ -4483,7 +4707,7 @@
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="89" t="s">
         <v>98</v>
       </c>
       <c r="C17" s="21" t="s">
@@ -4500,7 +4724,7 @@
       <c r="J17" s="9"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B18" s="6"/>
+      <c r="B18" s="85"/>
       <c r="C18" s="19"/>
       <c r="E18" s="8"/>
       <c r="F18" s="19"/>
@@ -4512,7 +4736,7 @@
       </c>
     </row>
     <row r="19" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="6"/>
+      <c r="B19" s="85"/>
       <c r="C19" s="21"/>
       <c r="E19" s="6"/>
       <c r="F19" s="21"/>
@@ -4520,60 +4744,205 @@
       <c r="I19" s="21"/>
     </row>
     <row r="20" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="79" t="s">
+      <c r="B20" s="94" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="80"/>
-      <c r="E20" s="79" t="s">
+      <c r="C20" s="95"/>
+      <c r="E20" s="94" t="s">
         <v>59</v>
       </c>
-      <c r="F20" s="80"/>
-      <c r="H20" s="79" t="s">
+      <c r="F20" s="95"/>
+      <c r="H20" s="94" t="s">
         <v>59</v>
       </c>
-      <c r="I20" s="80"/>
+      <c r="I20" s="95"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B21" s="85"/>
-      <c r="C21" s="86"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="85"/>
-      <c r="F21" s="86"/>
+      <c r="B21" s="100"/>
+      <c r="C21" s="101"/>
+      <c r="E21" s="100"/>
+      <c r="F21" s="101"/>
       <c r="G21" s="14"/>
-      <c r="H21" s="85"/>
-      <c r="I21" s="86"/>
+      <c r="H21" s="100"/>
+      <c r="I21" s="101"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B22" s="87"/>
-      <c r="C22" s="88"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="87"/>
-      <c r="F22" s="88"/>
+      <c r="B22" s="102"/>
+      <c r="C22" s="103"/>
+      <c r="E22" s="102"/>
+      <c r="F22" s="103"/>
       <c r="G22" s="14"/>
-      <c r="H22" s="87"/>
-      <c r="I22" s="88"/>
+      <c r="H22" s="102"/>
+      <c r="I22" s="103"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B23" s="81"/>
-      <c r="C23" s="82"/>
-      <c r="E23" s="81"/>
-      <c r="F23" s="82"/>
-      <c r="H23" s="81"/>
-      <c r="I23" s="82"/>
+      <c r="B23" s="96"/>
+      <c r="C23" s="97"/>
+      <c r="E23" s="96"/>
+      <c r="F23" s="97"/>
+      <c r="H23" s="96"/>
+      <c r="I23" s="97"/>
     </row>
     <row r="24" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="83"/>
-      <c r="C24" s="84"/>
-      <c r="E24" s="83"/>
-      <c r="F24" s="84"/>
-      <c r="H24" s="83"/>
-      <c r="I24" s="84"/>
+      <c r="B24" s="98"/>
+      <c r="C24" s="99"/>
+      <c r="E24" s="98"/>
+      <c r="F24" s="99"/>
+      <c r="H24" s="98"/>
+      <c r="I24" s="99"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B25" s="14"/>
+      <c r="B25" s="91"/>
+      <c r="C25" s="78"/>
+      <c r="E25" s="78"/>
+      <c r="F25" s="78"/>
+      <c r="H25" s="78"/>
+      <c r="I25" s="78"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B26" s="14"/>
+      <c r="B26" s="91"/>
+      <c r="C26" s="78"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="78"/>
+      <c r="H26" s="78"/>
+      <c r="I26" s="78"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B27" s="91"/>
+      <c r="C27" s="78"/>
+      <c r="E27" s="78"/>
+      <c r="F27" s="78"/>
+      <c r="H27" s="78"/>
+      <c r="I27" s="78"/>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B28" s="91"/>
+      <c r="C28" s="78"/>
+      <c r="E28" s="78"/>
+      <c r="F28" s="78"/>
+      <c r="H28" s="78"/>
+      <c r="I28" s="78"/>
+    </row>
+    <row r="29" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:10" s="5" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="83" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="83" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B31" s="84" t="s">
+        <v>188</v>
+      </c>
+      <c r="D31" s="84" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B32" s="85" t="s">
+        <v>186</v>
+      </c>
+      <c r="D32" s="85" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B33" s="86" t="s">
+        <v>187</v>
+      </c>
+      <c r="D33" s="86" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B34" s="85" t="s">
+        <v>194</v>
+      </c>
+      <c r="D34" s="85" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B35" s="86" t="s">
+        <v>195</v>
+      </c>
+      <c r="D35" s="86"/>
+    </row>
+    <row r="36" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="85"/>
+      <c r="D36" s="85"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B37" s="79" t="s">
+        <v>193</v>
+      </c>
+      <c r="C37" s="14"/>
+      <c r="D37" s="79" t="s">
+        <v>196</v>
+      </c>
+      <c r="E37" s="14"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B38" s="80" t="s">
+        <v>192</v>
+      </c>
+      <c r="C38" s="14"/>
+      <c r="D38" s="80"/>
+      <c r="E38" s="14"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B39" s="80" t="s">
+        <v>162</v>
+      </c>
+      <c r="D39" s="80"/>
+    </row>
+    <row r="40" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="87"/>
+      <c r="D40" s="87"/>
+    </row>
+    <row r="45" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D46" s="83" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D47" s="86" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D48" s="85" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D49" s="85" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D50" s="88"/>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D51" s="89"/>
+    </row>
+    <row r="52" spans="4:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D52" s="85"/>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D53" s="79"/>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D54" s="80"/>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D55" s="80"/>
+    </row>
+    <row r="56" spans="4:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D56" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="21">
@@ -4628,15 +4997,15 @@
     </row>
     <row r="31" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="2:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="77" t="s">
+      <c r="B32" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="C32" s="78"/>
+      <c r="C32" s="93"/>
       <c r="D32" s="5"/>
-      <c r="E32" s="77" t="s">
+      <c r="E32" s="92" t="s">
         <v>20</v>
       </c>
-      <c r="F32" s="78"/>
+      <c r="F32" s="93"/>
       <c r="H32" s="59" t="s">
         <v>18</v>
       </c>
@@ -4822,15 +5191,15 @@
     </row>
     <row r="43" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="2:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="77" t="s">
+      <c r="B44" s="92" t="s">
         <v>72</v>
       </c>
-      <c r="C44" s="78"/>
+      <c r="C44" s="93"/>
       <c r="D44" s="5"/>
-      <c r="E44" s="77" t="s">
+      <c r="E44" s="92" t="s">
         <v>75</v>
       </c>
-      <c r="F44" s="78"/>
+      <c r="F44" s="93"/>
       <c r="H44" s="59" t="s">
         <v>72</v>
       </c>
@@ -4997,7 +5366,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104CFFA4-B0A1-1A4A-AFD7-C18B47CC4B2A}">
   <dimension ref="B1:J64"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A103" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="B30" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="L120" sqref="L120"/>
     </sheetView>
   </sheetViews>
@@ -5014,7 +5383,7 @@
   <sheetData>
     <row r="1" spans="2:6" ht="5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B2" s="89" t="s">
+      <c r="B2" s="106" t="s">
         <v>27</v>
       </c>
       <c r="D2" s="15" t="s">
@@ -5023,7 +5392,7 @@
       <c r="E2" s="24"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="90"/>
+      <c r="B3" s="107"/>
       <c r="D3" s="17" t="s">
         <v>106</v>
       </c>
@@ -5051,7 +5420,7 @@
       <c r="E6" s="14"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C9" s="91" t="s">
+      <c r="C9" s="104" t="s">
         <v>28</v>
       </c>
       <c r="E9" s="15" t="s">
@@ -5060,7 +5429,7 @@
       <c r="F9" s="24"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C10" s="92"/>
+      <c r="C10" s="105"/>
       <c r="E10" s="17" t="s">
         <v>38</v>
       </c>
@@ -5079,7 +5448,7 @@
       <c r="F12" s="24"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C15" s="91" t="s">
+      <c r="C15" s="104" t="s">
         <v>29</v>
       </c>
       <c r="E15" s="15" t="s">
@@ -5088,14 +5457,14 @@
       <c r="F15" s="24"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C16" s="92"/>
+      <c r="C16" s="105"/>
       <c r="E16" s="16" t="s">
         <v>42</v>
       </c>
       <c r="F16" s="24"/>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C19" s="91" t="s">
+      <c r="C19" s="104" t="s">
         <v>30</v>
       </c>
       <c r="E19" s="15" t="s">
@@ -5104,7 +5473,7 @@
       <c r="F19" s="24"/>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C20" s="92"/>
+      <c r="C20" s="105"/>
       <c r="E20" s="17" t="s">
         <v>43</v>
       </c>
@@ -5127,7 +5496,7 @@
       <c r="F23" s="24"/>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C25" s="91" t="s">
+      <c r="C25" s="104" t="s">
         <v>107</v>
       </c>
       <c r="E25" s="15" t="s">
@@ -5135,7 +5504,7 @@
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C26" s="92"/>
+      <c r="C26" s="105"/>
       <c r="E26" s="17" t="s">
         <v>108</v>
       </c>
@@ -5154,7 +5523,7 @@
       <c r="E30" s="29"/>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C31" s="91" t="s">
+      <c r="C31" s="104" t="s">
         <v>32</v>
       </c>
       <c r="E31" s="15" t="s">
@@ -5164,7 +5533,7 @@
       <c r="G31" s="14"/>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C32" s="92"/>
+      <c r="C32" s="105"/>
       <c r="E32" s="17" t="s">
         <v>76</v>
       </c>
@@ -5179,7 +5548,7 @@
       <c r="G33" s="14"/>
     </row>
     <row r="36" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C36" s="91" t="s">
+      <c r="C36" s="104" t="s">
         <v>33</v>
       </c>
       <c r="E36" s="12" t="s">
@@ -5190,7 +5559,7 @@
       </c>
     </row>
     <row r="37" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C37" s="92"/>
+      <c r="C37" s="105"/>
       <c r="G37" s="17" t="s">
         <v>102</v>
       </c>
@@ -5222,7 +5591,7 @@
       <c r="G42" s="29"/>
     </row>
     <row r="45" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C45" s="91" t="s">
+      <c r="C45" s="104" t="s">
         <v>31</v>
       </c>
       <c r="D45" s="18"/>
@@ -5232,7 +5601,7 @@
       <c r="G45" s="29"/>
     </row>
     <row r="46" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C46" s="92"/>
+      <c r="C46" s="105"/>
       <c r="D46" s="18"/>
       <c r="E46" s="16" t="s">
         <v>52</v>
@@ -5328,12 +5697,12 @@
       <c r="G61" s="29"/>
     </row>
     <row r="62" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C62" s="91" t="s">
-        <v>178</v>
+      <c r="C62" s="104" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="63" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C63" s="92"/>
+      <c r="C63" s="105"/>
     </row>
     <row r="64" spans="3:10" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -5613,12 +5982,12 @@
       <c r="E7" s="26"/>
       <c r="F7" s="27"/>
       <c r="G7" s="29"/>
-      <c r="H7" s="108" t="s">
+      <c r="H7" s="117" t="s">
         <v>145</v>
       </c>
-      <c r="I7" s="109"/>
-      <c r="J7" s="109"/>
-      <c r="K7" s="110"/>
+      <c r="I7" s="118"/>
+      <c r="J7" s="118"/>
+      <c r="K7" s="119"/>
       <c r="L7" s="30"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
@@ -5628,10 +5997,10 @@
       <c r="E8" s="29"/>
       <c r="F8" s="30"/>
       <c r="G8" s="29"/>
-      <c r="H8" s="111"/>
-      <c r="I8" s="112"/>
-      <c r="J8" s="112"/>
-      <c r="K8" s="113"/>
+      <c r="H8" s="120"/>
+      <c r="I8" s="121"/>
+      <c r="J8" s="121"/>
+      <c r="K8" s="122"/>
       <c r="L8" s="30"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
@@ -5641,10 +6010,10 @@
       <c r="E9" s="32"/>
       <c r="F9" s="33"/>
       <c r="G9" s="29"/>
-      <c r="H9" s="111"/>
-      <c r="I9" s="112"/>
-      <c r="J9" s="112"/>
-      <c r="K9" s="113"/>
+      <c r="H9" s="120"/>
+      <c r="I9" s="121"/>
+      <c r="J9" s="121"/>
+      <c r="K9" s="122"/>
       <c r="L9" s="30"/>
     </row>
     <row r="10" spans="2:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -5654,10 +6023,10 @@
       <c r="E10" s="29"/>
       <c r="F10" s="29"/>
       <c r="G10" s="29"/>
-      <c r="H10" s="111"/>
-      <c r="I10" s="112"/>
-      <c r="J10" s="112"/>
-      <c r="K10" s="113"/>
+      <c r="H10" s="120"/>
+      <c r="I10" s="121"/>
+      <c r="J10" s="121"/>
+      <c r="K10" s="122"/>
       <c r="L10" s="30"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.2">
@@ -5669,10 +6038,10 @@
       <c r="E11" s="26"/>
       <c r="F11" s="27"/>
       <c r="G11" s="29"/>
-      <c r="H11" s="111"/>
-      <c r="I11" s="112"/>
-      <c r="J11" s="112"/>
-      <c r="K11" s="113"/>
+      <c r="H11" s="120"/>
+      <c r="I11" s="121"/>
+      <c r="J11" s="121"/>
+      <c r="K11" s="122"/>
       <c r="L11" s="30"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
@@ -5684,10 +6053,10 @@
       <c r="E12" s="29"/>
       <c r="F12" s="30"/>
       <c r="G12" s="29"/>
-      <c r="H12" s="111"/>
-      <c r="I12" s="112"/>
-      <c r="J12" s="112"/>
-      <c r="K12" s="113"/>
+      <c r="H12" s="120"/>
+      <c r="I12" s="121"/>
+      <c r="J12" s="121"/>
+      <c r="K12" s="122"/>
       <c r="L12" s="30"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.2">
@@ -5699,10 +6068,10 @@
       <c r="E13" s="29"/>
       <c r="F13" s="30"/>
       <c r="G13" s="29"/>
-      <c r="H13" s="111"/>
-      <c r="I13" s="112"/>
-      <c r="J13" s="112"/>
-      <c r="K13" s="113"/>
+      <c r="H13" s="120"/>
+      <c r="I13" s="121"/>
+      <c r="J13" s="121"/>
+      <c r="K13" s="122"/>
       <c r="L13" s="30"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.2">
@@ -5714,10 +6083,10 @@
       <c r="E14" s="32"/>
       <c r="F14" s="33"/>
       <c r="G14" s="29"/>
-      <c r="H14" s="111"/>
-      <c r="I14" s="112"/>
-      <c r="J14" s="112"/>
-      <c r="K14" s="113"/>
+      <c r="H14" s="120"/>
+      <c r="I14" s="121"/>
+      <c r="J14" s="121"/>
+      <c r="K14" s="122"/>
       <c r="L14" s="30"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
@@ -5727,10 +6096,10 @@
       <c r="E15" s="29"/>
       <c r="F15" s="29"/>
       <c r="G15" s="29"/>
-      <c r="H15" s="111"/>
-      <c r="I15" s="112"/>
-      <c r="J15" s="112"/>
-      <c r="K15" s="113"/>
+      <c r="H15" s="120"/>
+      <c r="I15" s="121"/>
+      <c r="J15" s="121"/>
+      <c r="K15" s="122"/>
       <c r="L15" s="30"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.2">
@@ -5742,10 +6111,10 @@
       <c r="E16" s="26"/>
       <c r="F16" s="27"/>
       <c r="G16" s="29"/>
-      <c r="H16" s="111"/>
-      <c r="I16" s="112"/>
-      <c r="J16" s="112"/>
-      <c r="K16" s="113"/>
+      <c r="H16" s="120"/>
+      <c r="I16" s="121"/>
+      <c r="J16" s="121"/>
+      <c r="K16" s="122"/>
       <c r="L16" s="30"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.2">
@@ -5757,10 +6126,10 @@
       <c r="E17" s="29"/>
       <c r="F17" s="30"/>
       <c r="G17" s="29"/>
-      <c r="H17" s="111"/>
-      <c r="I17" s="112"/>
-      <c r="J17" s="112"/>
-      <c r="K17" s="113"/>
+      <c r="H17" s="120"/>
+      <c r="I17" s="121"/>
+      <c r="J17" s="121"/>
+      <c r="K17" s="122"/>
       <c r="L17" s="30"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.2">
@@ -5772,10 +6141,10 @@
       <c r="E18" s="29"/>
       <c r="F18" s="30"/>
       <c r="G18" s="29"/>
-      <c r="H18" s="111"/>
-      <c r="I18" s="112"/>
-      <c r="J18" s="112"/>
-      <c r="K18" s="113"/>
+      <c r="H18" s="120"/>
+      <c r="I18" s="121"/>
+      <c r="J18" s="121"/>
+      <c r="K18" s="122"/>
       <c r="L18" s="30"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.2">
@@ -5785,10 +6154,10 @@
       <c r="E19" s="29"/>
       <c r="F19" s="30"/>
       <c r="G19" s="29"/>
-      <c r="H19" s="111"/>
-      <c r="I19" s="112"/>
-      <c r="J19" s="112"/>
-      <c r="K19" s="113"/>
+      <c r="H19" s="120"/>
+      <c r="I19" s="121"/>
+      <c r="J19" s="121"/>
+      <c r="K19" s="122"/>
       <c r="L19" s="30"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
@@ -5798,10 +6167,10 @@
       <c r="E20" s="32"/>
       <c r="F20" s="33"/>
       <c r="G20" s="29"/>
-      <c r="H20" s="114"/>
-      <c r="I20" s="115"/>
-      <c r="J20" s="115"/>
-      <c r="K20" s="116"/>
+      <c r="H20" s="123"/>
+      <c r="I20" s="124"/>
+      <c r="J20" s="124"/>
+      <c r="K20" s="125"/>
       <c r="L20" s="30"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.2">
@@ -5968,49 +6337,49 @@
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B36" s="28"/>
-      <c r="C36" s="93" t="s">
+      <c r="C36" s="129" t="s">
         <v>148</v>
       </c>
-      <c r="D36" s="94"/>
-      <c r="E36" s="95"/>
-      <c r="F36" s="91" t="s">
+      <c r="D36" s="130"/>
+      <c r="E36" s="131"/>
+      <c r="F36" s="104" t="s">
         <v>149</v>
       </c>
       <c r="G36" s="29"/>
-      <c r="H36" s="99" t="s">
+      <c r="H36" s="108" t="s">
         <v>155</v>
       </c>
-      <c r="I36" s="100"/>
-      <c r="J36" s="100"/>
-      <c r="K36" s="101"/>
+      <c r="I36" s="109"/>
+      <c r="J36" s="109"/>
+      <c r="K36" s="110"/>
       <c r="L36" s="30"/>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B37" s="28"/>
-      <c r="C37" s="96"/>
-      <c r="D37" s="97"/>
-      <c r="E37" s="98"/>
-      <c r="F37" s="92"/>
+      <c r="C37" s="132"/>
+      <c r="D37" s="133"/>
+      <c r="E37" s="134"/>
+      <c r="F37" s="105"/>
       <c r="G37" s="29"/>
-      <c r="H37" s="102"/>
-      <c r="I37" s="103"/>
-      <c r="J37" s="103"/>
-      <c r="K37" s="104"/>
+      <c r="H37" s="111"/>
+      <c r="I37" s="112"/>
+      <c r="J37" s="112"/>
+      <c r="K37" s="113"/>
       <c r="L37" s="30"/>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B38" s="28"/>
-      <c r="C38" s="117" t="s">
+      <c r="C38" s="126" t="s">
         <v>151</v>
       </c>
-      <c r="D38" s="118"/>
-      <c r="E38" s="118"/>
-      <c r="F38" s="119"/>
+      <c r="D38" s="127"/>
+      <c r="E38" s="127"/>
+      <c r="F38" s="128"/>
       <c r="G38" s="29"/>
-      <c r="H38" s="105"/>
-      <c r="I38" s="106"/>
-      <c r="J38" s="106"/>
-      <c r="K38" s="107"/>
+      <c r="H38" s="114"/>
+      <c r="I38" s="115"/>
+      <c r="J38" s="115"/>
+      <c r="K38" s="116"/>
       <c r="L38" s="30"/>
     </row>
     <row r="39" spans="2:12" ht="19" x14ac:dyDescent="0.2">
@@ -6041,82 +6410,82 @@
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B41" s="28"/>
-      <c r="C41" s="120" t="s">
+      <c r="C41" s="135" t="s">
         <v>150</v>
       </c>
-      <c r="D41" s="121"/>
-      <c r="E41" s="121"/>
-      <c r="F41" s="121"/>
-      <c r="G41" s="121"/>
-      <c r="H41" s="121"/>
-      <c r="I41" s="121"/>
-      <c r="J41" s="121"/>
-      <c r="K41" s="122"/>
+      <c r="D41" s="136"/>
+      <c r="E41" s="136"/>
+      <c r="F41" s="136"/>
+      <c r="G41" s="136"/>
+      <c r="H41" s="136"/>
+      <c r="I41" s="136"/>
+      <c r="J41" s="136"/>
+      <c r="K41" s="137"/>
       <c r="L41" s="67"/>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B42" s="28"/>
-      <c r="C42" s="123"/>
-      <c r="D42" s="124"/>
-      <c r="E42" s="124"/>
-      <c r="F42" s="124"/>
-      <c r="G42" s="124"/>
-      <c r="H42" s="124"/>
-      <c r="I42" s="124"/>
-      <c r="J42" s="124"/>
-      <c r="K42" s="125"/>
+      <c r="C42" s="138"/>
+      <c r="D42" s="139"/>
+      <c r="E42" s="139"/>
+      <c r="F42" s="139"/>
+      <c r="G42" s="139"/>
+      <c r="H42" s="139"/>
+      <c r="I42" s="139"/>
+      <c r="J42" s="139"/>
+      <c r="K42" s="140"/>
       <c r="L42" s="67"/>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B43" s="28"/>
-      <c r="C43" s="123"/>
-      <c r="D43" s="124"/>
-      <c r="E43" s="124"/>
-      <c r="F43" s="124"/>
-      <c r="G43" s="124"/>
-      <c r="H43" s="124"/>
-      <c r="I43" s="124"/>
-      <c r="J43" s="124"/>
-      <c r="K43" s="125"/>
+      <c r="C43" s="138"/>
+      <c r="D43" s="139"/>
+      <c r="E43" s="139"/>
+      <c r="F43" s="139"/>
+      <c r="G43" s="139"/>
+      <c r="H43" s="139"/>
+      <c r="I43" s="139"/>
+      <c r="J43" s="139"/>
+      <c r="K43" s="140"/>
       <c r="L43" s="67"/>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B44" s="28"/>
-      <c r="C44" s="123"/>
-      <c r="D44" s="124"/>
-      <c r="E44" s="124"/>
-      <c r="F44" s="124"/>
-      <c r="G44" s="124"/>
-      <c r="H44" s="124"/>
-      <c r="I44" s="124"/>
-      <c r="J44" s="124"/>
-      <c r="K44" s="125"/>
+      <c r="C44" s="138"/>
+      <c r="D44" s="139"/>
+      <c r="E44" s="139"/>
+      <c r="F44" s="139"/>
+      <c r="G44" s="139"/>
+      <c r="H44" s="139"/>
+      <c r="I44" s="139"/>
+      <c r="J44" s="139"/>
+      <c r="K44" s="140"/>
       <c r="L44" s="67"/>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B45" s="28"/>
-      <c r="C45" s="123"/>
-      <c r="D45" s="124"/>
-      <c r="E45" s="124"/>
-      <c r="F45" s="124"/>
-      <c r="G45" s="124"/>
-      <c r="H45" s="124"/>
-      <c r="I45" s="124"/>
-      <c r="J45" s="124"/>
-      <c r="K45" s="125"/>
+      <c r="C45" s="138"/>
+      <c r="D45" s="139"/>
+      <c r="E45" s="139"/>
+      <c r="F45" s="139"/>
+      <c r="G45" s="139"/>
+      <c r="H45" s="139"/>
+      <c r="I45" s="139"/>
+      <c r="J45" s="139"/>
+      <c r="K45" s="140"/>
       <c r="L45" s="67"/>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B46" s="28"/>
-      <c r="C46" s="126"/>
-      <c r="D46" s="127"/>
-      <c r="E46" s="127"/>
-      <c r="F46" s="127"/>
-      <c r="G46" s="127"/>
-      <c r="H46" s="127"/>
-      <c r="I46" s="127"/>
-      <c r="J46" s="127"/>
-      <c r="K46" s="128"/>
+      <c r="C46" s="141"/>
+      <c r="D46" s="142"/>
+      <c r="E46" s="142"/>
+      <c r="F46" s="142"/>
+      <c r="G46" s="142"/>
+      <c r="H46" s="142"/>
+      <c r="I46" s="142"/>
+      <c r="J46" s="142"/>
+      <c r="K46" s="143"/>
       <c r="L46" s="67"/>
     </row>
     <row r="47" spans="2:12" ht="21" x14ac:dyDescent="0.2">
@@ -6147,32 +6516,32 @@
     </row>
     <row r="49" spans="2:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="28"/>
-      <c r="C49" s="93" t="s">
+      <c r="C49" s="129" t="s">
         <v>152</v>
       </c>
-      <c r="D49" s="94"/>
-      <c r="E49" s="94"/>
-      <c r="F49" s="95"/>
+      <c r="D49" s="130"/>
+      <c r="E49" s="130"/>
+      <c r="F49" s="131"/>
       <c r="G49" s="29"/>
-      <c r="H49" s="108" t="s">
+      <c r="H49" s="117" t="s">
         <v>154</v>
       </c>
-      <c r="I49" s="109"/>
-      <c r="J49" s="109"/>
-      <c r="K49" s="110"/>
+      <c r="I49" s="118"/>
+      <c r="J49" s="118"/>
+      <c r="K49" s="119"/>
       <c r="L49" s="67"/>
     </row>
     <row r="50" spans="2:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="28"/>
-      <c r="C50" s="96"/>
-      <c r="D50" s="97"/>
-      <c r="E50" s="97"/>
-      <c r="F50" s="98"/>
+      <c r="C50" s="132"/>
+      <c r="D50" s="133"/>
+      <c r="E50" s="133"/>
+      <c r="F50" s="134"/>
       <c r="G50" s="29"/>
-      <c r="H50" s="111"/>
-      <c r="I50" s="112"/>
-      <c r="J50" s="112"/>
-      <c r="K50" s="113"/>
+      <c r="H50" s="120"/>
+      <c r="I50" s="121"/>
+      <c r="J50" s="121"/>
+      <c r="K50" s="122"/>
       <c r="L50" s="67"/>
     </row>
     <row r="51" spans="2:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
@@ -6182,10 +6551,10 @@
       <c r="E51" s="29"/>
       <c r="F51" s="29"/>
       <c r="G51" s="29"/>
-      <c r="H51" s="111"/>
-      <c r="I51" s="112"/>
-      <c r="J51" s="112"/>
-      <c r="K51" s="113"/>
+      <c r="H51" s="120"/>
+      <c r="I51" s="121"/>
+      <c r="J51" s="121"/>
+      <c r="K51" s="122"/>
       <c r="L51" s="67"/>
     </row>
     <row r="52" spans="2:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
@@ -6195,129 +6564,129 @@
       <c r="E52" s="29"/>
       <c r="F52" s="29"/>
       <c r="G52" s="29"/>
-      <c r="H52" s="111"/>
-      <c r="I52" s="112"/>
-      <c r="J52" s="112"/>
-      <c r="K52" s="113"/>
+      <c r="H52" s="120"/>
+      <c r="I52" s="121"/>
+      <c r="J52" s="121"/>
+      <c r="K52" s="122"/>
       <c r="L52" s="67"/>
     </row>
     <row r="53" spans="2:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B53" s="28"/>
-      <c r="C53" s="99" t="s">
+      <c r="C53" s="108" t="s">
         <v>153</v>
       </c>
-      <c r="D53" s="100"/>
-      <c r="E53" s="100"/>
-      <c r="F53" s="101"/>
+      <c r="D53" s="109"/>
+      <c r="E53" s="109"/>
+      <c r="F53" s="110"/>
       <c r="G53" s="29"/>
-      <c r="H53" s="111"/>
-      <c r="I53" s="112"/>
-      <c r="J53" s="112"/>
-      <c r="K53" s="113"/>
+      <c r="H53" s="120"/>
+      <c r="I53" s="121"/>
+      <c r="J53" s="121"/>
+      <c r="K53" s="122"/>
       <c r="L53" s="67"/>
     </row>
     <row r="54" spans="2:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B54" s="28"/>
-      <c r="C54" s="102"/>
-      <c r="D54" s="103"/>
-      <c r="E54" s="103"/>
-      <c r="F54" s="104"/>
+      <c r="C54" s="111"/>
+      <c r="D54" s="112"/>
+      <c r="E54" s="112"/>
+      <c r="F54" s="113"/>
       <c r="G54" s="29"/>
-      <c r="H54" s="111"/>
-      <c r="I54" s="112"/>
-      <c r="J54" s="112"/>
-      <c r="K54" s="113"/>
+      <c r="H54" s="120"/>
+      <c r="I54" s="121"/>
+      <c r="J54" s="121"/>
+      <c r="K54" s="122"/>
       <c r="L54" s="67"/>
     </row>
     <row r="55" spans="2:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="28"/>
-      <c r="C55" s="102"/>
-      <c r="D55" s="103"/>
-      <c r="E55" s="103"/>
-      <c r="F55" s="104"/>
+      <c r="C55" s="111"/>
+      <c r="D55" s="112"/>
+      <c r="E55" s="112"/>
+      <c r="F55" s="113"/>
       <c r="G55" s="29"/>
-      <c r="H55" s="111"/>
-      <c r="I55" s="112"/>
-      <c r="J55" s="112"/>
-      <c r="K55" s="113"/>
+      <c r="H55" s="120"/>
+      <c r="I55" s="121"/>
+      <c r="J55" s="121"/>
+      <c r="K55" s="122"/>
       <c r="L55" s="67"/>
     </row>
     <row r="56" spans="2:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B56" s="28"/>
-      <c r="C56" s="102"/>
-      <c r="D56" s="103"/>
-      <c r="E56" s="103"/>
-      <c r="F56" s="104"/>
+      <c r="C56" s="111"/>
+      <c r="D56" s="112"/>
+      <c r="E56" s="112"/>
+      <c r="F56" s="113"/>
       <c r="G56" s="29"/>
-      <c r="H56" s="111"/>
-      <c r="I56" s="112"/>
-      <c r="J56" s="112"/>
-      <c r="K56" s="113"/>
+      <c r="H56" s="120"/>
+      <c r="I56" s="121"/>
+      <c r="J56" s="121"/>
+      <c r="K56" s="122"/>
       <c r="L56" s="67"/>
     </row>
     <row r="57" spans="2:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="28"/>
-      <c r="C57" s="102"/>
-      <c r="D57" s="103"/>
-      <c r="E57" s="103"/>
-      <c r="F57" s="104"/>
+      <c r="C57" s="111"/>
+      <c r="D57" s="112"/>
+      <c r="E57" s="112"/>
+      <c r="F57" s="113"/>
       <c r="G57" s="29"/>
-      <c r="H57" s="111"/>
-      <c r="I57" s="112"/>
-      <c r="J57" s="112"/>
-      <c r="K57" s="113"/>
+      <c r="H57" s="120"/>
+      <c r="I57" s="121"/>
+      <c r="J57" s="121"/>
+      <c r="K57" s="122"/>
       <c r="L57" s="67"/>
     </row>
     <row r="58" spans="2:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="28"/>
-      <c r="C58" s="102"/>
-      <c r="D58" s="103"/>
-      <c r="E58" s="103"/>
-      <c r="F58" s="104"/>
+      <c r="C58" s="111"/>
+      <c r="D58" s="112"/>
+      <c r="E58" s="112"/>
+      <c r="F58" s="113"/>
       <c r="G58" s="29"/>
-      <c r="H58" s="111"/>
-      <c r="I58" s="112"/>
-      <c r="J58" s="112"/>
-      <c r="K58" s="113"/>
+      <c r="H58" s="120"/>
+      <c r="I58" s="121"/>
+      <c r="J58" s="121"/>
+      <c r="K58" s="122"/>
       <c r="L58" s="30"/>
     </row>
     <row r="59" spans="2:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="28"/>
-      <c r="C59" s="102"/>
-      <c r="D59" s="103"/>
-      <c r="E59" s="103"/>
-      <c r="F59" s="104"/>
+      <c r="C59" s="111"/>
+      <c r="D59" s="112"/>
+      <c r="E59" s="112"/>
+      <c r="F59" s="113"/>
       <c r="G59" s="29"/>
-      <c r="H59" s="111"/>
-      <c r="I59" s="112"/>
-      <c r="J59" s="112"/>
-      <c r="K59" s="113"/>
+      <c r="H59" s="120"/>
+      <c r="I59" s="121"/>
+      <c r="J59" s="121"/>
+      <c r="K59" s="122"/>
       <c r="L59" s="30"/>
     </row>
     <row r="60" spans="2:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B60" s="28"/>
-      <c r="C60" s="102"/>
-      <c r="D60" s="103"/>
-      <c r="E60" s="103"/>
-      <c r="F60" s="104"/>
+      <c r="C60" s="111"/>
+      <c r="D60" s="112"/>
+      <c r="E60" s="112"/>
+      <c r="F60" s="113"/>
       <c r="G60" s="29"/>
-      <c r="H60" s="111"/>
-      <c r="I60" s="112"/>
-      <c r="J60" s="112"/>
-      <c r="K60" s="113"/>
+      <c r="H60" s="120"/>
+      <c r="I60" s="121"/>
+      <c r="J60" s="121"/>
+      <c r="K60" s="122"/>
       <c r="L60" s="30"/>
     </row>
     <row r="61" spans="2:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B61" s="28"/>
-      <c r="C61" s="105"/>
-      <c r="D61" s="106"/>
-      <c r="E61" s="106"/>
-      <c r="F61" s="107"/>
+      <c r="C61" s="114"/>
+      <c r="D61" s="115"/>
+      <c r="E61" s="115"/>
+      <c r="F61" s="116"/>
       <c r="G61" s="29"/>
-      <c r="H61" s="114"/>
-      <c r="I61" s="115"/>
-      <c r="J61" s="115"/>
-      <c r="K61" s="116"/>
+      <c r="H61" s="123"/>
+      <c r="I61" s="124"/>
+      <c r="J61" s="124"/>
+      <c r="K61" s="125"/>
       <c r="L61" s="30"/>
     </row>
     <row r="62" spans="2:12" x14ac:dyDescent="0.2">
@@ -6361,15 +6730,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="C53:F61"/>
+    <mergeCell ref="H49:K61"/>
+    <mergeCell ref="C38:F38"/>
+    <mergeCell ref="H36:K38"/>
     <mergeCell ref="H7:K20"/>
     <mergeCell ref="C36:E37"/>
     <mergeCell ref="F36:F37"/>
     <mergeCell ref="C41:K46"/>
     <mergeCell ref="C49:F50"/>
-    <mergeCell ref="C53:F61"/>
-    <mergeCell ref="H49:K61"/>
-    <mergeCell ref="C38:F38"/>
-    <mergeCell ref="H36:K38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6379,8 +6748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8E17ED-892D-D04F-869B-AE05270EAAF6}">
   <dimension ref="F29:J43"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6443,18 +6812,24 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CBFD39B-43B3-0D45-98DE-0DFDCC0D1885}">
-  <dimension ref="A1"/>
+  <dimension ref="S16"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5:R26"/>
+    <sheetView topLeftCell="G8" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5:U24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="14" max="14" width="17.83203125" customWidth="1"/>
-    <col min="17" max="17" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5" customWidth="1"/>
+    <col min="18" max="18" width="30.33203125" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="16" spans="19:19" x14ac:dyDescent="0.2">
+      <c r="S16" s="76"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -6462,10 +6837,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{708EB1BC-2998-4147-87D5-799A3B5DE066}">
-  <dimension ref="B34:D41"/>
+  <dimension ref="B34:F42"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A17" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView showGridLines="0" topLeftCell="A23" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6476,30 +6851,30 @@
     <col min="4" max="4" width="42.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="34" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="2:4" s="70" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="76" t="s">
+    <row r="34" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="2:6" s="70" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="75" t="s">
         <v>170</v>
       </c>
-      <c r="C35" s="76" t="s">
+      <c r="C35" s="75" t="s">
         <v>164</v>
       </c>
-      <c r="D35" s="76" t="s">
+      <c r="D35" s="75" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="36" spans="2:4" ht="85" x14ac:dyDescent="0.2">
-      <c r="B36" s="75" t="s">
+    <row r="36" spans="2:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="B36" s="74" t="s">
         <v>166</v>
       </c>
-      <c r="C36" s="75" t="s">
+      <c r="C36" s="74" t="s">
+        <v>174</v>
+      </c>
+      <c r="D36" s="74" t="s">
         <v>175</v>
       </c>
-      <c r="D36" s="75" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="2:6" ht="34" x14ac:dyDescent="0.2">
       <c r="B37" s="73" t="s">
         <v>167</v>
       </c>
@@ -6510,35 +6885,56 @@
         <v>171</v>
       </c>
     </row>
-    <row r="38" spans="2:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:6" ht="34" x14ac:dyDescent="0.2">
       <c r="B38" s="72" t="s">
-        <v>177</v>
-      </c>
-      <c r="C38" s="72"/>
-      <c r="D38" s="72"/>
-    </row>
-    <row r="39" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+        <v>176</v>
+      </c>
+      <c r="C38" s="72" t="s">
+        <v>178</v>
+      </c>
+      <c r="D38" s="72" t="s">
+        <v>179</v>
+      </c>
+      <c r="F38" s="76"/>
+    </row>
+    <row r="39" spans="2:6" ht="68" x14ac:dyDescent="0.2">
       <c r="B39" s="73" t="s">
+        <v>183</v>
+      </c>
+      <c r="C39" s="73" t="s">
+        <v>184</v>
+      </c>
+      <c r="D39" s="73" t="s">
+        <v>185</v>
+      </c>
+      <c r="F39" s="76"/>
+    </row>
+    <row r="40" spans="2:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="B40" s="72" t="s">
         <v>168</v>
       </c>
-      <c r="C39" s="73"/>
-      <c r="D39" s="73"/>
-    </row>
-    <row r="40" spans="2:4" ht="86" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="74" t="s">
+      <c r="C40" s="72" t="s">
+        <v>182</v>
+      </c>
+      <c r="D40" s="72" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" ht="69" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="77" t="s">
         <v>169</v>
       </c>
-      <c r="C40" s="74" t="s">
+      <c r="C41" s="77" t="s">
         <v>172</v>
       </c>
-      <c r="D40" s="74" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B41" s="71"/>
-      <c r="C41" s="71"/>
-      <c r="D41" s="71"/>
+      <c r="D41" s="77" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B42" s="71"/>
+      <c r="C42" s="71"/>
+      <c r="D42" s="71"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>